<commit_message>
Add customer and vendor information fields
</commit_message>
<xml_diff>
--- a/winApp/bin/Debug/Output.xlsx
+++ b/winApp/bin/Debug/Output.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UserName\Desktop\winApp01\winApp\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\WinApp\winApp\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA22C1B1-2F34-4379-8379-92B405B943EE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{994721CD-E0A3-4F9D-BFB0-8237AE060D5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5790" yWindow="2025" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21720" yWindow="3510" windowWidth="23685" windowHeight="11340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="стр.1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">стр.1!$A$1:$FE$44</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">стр.1!$A$1:$FE$36</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="75">
   <si>
     <t>Единица
 измерения</t>
@@ -249,37 +249,13 @@
     <t>Регистра-ционный номер таможенной декларации</t>
   </si>
   <si>
-    <t>Плитка улица</t>
-  </si>
-  <si>
-    <t>шт</t>
-  </si>
-  <si>
-    <t>Клей для плитки Сeresit СМ 9, 25 кг</t>
-  </si>
-  <si>
-    <t>Красящая добавка в раствор Hormusend</t>
-  </si>
-  <si>
-    <t>Клей для плитки Unis XXI, 25 кг</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Шовный заполнитель для брусчатки живая краска диамант на эпоксидной основе песочный </t>
-  </si>
-  <si>
-    <t>Водостоки для тротуарной плитки 500x160x60 мм</t>
-  </si>
-  <si>
-    <t>Плитка тротуарная 12-кирпичей</t>
-  </si>
-  <si>
-    <t>Тротуарная брусчатка ЛСР Мюнхен RF</t>
-  </si>
-  <si>
-    <t>Тротуарная брусчатка ЛСР Глазго RF</t>
-  </si>
-  <si>
-    <t>Клей цементный White Hills</t>
+    <t>Песка</t>
+  </si>
+  <si>
+    <t>м3</t>
+  </si>
+  <si>
+    <t>Щебня</t>
   </si>
 </sst>
 </file>
@@ -885,7 +861,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:FE44"/>
+  <dimension ref="A1:FE36"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A25" sqref="A25:T25"/>
@@ -4027,7 +4003,7 @@
       <c r="AR25" s="51"/>
       <c r="AS25" s="52"/>
       <c r="AT25" s="38">
-        <v>72</v>
+        <v>5</v>
       </c>
       <c r="AU25" s="39"/>
       <c r="AV25" s="39"/>
@@ -4037,7 +4013,7 @@
       <c r="AZ25" s="39"/>
       <c r="BA25" s="40"/>
       <c r="BB25" s="38">
-        <v>501.79</v>
+        <v>845.12</v>
       </c>
       <c r="BC25" s="39"/>
       <c r="BD25" s="39"/>
@@ -4097,7 +4073,7 @@
       <c r="DF25" s="39"/>
       <c r="DG25" s="40"/>
       <c r="DH25" s="38">
-        <v>36128.880000000005</v>
+        <v>4225.6000000000004</v>
       </c>
       <c r="DI25" s="39"/>
       <c r="DJ25" s="39"/>
@@ -4149,7 +4125,7 @@
       <c r="FD25" s="49"/>
       <c r="FE25" s="56"/>
     </row>
-    <row r="26" spans="1:161" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:161" s="2" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="42" t="s">
         <v>74</v>
       </c>
@@ -4210,7 +4186,7 @@
       <c r="AZ26" s="39"/>
       <c r="BA26" s="40"/>
       <c r="BB26" s="38">
-        <v>2515.2399999999998</v>
+        <v>664.7</v>
       </c>
       <c r="BC26" s="39"/>
       <c r="BD26" s="39"/>
@@ -4270,7 +4246,7 @@
       <c r="DF26" s="39"/>
       <c r="DG26" s="40"/>
       <c r="DH26" s="38">
-        <v>5030.4799999999996</v>
+        <v>1329.4</v>
       </c>
       <c r="DI26" s="39"/>
       <c r="DJ26" s="39"/>
@@ -4322,10 +4298,8 @@
       <c r="FD26" s="49"/>
       <c r="FE26" s="56"/>
     </row>
-    <row r="27" spans="1:161" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="42" t="s">
-        <v>75</v>
-      </c>
+    <row r="27" spans="1:161" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A27" s="42"/>
       <c r="B27" s="43"/>
       <c r="C27" s="43"/>
       <c r="D27" s="43"/>
@@ -4358,10 +4332,8 @@
       <c r="AE27" s="49"/>
       <c r="AF27" s="49"/>
       <c r="AG27" s="49"/>
-      <c r="AH27" s="56"/>
-      <c r="AI27" s="50" t="s">
-        <v>73</v>
-      </c>
+      <c r="AH27" s="49"/>
+      <c r="AI27" s="50"/>
       <c r="AJ27" s="51"/>
       <c r="AK27" s="51"/>
       <c r="AL27" s="51"/>
@@ -4372,9 +4344,7 @@
       <c r="AQ27" s="51"/>
       <c r="AR27" s="51"/>
       <c r="AS27" s="52"/>
-      <c r="AT27" s="38">
-        <v>1</v>
-      </c>
+      <c r="AT27" s="38"/>
       <c r="AU27" s="39"/>
       <c r="AV27" s="39"/>
       <c r="AW27" s="39"/>
@@ -4382,9 +4352,7 @@
       <c r="AY27" s="39"/>
       <c r="AZ27" s="39"/>
       <c r="BA27" s="40"/>
-      <c r="BB27" s="38">
-        <v>1592.19</v>
-      </c>
+      <c r="BB27" s="38"/>
       <c r="BC27" s="39"/>
       <c r="BD27" s="39"/>
       <c r="BE27" s="39"/>
@@ -4442,9 +4410,7 @@
       <c r="DE27" s="39"/>
       <c r="DF27" s="39"/>
       <c r="DG27" s="40"/>
-      <c r="DH27" s="38">
-        <v>1592.19</v>
-      </c>
+      <c r="DH27" s="38"/>
       <c r="DI27" s="39"/>
       <c r="DJ27" s="39"/>
       <c r="DK27" s="39"/>
@@ -4468,7 +4434,7 @@
       <c r="EC27" s="49"/>
       <c r="ED27" s="49"/>
       <c r="EE27" s="49"/>
-      <c r="EF27" s="56"/>
+      <c r="EF27" s="49"/>
       <c r="EG27" s="53"/>
       <c r="EH27" s="54"/>
       <c r="EI27" s="54"/>
@@ -4482,92 +4448,86 @@
       <c r="EQ27" s="54"/>
       <c r="ER27" s="54"/>
       <c r="ES27" s="55"/>
-      <c r="ET27" s="48"/>
-      <c r="EU27" s="49"/>
-      <c r="EV27" s="49"/>
-      <c r="EW27" s="49"/>
-      <c r="EX27" s="49"/>
-      <c r="EY27" s="49"/>
-      <c r="EZ27" s="49"/>
-      <c r="FA27" s="49"/>
-      <c r="FB27" s="49"/>
-      <c r="FC27" s="49"/>
-      <c r="FD27" s="49"/>
-      <c r="FE27" s="56"/>
+      <c r="ET27" s="41"/>
+      <c r="EU27" s="41"/>
+      <c r="EV27" s="41"/>
+      <c r="EW27" s="41"/>
+      <c r="EX27" s="41"/>
+      <c r="EY27" s="41"/>
+      <c r="EZ27" s="41"/>
+      <c r="FA27" s="41"/>
+      <c r="FB27" s="41"/>
+      <c r="FC27" s="41"/>
+      <c r="FD27" s="41"/>
+      <c r="FE27" s="41"/>
     </row>
-    <row r="28" spans="1:161" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="42" t="s">
-        <v>76</v>
-      </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
-      <c r="K28" s="43"/>
-      <c r="L28" s="43"/>
-      <c r="M28" s="43"/>
-      <c r="N28" s="43"/>
-      <c r="O28" s="43"/>
-      <c r="P28" s="43"/>
-      <c r="Q28" s="43"/>
-      <c r="R28" s="43"/>
-      <c r="S28" s="43"/>
-      <c r="T28" s="44"/>
-      <c r="U28" s="45"/>
-      <c r="V28" s="46"/>
-      <c r="W28" s="46"/>
-      <c r="X28" s="46"/>
-      <c r="Y28" s="46"/>
-      <c r="Z28" s="46"/>
-      <c r="AA28" s="46"/>
-      <c r="AB28" s="47"/>
-      <c r="AC28" s="48"/>
-      <c r="AD28" s="49"/>
-      <c r="AE28" s="49"/>
-      <c r="AF28" s="49"/>
-      <c r="AG28" s="49"/>
-      <c r="AH28" s="56"/>
-      <c r="AI28" s="50" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ28" s="51"/>
-      <c r="AK28" s="51"/>
-      <c r="AL28" s="51"/>
-      <c r="AM28" s="51"/>
-      <c r="AN28" s="51"/>
-      <c r="AO28" s="51"/>
-      <c r="AP28" s="51"/>
-      <c r="AQ28" s="51"/>
-      <c r="AR28" s="51"/>
-      <c r="AS28" s="52"/>
-      <c r="AT28" s="38">
-        <v>1</v>
-      </c>
-      <c r="AU28" s="39"/>
-      <c r="AV28" s="39"/>
-      <c r="AW28" s="39"/>
-      <c r="AX28" s="39"/>
-      <c r="AY28" s="39"/>
-      <c r="AZ28" s="39"/>
-      <c r="BA28" s="40"/>
-      <c r="BB28" s="38">
-        <v>1575.4</v>
-      </c>
-      <c r="BC28" s="39"/>
-      <c r="BD28" s="39"/>
-      <c r="BE28" s="39"/>
-      <c r="BF28" s="39"/>
-      <c r="BG28" s="39"/>
-      <c r="BH28" s="39"/>
-      <c r="BI28" s="39"/>
-      <c r="BJ28" s="39"/>
-      <c r="BK28" s="39"/>
-      <c r="BL28" s="40"/>
+    <row r="28" spans="1:161" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A28" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
+      <c r="K28" s="37"/>
+      <c r="L28" s="37"/>
+      <c r="M28" s="37"/>
+      <c r="N28" s="37"/>
+      <c r="O28" s="37"/>
+      <c r="P28" s="37"/>
+      <c r="Q28" s="37"/>
+      <c r="R28" s="37"/>
+      <c r="S28" s="37"/>
+      <c r="T28" s="37"/>
+      <c r="U28" s="37"/>
+      <c r="V28" s="37"/>
+      <c r="W28" s="37"/>
+      <c r="X28" s="37"/>
+      <c r="Y28" s="37"/>
+      <c r="Z28" s="37"/>
+      <c r="AA28" s="37"/>
+      <c r="AB28" s="37"/>
+      <c r="AC28" s="37"/>
+      <c r="AD28" s="37"/>
+      <c r="AE28" s="37"/>
+      <c r="AF28" s="37"/>
+      <c r="AG28" s="37"/>
+      <c r="AH28" s="37"/>
+      <c r="AI28" s="37"/>
+      <c r="AJ28" s="37"/>
+      <c r="AK28" s="37"/>
+      <c r="AL28" s="37"/>
+      <c r="AM28" s="37"/>
+      <c r="AN28" s="37"/>
+      <c r="AO28" s="37"/>
+      <c r="AP28" s="37"/>
+      <c r="AQ28" s="37"/>
+      <c r="AR28" s="37"/>
+      <c r="AS28" s="37"/>
+      <c r="AT28" s="37"/>
+      <c r="AU28" s="37"/>
+      <c r="AV28" s="37"/>
+      <c r="AW28" s="37"/>
+      <c r="AX28" s="37"/>
+      <c r="AY28" s="37"/>
+      <c r="AZ28" s="37"/>
+      <c r="BA28" s="37"/>
+      <c r="BB28" s="37"/>
+      <c r="BC28" s="37"/>
+      <c r="BD28" s="37"/>
+      <c r="BE28" s="37"/>
+      <c r="BF28" s="37"/>
+      <c r="BG28" s="37"/>
+      <c r="BH28" s="37"/>
+      <c r="BI28" s="37"/>
+      <c r="BJ28" s="37"/>
+      <c r="BK28" s="37"/>
+      <c r="BL28" s="37"/>
       <c r="BM28" s="38"/>
       <c r="BN28" s="39"/>
       <c r="BO28" s="39"/>
@@ -4583,7 +4543,9 @@
       <c r="BY28" s="39"/>
       <c r="BZ28" s="39"/>
       <c r="CA28" s="40"/>
-      <c r="CB28" s="38"/>
+      <c r="CB28" s="38" t="s">
+        <v>23</v>
+      </c>
       <c r="CC28" s="39"/>
       <c r="CD28" s="39"/>
       <c r="CE28" s="39"/>
@@ -4592,8 +4554,8 @@
       <c r="CH28" s="39"/>
       <c r="CI28" s="39"/>
       <c r="CJ28" s="39"/>
-      <c r="CK28" s="40"/>
-      <c r="CL28" s="38"/>
+      <c r="CK28" s="39"/>
+      <c r="CL28" s="39"/>
       <c r="CM28" s="39"/>
       <c r="CN28" s="39"/>
       <c r="CO28" s="39"/>
@@ -4603,1994 +4565,512 @@
       <c r="CS28" s="39"/>
       <c r="CT28" s="39"/>
       <c r="CU28" s="40"/>
-      <c r="CV28" s="38"/>
-      <c r="CW28" s="39"/>
-      <c r="CX28" s="39"/>
-      <c r="CY28" s="39"/>
-      <c r="CZ28" s="39"/>
-      <c r="DA28" s="39"/>
-      <c r="DB28" s="39"/>
-      <c r="DC28" s="39"/>
-      <c r="DD28" s="39"/>
-      <c r="DE28" s="39"/>
-      <c r="DF28" s="39"/>
-      <c r="DG28" s="40"/>
-      <c r="DH28" s="38">
-        <v>1575.4</v>
-      </c>
-      <c r="DI28" s="39"/>
-      <c r="DJ28" s="39"/>
-      <c r="DK28" s="39"/>
-      <c r="DL28" s="39"/>
-      <c r="DM28" s="39"/>
-      <c r="DN28" s="39"/>
-      <c r="DO28" s="39"/>
-      <c r="DP28" s="39"/>
-      <c r="DQ28" s="39"/>
-      <c r="DR28" s="39"/>
-      <c r="DS28" s="39"/>
-      <c r="DT28" s="39"/>
-      <c r="DU28" s="39"/>
-      <c r="DV28" s="40"/>
-      <c r="DW28" s="48"/>
-      <c r="DX28" s="49"/>
-      <c r="DY28" s="49"/>
-      <c r="DZ28" s="49"/>
-      <c r="EA28" s="49"/>
-      <c r="EB28" s="49"/>
-      <c r="EC28" s="49"/>
-      <c r="ED28" s="49"/>
-      <c r="EE28" s="49"/>
-      <c r="EF28" s="56"/>
-      <c r="EG28" s="53"/>
-      <c r="EH28" s="54"/>
-      <c r="EI28" s="54"/>
-      <c r="EJ28" s="54"/>
-      <c r="EK28" s="54"/>
-      <c r="EL28" s="54"/>
-      <c r="EM28" s="54"/>
-      <c r="EN28" s="54"/>
-      <c r="EO28" s="54"/>
-      <c r="EP28" s="54"/>
-      <c r="EQ28" s="54"/>
-      <c r="ER28" s="54"/>
-      <c r="ES28" s="55"/>
-      <c r="ET28" s="48"/>
-      <c r="EU28" s="49"/>
-      <c r="EV28" s="49"/>
-      <c r="EW28" s="49"/>
-      <c r="EX28" s="49"/>
-      <c r="EY28" s="49"/>
-      <c r="EZ28" s="49"/>
-      <c r="FA28" s="49"/>
-      <c r="FB28" s="49"/>
-      <c r="FC28" s="49"/>
-      <c r="FD28" s="49"/>
-      <c r="FE28" s="56"/>
+      <c r="CV28" s="35"/>
+      <c r="CW28" s="35"/>
+      <c r="CX28" s="35"/>
+      <c r="CY28" s="35"/>
+      <c r="CZ28" s="35"/>
+      <c r="DA28" s="35"/>
+      <c r="DB28" s="35"/>
+      <c r="DC28" s="35"/>
+      <c r="DD28" s="35"/>
+      <c r="DE28" s="35"/>
+      <c r="DF28" s="35"/>
+      <c r="DG28" s="35"/>
+      <c r="DH28" s="35">
+        <v>5555</v>
+      </c>
+      <c r="DI28" s="35"/>
+      <c r="DJ28" s="35"/>
+      <c r="DK28" s="35"/>
+      <c r="DL28" s="35"/>
+      <c r="DM28" s="35"/>
+      <c r="DN28" s="35"/>
+      <c r="DO28" s="35"/>
+      <c r="DP28" s="35"/>
+      <c r="DQ28" s="35"/>
+      <c r="DR28" s="35"/>
+      <c r="DS28" s="35"/>
+      <c r="DT28" s="35"/>
+      <c r="DU28" s="35"/>
+      <c r="DV28" s="35"/>
     </row>
-    <row r="29" spans="1:161" s="2" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
-      <c r="K29" s="43"/>
-      <c r="L29" s="43"/>
-      <c r="M29" s="43"/>
-      <c r="N29" s="43"/>
-      <c r="O29" s="43"/>
-      <c r="P29" s="43"/>
-      <c r="Q29" s="43"/>
-      <c r="R29" s="43"/>
-      <c r="S29" s="43"/>
-      <c r="T29" s="44"/>
-      <c r="U29" s="45"/>
-      <c r="V29" s="46"/>
-      <c r="W29" s="46"/>
-      <c r="X29" s="46"/>
-      <c r="Y29" s="46"/>
-      <c r="Z29" s="46"/>
-      <c r="AA29" s="46"/>
-      <c r="AB29" s="47"/>
-      <c r="AC29" s="48"/>
-      <c r="AD29" s="49"/>
-      <c r="AE29" s="49"/>
-      <c r="AF29" s="49"/>
-      <c r="AG29" s="49"/>
-      <c r="AH29" s="56"/>
-      <c r="AI29" s="50" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ29" s="51"/>
-      <c r="AK29" s="51"/>
-      <c r="AL29" s="51"/>
-      <c r="AM29" s="51"/>
-      <c r="AN29" s="51"/>
-      <c r="AO29" s="51"/>
-      <c r="AP29" s="51"/>
-      <c r="AQ29" s="51"/>
-      <c r="AR29" s="51"/>
-      <c r="AS29" s="52"/>
-      <c r="AT29" s="38">
-        <v>1</v>
-      </c>
-      <c r="AU29" s="39"/>
-      <c r="AV29" s="39"/>
-      <c r="AW29" s="39"/>
-      <c r="AX29" s="39"/>
-      <c r="AY29" s="39"/>
-      <c r="AZ29" s="39"/>
-      <c r="BA29" s="40"/>
-      <c r="BB29" s="38">
-        <v>3804.05</v>
-      </c>
-      <c r="BC29" s="39"/>
-      <c r="BD29" s="39"/>
-      <c r="BE29" s="39"/>
-      <c r="BF29" s="39"/>
-      <c r="BG29" s="39"/>
-      <c r="BH29" s="39"/>
-      <c r="BI29" s="39"/>
-      <c r="BJ29" s="39"/>
-      <c r="BK29" s="39"/>
-      <c r="BL29" s="40"/>
-      <c r="BM29" s="38"/>
-      <c r="BN29" s="39"/>
-      <c r="BO29" s="39"/>
-      <c r="BP29" s="39"/>
-      <c r="BQ29" s="39"/>
-      <c r="BR29" s="39"/>
-      <c r="BS29" s="39"/>
-      <c r="BT29" s="39"/>
-      <c r="BU29" s="39"/>
-      <c r="BV29" s="39"/>
-      <c r="BW29" s="39"/>
-      <c r="BX29" s="39"/>
-      <c r="BY29" s="39"/>
-      <c r="BZ29" s="39"/>
-      <c r="CA29" s="40"/>
-      <c r="CB29" s="38"/>
-      <c r="CC29" s="39"/>
-      <c r="CD29" s="39"/>
-      <c r="CE29" s="39"/>
-      <c r="CF29" s="39"/>
-      <c r="CG29" s="39"/>
-      <c r="CH29" s="39"/>
-      <c r="CI29" s="39"/>
-      <c r="CJ29" s="39"/>
-      <c r="CK29" s="40"/>
-      <c r="CL29" s="38"/>
-      <c r="CM29" s="39"/>
-      <c r="CN29" s="39"/>
-      <c r="CO29" s="39"/>
-      <c r="CP29" s="39"/>
-      <c r="CQ29" s="39"/>
-      <c r="CR29" s="39"/>
-      <c r="CS29" s="39"/>
-      <c r="CT29" s="39"/>
-      <c r="CU29" s="40"/>
-      <c r="CV29" s="38"/>
-      <c r="CW29" s="39"/>
-      <c r="CX29" s="39"/>
-      <c r="CY29" s="39"/>
-      <c r="CZ29" s="39"/>
-      <c r="DA29" s="39"/>
-      <c r="DB29" s="39"/>
-      <c r="DC29" s="39"/>
-      <c r="DD29" s="39"/>
-      <c r="DE29" s="39"/>
-      <c r="DF29" s="39"/>
-      <c r="DG29" s="40"/>
-      <c r="DH29" s="38">
-        <v>3804.05</v>
-      </c>
-      <c r="DI29" s="39"/>
-      <c r="DJ29" s="39"/>
-      <c r="DK29" s="39"/>
-      <c r="DL29" s="39"/>
-      <c r="DM29" s="39"/>
-      <c r="DN29" s="39"/>
-      <c r="DO29" s="39"/>
-      <c r="DP29" s="39"/>
-      <c r="DQ29" s="39"/>
-      <c r="DR29" s="39"/>
-      <c r="DS29" s="39"/>
-      <c r="DT29" s="39"/>
-      <c r="DU29" s="39"/>
-      <c r="DV29" s="40"/>
-      <c r="DW29" s="48"/>
-      <c r="DX29" s="49"/>
-      <c r="DY29" s="49"/>
-      <c r="DZ29" s="49"/>
-      <c r="EA29" s="49"/>
-      <c r="EB29" s="49"/>
-      <c r="EC29" s="49"/>
-      <c r="ED29" s="49"/>
-      <c r="EE29" s="49"/>
-      <c r="EF29" s="56"/>
-      <c r="EG29" s="53"/>
-      <c r="EH29" s="54"/>
-      <c r="EI29" s="54"/>
-      <c r="EJ29" s="54"/>
-      <c r="EK29" s="54"/>
-      <c r="EL29" s="54"/>
-      <c r="EM29" s="54"/>
-      <c r="EN29" s="54"/>
-      <c r="EO29" s="54"/>
-      <c r="EP29" s="54"/>
-      <c r="EQ29" s="54"/>
-      <c r="ER29" s="54"/>
-      <c r="ES29" s="55"/>
-      <c r="ET29" s="48"/>
-      <c r="EU29" s="49"/>
-      <c r="EV29" s="49"/>
-      <c r="EW29" s="49"/>
-      <c r="EX29" s="49"/>
-      <c r="EY29" s="49"/>
-      <c r="EZ29" s="49"/>
-      <c r="FA29" s="49"/>
-      <c r="FB29" s="49"/>
-      <c r="FC29" s="49"/>
-      <c r="FD29" s="49"/>
-      <c r="FE29" s="56"/>
+    <row r="29" spans="1:161" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:161" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="CD30" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="30" spans="1:161" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="42" t="s">
-        <v>78</v>
-      </c>
-      <c r="B30" s="43"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="43"/>
-      <c r="J30" s="43"/>
-      <c r="K30" s="43"/>
-      <c r="L30" s="43"/>
-      <c r="M30" s="43"/>
-      <c r="N30" s="43"/>
-      <c r="O30" s="43"/>
-      <c r="P30" s="43"/>
-      <c r="Q30" s="43"/>
-      <c r="R30" s="43"/>
-      <c r="S30" s="43"/>
-      <c r="T30" s="44"/>
-      <c r="U30" s="45"/>
-      <c r="V30" s="46"/>
-      <c r="W30" s="46"/>
-      <c r="X30" s="46"/>
-      <c r="Y30" s="46"/>
-      <c r="Z30" s="46"/>
-      <c r="AA30" s="46"/>
-      <c r="AB30" s="47"/>
-      <c r="AC30" s="48"/>
-      <c r="AD30" s="49"/>
-      <c r="AE30" s="49"/>
-      <c r="AF30" s="49"/>
-      <c r="AG30" s="49"/>
-      <c r="AH30" s="56"/>
-      <c r="AI30" s="50" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ30" s="51"/>
-      <c r="AK30" s="51"/>
-      <c r="AL30" s="51"/>
-      <c r="AM30" s="51"/>
-      <c r="AN30" s="51"/>
-      <c r="AO30" s="51"/>
-      <c r="AP30" s="51"/>
-      <c r="AQ30" s="51"/>
-      <c r="AR30" s="51"/>
-      <c r="AS30" s="52"/>
-      <c r="AT30" s="38">
-        <v>2</v>
-      </c>
-      <c r="AU30" s="39"/>
-      <c r="AV30" s="39"/>
-      <c r="AW30" s="39"/>
-      <c r="AX30" s="39"/>
-      <c r="AY30" s="39"/>
-      <c r="AZ30" s="39"/>
-      <c r="BA30" s="40"/>
-      <c r="BB30" s="38">
-        <v>390.51</v>
-      </c>
-      <c r="BC30" s="39"/>
-      <c r="BD30" s="39"/>
-      <c r="BE30" s="39"/>
-      <c r="BF30" s="39"/>
-      <c r="BG30" s="39"/>
-      <c r="BH30" s="39"/>
-      <c r="BI30" s="39"/>
-      <c r="BJ30" s="39"/>
-      <c r="BK30" s="39"/>
-      <c r="BL30" s="40"/>
-      <c r="BM30" s="38"/>
-      <c r="BN30" s="39"/>
-      <c r="BO30" s="39"/>
-      <c r="BP30" s="39"/>
-      <c r="BQ30" s="39"/>
-      <c r="BR30" s="39"/>
-      <c r="BS30" s="39"/>
-      <c r="BT30" s="39"/>
-      <c r="BU30" s="39"/>
-      <c r="BV30" s="39"/>
-      <c r="BW30" s="39"/>
-      <c r="BX30" s="39"/>
-      <c r="BY30" s="39"/>
-      <c r="BZ30" s="39"/>
-      <c r="CA30" s="40"/>
-      <c r="CB30" s="38"/>
-      <c r="CC30" s="39"/>
-      <c r="CD30" s="39"/>
-      <c r="CE30" s="39"/>
-      <c r="CF30" s="39"/>
-      <c r="CG30" s="39"/>
-      <c r="CH30" s="39"/>
-      <c r="CI30" s="39"/>
-      <c r="CJ30" s="39"/>
-      <c r="CK30" s="40"/>
-      <c r="CL30" s="38"/>
-      <c r="CM30" s="39"/>
-      <c r="CN30" s="39"/>
-      <c r="CO30" s="39"/>
-      <c r="CP30" s="39"/>
-      <c r="CQ30" s="39"/>
-      <c r="CR30" s="39"/>
-      <c r="CS30" s="39"/>
-      <c r="CT30" s="39"/>
-      <c r="CU30" s="40"/>
-      <c r="CV30" s="38"/>
-      <c r="CW30" s="39"/>
-      <c r="CX30" s="39"/>
-      <c r="CY30" s="39"/>
-      <c r="CZ30" s="39"/>
-      <c r="DA30" s="39"/>
-      <c r="DB30" s="39"/>
-      <c r="DC30" s="39"/>
-      <c r="DD30" s="39"/>
-      <c r="DE30" s="39"/>
-      <c r="DF30" s="39"/>
-      <c r="DG30" s="40"/>
-      <c r="DH30" s="38">
-        <v>781.02</v>
-      </c>
-      <c r="DI30" s="39"/>
-      <c r="DJ30" s="39"/>
-      <c r="DK30" s="39"/>
-      <c r="DL30" s="39"/>
-      <c r="DM30" s="39"/>
-      <c r="DN30" s="39"/>
-      <c r="DO30" s="39"/>
-      <c r="DP30" s="39"/>
-      <c r="DQ30" s="39"/>
-      <c r="DR30" s="39"/>
-      <c r="DS30" s="39"/>
-      <c r="DT30" s="39"/>
-      <c r="DU30" s="39"/>
-      <c r="DV30" s="40"/>
-      <c r="DW30" s="48"/>
-      <c r="DX30" s="49"/>
-      <c r="DY30" s="49"/>
-      <c r="DZ30" s="49"/>
-      <c r="EA30" s="49"/>
-      <c r="EB30" s="49"/>
-      <c r="EC30" s="49"/>
-      <c r="ED30" s="49"/>
-      <c r="EE30" s="49"/>
-      <c r="EF30" s="56"/>
-      <c r="EG30" s="53"/>
-      <c r="EH30" s="54"/>
-      <c r="EI30" s="54"/>
-      <c r="EJ30" s="54"/>
-      <c r="EK30" s="54"/>
-      <c r="EL30" s="54"/>
-      <c r="EM30" s="54"/>
-      <c r="EN30" s="54"/>
-      <c r="EO30" s="54"/>
-      <c r="EP30" s="54"/>
-      <c r="EQ30" s="54"/>
-      <c r="ER30" s="54"/>
-      <c r="ES30" s="55"/>
-      <c r="ET30" s="48"/>
-      <c r="EU30" s="49"/>
-      <c r="EV30" s="49"/>
-      <c r="EW30" s="49"/>
-      <c r="EX30" s="49"/>
-      <c r="EY30" s="49"/>
-      <c r="EZ30" s="49"/>
-      <c r="FA30" s="49"/>
-      <c r="FB30" s="49"/>
-      <c r="FC30" s="49"/>
-      <c r="FD30" s="49"/>
-      <c r="FE30" s="56"/>
+    <row r="31" spans="1:161" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH31" s="28"/>
+      <c r="AI31" s="28"/>
+      <c r="AJ31" s="28"/>
+      <c r="AK31" s="28"/>
+      <c r="AL31" s="28"/>
+      <c r="AM31" s="28"/>
+      <c r="AN31" s="28"/>
+      <c r="AO31" s="28"/>
+      <c r="AP31" s="28"/>
+      <c r="AQ31" s="28"/>
+      <c r="AR31" s="28"/>
+      <c r="AS31" s="28"/>
+      <c r="AT31" s="28"/>
+      <c r="AU31" s="28"/>
+      <c r="AV31" s="28"/>
+      <c r="AW31" s="28"/>
+      <c r="AZ31" s="28"/>
+      <c r="BA31" s="28"/>
+      <c r="BB31" s="28"/>
+      <c r="BC31" s="28"/>
+      <c r="BD31" s="28"/>
+      <c r="BE31" s="28"/>
+      <c r="BF31" s="28"/>
+      <c r="BG31" s="28"/>
+      <c r="BH31" s="28"/>
+      <c r="BI31" s="28"/>
+      <c r="BJ31" s="28"/>
+      <c r="BK31" s="28"/>
+      <c r="BL31" s="28"/>
+      <c r="BM31" s="28"/>
+      <c r="BN31" s="28"/>
+      <c r="BO31" s="28"/>
+      <c r="BP31" s="28"/>
+      <c r="BQ31" s="28"/>
+      <c r="BR31" s="28"/>
+      <c r="BS31" s="28"/>
+      <c r="BT31" s="28"/>
+      <c r="BU31" s="28"/>
+      <c r="BV31" s="28"/>
+      <c r="BW31" s="28"/>
+      <c r="BX31" s="28"/>
+      <c r="BY31" s="28"/>
+      <c r="BZ31" s="28"/>
+      <c r="CA31" s="28"/>
+      <c r="CB31" s="28"/>
+      <c r="CD31" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="DK31" s="28"/>
+      <c r="DL31" s="28"/>
+      <c r="DM31" s="28"/>
+      <c r="DN31" s="28"/>
+      <c r="DO31" s="28"/>
+      <c r="DP31" s="28"/>
+      <c r="DQ31" s="28"/>
+      <c r="DR31" s="28"/>
+      <c r="DS31" s="28"/>
+      <c r="DT31" s="28"/>
+      <c r="DU31" s="28"/>
+      <c r="DV31" s="28"/>
+      <c r="DW31" s="28"/>
+      <c r="DX31" s="28"/>
+      <c r="DY31" s="28"/>
+      <c r="DZ31" s="28"/>
+      <c r="EC31" s="28"/>
+      <c r="ED31" s="28"/>
+      <c r="EE31" s="28"/>
+      <c r="EF31" s="28"/>
+      <c r="EG31" s="28"/>
+      <c r="EH31" s="28"/>
+      <c r="EI31" s="28"/>
+      <c r="EJ31" s="28"/>
+      <c r="EK31" s="28"/>
+      <c r="EL31" s="28"/>
+      <c r="EM31" s="28"/>
+      <c r="EN31" s="28"/>
+      <c r="EO31" s="28"/>
+      <c r="EP31" s="28"/>
+      <c r="EQ31" s="28"/>
+      <c r="ER31" s="28"/>
+      <c r="ES31" s="28"/>
+      <c r="ET31" s="28"/>
+      <c r="EU31" s="28"/>
+      <c r="EV31" s="28"/>
+      <c r="EW31" s="28"/>
+      <c r="EX31" s="28"/>
+      <c r="EY31" s="28"/>
+      <c r="EZ31" s="28"/>
+      <c r="FA31" s="28"/>
+      <c r="FB31" s="28"/>
+      <c r="FC31" s="28"/>
+      <c r="FD31" s="28"/>
+      <c r="FE31" s="28"/>
     </row>
-    <row r="31" spans="1:161" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="42" t="s">
-        <v>79</v>
-      </c>
-      <c r="B31" s="43"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="43"/>
-      <c r="I31" s="43"/>
-      <c r="J31" s="43"/>
-      <c r="K31" s="43"/>
-      <c r="L31" s="43"/>
-      <c r="M31" s="43"/>
-      <c r="N31" s="43"/>
-      <c r="O31" s="43"/>
-      <c r="P31" s="43"/>
-      <c r="Q31" s="43"/>
-      <c r="R31" s="43"/>
-      <c r="S31" s="43"/>
-      <c r="T31" s="44"/>
-      <c r="U31" s="45"/>
-      <c r="V31" s="46"/>
-      <c r="W31" s="46"/>
-      <c r="X31" s="46"/>
-      <c r="Y31" s="46"/>
-      <c r="Z31" s="46"/>
-      <c r="AA31" s="46"/>
-      <c r="AB31" s="47"/>
-      <c r="AC31" s="48"/>
-      <c r="AD31" s="49"/>
-      <c r="AE31" s="49"/>
-      <c r="AF31" s="49"/>
-      <c r="AG31" s="49"/>
-      <c r="AH31" s="56"/>
-      <c r="AI31" s="50" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ31" s="51"/>
-      <c r="AK31" s="51"/>
-      <c r="AL31" s="51"/>
-      <c r="AM31" s="51"/>
-      <c r="AN31" s="51"/>
-      <c r="AO31" s="51"/>
-      <c r="AP31" s="51"/>
-      <c r="AQ31" s="51"/>
-      <c r="AR31" s="51"/>
-      <c r="AS31" s="52"/>
-      <c r="AT31" s="38">
-        <v>2</v>
-      </c>
-      <c r="AU31" s="39"/>
-      <c r="AV31" s="39"/>
-      <c r="AW31" s="39"/>
-      <c r="AX31" s="39"/>
-      <c r="AY31" s="39"/>
-      <c r="AZ31" s="39"/>
-      <c r="BA31" s="40"/>
-      <c r="BB31" s="38">
-        <v>446.02</v>
-      </c>
-      <c r="BC31" s="39"/>
-      <c r="BD31" s="39"/>
-      <c r="BE31" s="39"/>
-      <c r="BF31" s="39"/>
-      <c r="BG31" s="39"/>
-      <c r="BH31" s="39"/>
-      <c r="BI31" s="39"/>
-      <c r="BJ31" s="39"/>
-      <c r="BK31" s="39"/>
-      <c r="BL31" s="40"/>
-      <c r="BM31" s="38"/>
-      <c r="BN31" s="39"/>
-      <c r="BO31" s="39"/>
-      <c r="BP31" s="39"/>
-      <c r="BQ31" s="39"/>
-      <c r="BR31" s="39"/>
-      <c r="BS31" s="39"/>
-      <c r="BT31" s="39"/>
-      <c r="BU31" s="39"/>
-      <c r="BV31" s="39"/>
-      <c r="BW31" s="39"/>
-      <c r="BX31" s="39"/>
-      <c r="BY31" s="39"/>
-      <c r="BZ31" s="39"/>
-      <c r="CA31" s="40"/>
-      <c r="CB31" s="38"/>
-      <c r="CC31" s="39"/>
-      <c r="CD31" s="39"/>
-      <c r="CE31" s="39"/>
-      <c r="CF31" s="39"/>
-      <c r="CG31" s="39"/>
-      <c r="CH31" s="39"/>
-      <c r="CI31" s="39"/>
-      <c r="CJ31" s="39"/>
-      <c r="CK31" s="40"/>
-      <c r="CL31" s="38"/>
-      <c r="CM31" s="39"/>
-      <c r="CN31" s="39"/>
-      <c r="CO31" s="39"/>
-      <c r="CP31" s="39"/>
-      <c r="CQ31" s="39"/>
-      <c r="CR31" s="39"/>
-      <c r="CS31" s="39"/>
-      <c r="CT31" s="39"/>
-      <c r="CU31" s="40"/>
-      <c r="CV31" s="38"/>
-      <c r="CW31" s="39"/>
-      <c r="CX31" s="39"/>
-      <c r="CY31" s="39"/>
-      <c r="CZ31" s="39"/>
-      <c r="DA31" s="39"/>
-      <c r="DB31" s="39"/>
-      <c r="DC31" s="39"/>
-      <c r="DD31" s="39"/>
-      <c r="DE31" s="39"/>
-      <c r="DF31" s="39"/>
-      <c r="DG31" s="40"/>
-      <c r="DH31" s="38">
-        <v>892.04</v>
-      </c>
-      <c r="DI31" s="39"/>
-      <c r="DJ31" s="39"/>
-      <c r="DK31" s="39"/>
-      <c r="DL31" s="39"/>
-      <c r="DM31" s="39"/>
-      <c r="DN31" s="39"/>
-      <c r="DO31" s="39"/>
-      <c r="DP31" s="39"/>
-      <c r="DQ31" s="39"/>
-      <c r="DR31" s="39"/>
-      <c r="DS31" s="39"/>
-      <c r="DT31" s="39"/>
-      <c r="DU31" s="39"/>
-      <c r="DV31" s="40"/>
-      <c r="DW31" s="48"/>
-      <c r="DX31" s="49"/>
-      <c r="DY31" s="49"/>
-      <c r="DZ31" s="49"/>
-      <c r="EA31" s="49"/>
-      <c r="EB31" s="49"/>
-      <c r="EC31" s="49"/>
-      <c r="ED31" s="49"/>
-      <c r="EE31" s="49"/>
-      <c r="EF31" s="56"/>
-      <c r="EG31" s="53"/>
-      <c r="EH31" s="54"/>
-      <c r="EI31" s="54"/>
-      <c r="EJ31" s="54"/>
-      <c r="EK31" s="54"/>
-      <c r="EL31" s="54"/>
-      <c r="EM31" s="54"/>
-      <c r="EN31" s="54"/>
-      <c r="EO31" s="54"/>
-      <c r="EP31" s="54"/>
-      <c r="EQ31" s="54"/>
-      <c r="ER31" s="54"/>
-      <c r="ES31" s="55"/>
-      <c r="ET31" s="48"/>
-      <c r="EU31" s="49"/>
-      <c r="EV31" s="49"/>
-      <c r="EW31" s="49"/>
-      <c r="EX31" s="49"/>
-      <c r="EY31" s="49"/>
-      <c r="EZ31" s="49"/>
-      <c r="FA31" s="49"/>
-      <c r="FB31" s="49"/>
-      <c r="FC31" s="49"/>
-      <c r="FD31" s="49"/>
-      <c r="FE31" s="56"/>
+    <row r="32" spans="1:161" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH32" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="AI32" s="29"/>
+      <c r="AJ32" s="29"/>
+      <c r="AK32" s="29"/>
+      <c r="AL32" s="29"/>
+      <c r="AM32" s="29"/>
+      <c r="AN32" s="29"/>
+      <c r="AO32" s="29"/>
+      <c r="AP32" s="29"/>
+      <c r="AQ32" s="29"/>
+      <c r="AR32" s="29"/>
+      <c r="AS32" s="29"/>
+      <c r="AT32" s="29"/>
+      <c r="AU32" s="29"/>
+      <c r="AV32" s="29"/>
+      <c r="AW32" s="29"/>
+      <c r="AX32" s="6"/>
+      <c r="AY32" s="6"/>
+      <c r="AZ32" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="BA32" s="29"/>
+      <c r="BB32" s="29"/>
+      <c r="BC32" s="29"/>
+      <c r="BD32" s="29"/>
+      <c r="BE32" s="29"/>
+      <c r="BF32" s="29"/>
+      <c r="BG32" s="29"/>
+      <c r="BH32" s="29"/>
+      <c r="BI32" s="29"/>
+      <c r="BJ32" s="29"/>
+      <c r="BK32" s="29"/>
+      <c r="BL32" s="29"/>
+      <c r="BM32" s="29"/>
+      <c r="BN32" s="29"/>
+      <c r="BO32" s="29"/>
+      <c r="BP32" s="29"/>
+      <c r="BQ32" s="29"/>
+      <c r="BR32" s="29"/>
+      <c r="BS32" s="29"/>
+      <c r="BT32" s="29"/>
+      <c r="BU32" s="29"/>
+      <c r="BV32" s="29"/>
+      <c r="BW32" s="29"/>
+      <c r="BX32" s="29"/>
+      <c r="BY32" s="29"/>
+      <c r="BZ32" s="29"/>
+      <c r="CA32" s="29"/>
+      <c r="CB32" s="29"/>
+      <c r="DK32" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="DL32" s="29"/>
+      <c r="DM32" s="29"/>
+      <c r="DN32" s="29"/>
+      <c r="DO32" s="29"/>
+      <c r="DP32" s="29"/>
+      <c r="DQ32" s="29"/>
+      <c r="DR32" s="29"/>
+      <c r="DS32" s="29"/>
+      <c r="DT32" s="29"/>
+      <c r="DU32" s="29"/>
+      <c r="DV32" s="29"/>
+      <c r="DW32" s="29"/>
+      <c r="DX32" s="29"/>
+      <c r="DY32" s="29"/>
+      <c r="DZ32" s="29"/>
+      <c r="EA32" s="6"/>
+      <c r="EB32" s="6"/>
+      <c r="EC32" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="ED32" s="29"/>
+      <c r="EE32" s="29"/>
+      <c r="EF32" s="29"/>
+      <c r="EG32" s="29"/>
+      <c r="EH32" s="29"/>
+      <c r="EI32" s="29"/>
+      <c r="EJ32" s="29"/>
+      <c r="EK32" s="29"/>
+      <c r="EL32" s="29"/>
+      <c r="EM32" s="29"/>
+      <c r="EN32" s="29"/>
+      <c r="EO32" s="29"/>
+      <c r="EP32" s="29"/>
+      <c r="EQ32" s="29"/>
+      <c r="ER32" s="29"/>
+      <c r="ES32" s="29"/>
+      <c r="ET32" s="29"/>
+      <c r="EU32" s="29"/>
+      <c r="EV32" s="29"/>
+      <c r="EW32" s="29"/>
+      <c r="EX32" s="29"/>
+      <c r="EY32" s="29"/>
+      <c r="EZ32" s="29"/>
+      <c r="FA32" s="29"/>
+      <c r="FB32" s="29"/>
+      <c r="FC32" s="29"/>
+      <c r="FD32" s="29"/>
+      <c r="FE32" s="29"/>
     </row>
-    <row r="32" spans="1:161" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="42" t="s">
-        <v>80</v>
-      </c>
-      <c r="B32" s="43"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="43"/>
-      <c r="H32" s="43"/>
-      <c r="I32" s="43"/>
-      <c r="J32" s="43"/>
-      <c r="K32" s="43"/>
-      <c r="L32" s="43"/>
-      <c r="M32" s="43"/>
-      <c r="N32" s="43"/>
-      <c r="O32" s="43"/>
-      <c r="P32" s="43"/>
-      <c r="Q32" s="43"/>
-      <c r="R32" s="43"/>
-      <c r="S32" s="43"/>
-      <c r="T32" s="44"/>
-      <c r="U32" s="45"/>
-      <c r="V32" s="46"/>
-      <c r="W32" s="46"/>
-      <c r="X32" s="46"/>
-      <c r="Y32" s="46"/>
-      <c r="Z32" s="46"/>
-      <c r="AA32" s="46"/>
-      <c r="AB32" s="47"/>
-      <c r="AC32" s="48"/>
-      <c r="AD32" s="49"/>
-      <c r="AE32" s="49"/>
-      <c r="AF32" s="49"/>
-      <c r="AG32" s="49"/>
-      <c r="AH32" s="56"/>
-      <c r="AI32" s="50" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ32" s="51"/>
-      <c r="AK32" s="51"/>
-      <c r="AL32" s="51"/>
-      <c r="AM32" s="51"/>
-      <c r="AN32" s="51"/>
-      <c r="AO32" s="51"/>
-      <c r="AP32" s="51"/>
-      <c r="AQ32" s="51"/>
-      <c r="AR32" s="51"/>
-      <c r="AS32" s="52"/>
-      <c r="AT32" s="38">
-        <v>2</v>
-      </c>
-      <c r="AU32" s="39"/>
-      <c r="AV32" s="39"/>
-      <c r="AW32" s="39"/>
-      <c r="AX32" s="39"/>
-      <c r="AY32" s="39"/>
-      <c r="AZ32" s="39"/>
-      <c r="BA32" s="40"/>
-      <c r="BB32" s="38">
-        <v>612.5</v>
-      </c>
-      <c r="BC32" s="39"/>
-      <c r="BD32" s="39"/>
-      <c r="BE32" s="39"/>
-      <c r="BF32" s="39"/>
-      <c r="BG32" s="39"/>
-      <c r="BH32" s="39"/>
-      <c r="BI32" s="39"/>
-      <c r="BJ32" s="39"/>
-      <c r="BK32" s="39"/>
-      <c r="BL32" s="40"/>
-      <c r="BM32" s="38"/>
-      <c r="BN32" s="39"/>
-      <c r="BO32" s="39"/>
-      <c r="BP32" s="39"/>
-      <c r="BQ32" s="39"/>
-      <c r="BR32" s="39"/>
-      <c r="BS32" s="39"/>
-      <c r="BT32" s="39"/>
-      <c r="BU32" s="39"/>
-      <c r="BV32" s="39"/>
-      <c r="BW32" s="39"/>
-      <c r="BX32" s="39"/>
-      <c r="BY32" s="39"/>
-      <c r="BZ32" s="39"/>
-      <c r="CA32" s="40"/>
-      <c r="CB32" s="38"/>
-      <c r="CC32" s="39"/>
-      <c r="CD32" s="39"/>
-      <c r="CE32" s="39"/>
-      <c r="CF32" s="39"/>
-      <c r="CG32" s="39"/>
-      <c r="CH32" s="39"/>
-      <c r="CI32" s="39"/>
-      <c r="CJ32" s="39"/>
-      <c r="CK32" s="40"/>
-      <c r="CL32" s="38"/>
-      <c r="CM32" s="39"/>
-      <c r="CN32" s="39"/>
-      <c r="CO32" s="39"/>
-      <c r="CP32" s="39"/>
-      <c r="CQ32" s="39"/>
-      <c r="CR32" s="39"/>
-      <c r="CS32" s="39"/>
-      <c r="CT32" s="39"/>
-      <c r="CU32" s="40"/>
-      <c r="CV32" s="38"/>
-      <c r="CW32" s="39"/>
-      <c r="CX32" s="39"/>
-      <c r="CY32" s="39"/>
-      <c r="CZ32" s="39"/>
-      <c r="DA32" s="39"/>
-      <c r="DB32" s="39"/>
-      <c r="DC32" s="39"/>
-      <c r="DD32" s="39"/>
-      <c r="DE32" s="39"/>
-      <c r="DF32" s="39"/>
-      <c r="DG32" s="40"/>
-      <c r="DH32" s="38">
-        <v>1225</v>
-      </c>
-      <c r="DI32" s="39"/>
-      <c r="DJ32" s="39"/>
-      <c r="DK32" s="39"/>
-      <c r="DL32" s="39"/>
-      <c r="DM32" s="39"/>
-      <c r="DN32" s="39"/>
-      <c r="DO32" s="39"/>
-      <c r="DP32" s="39"/>
-      <c r="DQ32" s="39"/>
-      <c r="DR32" s="39"/>
-      <c r="DS32" s="39"/>
-      <c r="DT32" s="39"/>
-      <c r="DU32" s="39"/>
-      <c r="DV32" s="40"/>
-      <c r="DW32" s="48"/>
-      <c r="DX32" s="49"/>
-      <c r="DY32" s="49"/>
-      <c r="DZ32" s="49"/>
-      <c r="EA32" s="49"/>
-      <c r="EB32" s="49"/>
-      <c r="EC32" s="49"/>
-      <c r="ED32" s="49"/>
-      <c r="EE32" s="49"/>
-      <c r="EF32" s="56"/>
-      <c r="EG32" s="53"/>
-      <c r="EH32" s="54"/>
-      <c r="EI32" s="54"/>
-      <c r="EJ32" s="54"/>
-      <c r="EK32" s="54"/>
-      <c r="EL32" s="54"/>
-      <c r="EM32" s="54"/>
-      <c r="EN32" s="54"/>
-      <c r="EO32" s="54"/>
-      <c r="EP32" s="54"/>
-      <c r="EQ32" s="54"/>
-      <c r="ER32" s="54"/>
-      <c r="ES32" s="55"/>
-      <c r="ET32" s="48"/>
-      <c r="EU32" s="49"/>
-      <c r="EV32" s="49"/>
-      <c r="EW32" s="49"/>
-      <c r="EX32" s="49"/>
-      <c r="EY32" s="49"/>
-      <c r="EZ32" s="49"/>
-      <c r="FA32" s="49"/>
-      <c r="FB32" s="49"/>
-      <c r="FC32" s="49"/>
-      <c r="FD32" s="49"/>
-      <c r="FE32" s="56"/>
+    <row r="33" spans="1:161" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="33" spans="1:161" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="42" t="s">
-        <v>81</v>
-      </c>
-      <c r="B33" s="43"/>
-      <c r="C33" s="43"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="43"/>
-      <c r="H33" s="43"/>
-      <c r="I33" s="43"/>
-      <c r="J33" s="43"/>
-      <c r="K33" s="43"/>
-      <c r="L33" s="43"/>
-      <c r="M33" s="43"/>
-      <c r="N33" s="43"/>
-      <c r="O33" s="43"/>
-      <c r="P33" s="43"/>
-      <c r="Q33" s="43"/>
-      <c r="R33" s="43"/>
-      <c r="S33" s="43"/>
-      <c r="T33" s="44"/>
-      <c r="U33" s="45"/>
-      <c r="V33" s="46"/>
-      <c r="W33" s="46"/>
-      <c r="X33" s="46"/>
-      <c r="Y33" s="46"/>
-      <c r="Z33" s="46"/>
-      <c r="AA33" s="46"/>
-      <c r="AB33" s="47"/>
-      <c r="AC33" s="48"/>
-      <c r="AD33" s="49"/>
-      <c r="AE33" s="49"/>
-      <c r="AF33" s="49"/>
-      <c r="AG33" s="49"/>
-      <c r="AH33" s="56"/>
-      <c r="AI33" s="50" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ33" s="51"/>
-      <c r="AK33" s="51"/>
-      <c r="AL33" s="51"/>
-      <c r="AM33" s="51"/>
-      <c r="AN33" s="51"/>
-      <c r="AO33" s="51"/>
-      <c r="AP33" s="51"/>
-      <c r="AQ33" s="51"/>
-      <c r="AR33" s="51"/>
-      <c r="AS33" s="52"/>
-      <c r="AT33" s="38">
-        <v>3</v>
-      </c>
-      <c r="AU33" s="39"/>
-      <c r="AV33" s="39"/>
-      <c r="AW33" s="39"/>
-      <c r="AX33" s="39"/>
-      <c r="AY33" s="39"/>
-      <c r="AZ33" s="39"/>
-      <c r="BA33" s="40"/>
-      <c r="BB33" s="38">
-        <v>427.27</v>
-      </c>
-      <c r="BC33" s="39"/>
-      <c r="BD33" s="39"/>
-      <c r="BE33" s="39"/>
-      <c r="BF33" s="39"/>
-      <c r="BG33" s="39"/>
-      <c r="BH33" s="39"/>
-      <c r="BI33" s="39"/>
-      <c r="BJ33" s="39"/>
-      <c r="BK33" s="39"/>
-      <c r="BL33" s="40"/>
-      <c r="BM33" s="38"/>
-      <c r="BN33" s="39"/>
-      <c r="BO33" s="39"/>
-      <c r="BP33" s="39"/>
-      <c r="BQ33" s="39"/>
-      <c r="BR33" s="39"/>
-      <c r="BS33" s="39"/>
-      <c r="BT33" s="39"/>
-      <c r="BU33" s="39"/>
-      <c r="BV33" s="39"/>
-      <c r="BW33" s="39"/>
-      <c r="BX33" s="39"/>
-      <c r="BY33" s="39"/>
-      <c r="BZ33" s="39"/>
-      <c r="CA33" s="40"/>
-      <c r="CB33" s="38"/>
-      <c r="CC33" s="39"/>
-      <c r="CD33" s="39"/>
-      <c r="CE33" s="39"/>
-      <c r="CF33" s="39"/>
-      <c r="CG33" s="39"/>
-      <c r="CH33" s="39"/>
-      <c r="CI33" s="39"/>
-      <c r="CJ33" s="39"/>
-      <c r="CK33" s="40"/>
-      <c r="CL33" s="38"/>
-      <c r="CM33" s="39"/>
-      <c r="CN33" s="39"/>
-      <c r="CO33" s="39"/>
-      <c r="CP33" s="39"/>
-      <c r="CQ33" s="39"/>
-      <c r="CR33" s="39"/>
-      <c r="CS33" s="39"/>
-      <c r="CT33" s="39"/>
-      <c r="CU33" s="40"/>
-      <c r="CV33" s="38"/>
-      <c r="CW33" s="39"/>
-      <c r="CX33" s="39"/>
-      <c r="CY33" s="39"/>
-      <c r="CZ33" s="39"/>
-      <c r="DA33" s="39"/>
-      <c r="DB33" s="39"/>
-      <c r="DC33" s="39"/>
-      <c r="DD33" s="39"/>
-      <c r="DE33" s="39"/>
-      <c r="DF33" s="39"/>
-      <c r="DG33" s="40"/>
-      <c r="DH33" s="38">
-        <v>1281.81</v>
-      </c>
-      <c r="DI33" s="39"/>
-      <c r="DJ33" s="39"/>
-      <c r="DK33" s="39"/>
-      <c r="DL33" s="39"/>
-      <c r="DM33" s="39"/>
-      <c r="DN33" s="39"/>
-      <c r="DO33" s="39"/>
-      <c r="DP33" s="39"/>
-      <c r="DQ33" s="39"/>
-      <c r="DR33" s="39"/>
-      <c r="DS33" s="39"/>
-      <c r="DT33" s="39"/>
-      <c r="DU33" s="39"/>
-      <c r="DV33" s="40"/>
-      <c r="DW33" s="48"/>
-      <c r="DX33" s="49"/>
-      <c r="DY33" s="49"/>
-      <c r="DZ33" s="49"/>
-      <c r="EA33" s="49"/>
-      <c r="EB33" s="49"/>
-      <c r="EC33" s="49"/>
-      <c r="ED33" s="49"/>
-      <c r="EE33" s="49"/>
-      <c r="EF33" s="56"/>
-      <c r="EG33" s="53"/>
-      <c r="EH33" s="54"/>
-      <c r="EI33" s="54"/>
-      <c r="EJ33" s="54"/>
-      <c r="EK33" s="54"/>
-      <c r="EL33" s="54"/>
-      <c r="EM33" s="54"/>
-      <c r="EN33" s="54"/>
-      <c r="EO33" s="54"/>
-      <c r="EP33" s="54"/>
-      <c r="EQ33" s="54"/>
-      <c r="ER33" s="54"/>
-      <c r="ES33" s="55"/>
-      <c r="ET33" s="48"/>
-      <c r="EU33" s="49"/>
-      <c r="EV33" s="49"/>
-      <c r="EW33" s="49"/>
-      <c r="EX33" s="49"/>
-      <c r="EY33" s="49"/>
-      <c r="EZ33" s="49"/>
-      <c r="FA33" s="49"/>
-      <c r="FB33" s="49"/>
-      <c r="FC33" s="49"/>
-      <c r="FD33" s="49"/>
-      <c r="FE33" s="56"/>
+    <row r="34" spans="1:161" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM34" s="28"/>
+      <c r="AN34" s="28"/>
+      <c r="AO34" s="28"/>
+      <c r="AP34" s="28"/>
+      <c r="AQ34" s="28"/>
+      <c r="AR34" s="28"/>
+      <c r="AS34" s="28"/>
+      <c r="AT34" s="28"/>
+      <c r="AU34" s="28"/>
+      <c r="AV34" s="28"/>
+      <c r="AW34" s="28"/>
+      <c r="AX34" s="28"/>
+      <c r="AY34" s="28"/>
+      <c r="AZ34" s="28"/>
+      <c r="BA34" s="28"/>
+      <c r="BB34" s="28"/>
+      <c r="BE34" s="28"/>
+      <c r="BF34" s="28"/>
+      <c r="BG34" s="28"/>
+      <c r="BH34" s="28"/>
+      <c r="BI34" s="28"/>
+      <c r="BJ34" s="28"/>
+      <c r="BK34" s="28"/>
+      <c r="BL34" s="28"/>
+      <c r="BM34" s="28"/>
+      <c r="BN34" s="28"/>
+      <c r="BO34" s="28"/>
+      <c r="BP34" s="28"/>
+      <c r="BQ34" s="28"/>
+      <c r="BR34" s="28"/>
+      <c r="BS34" s="28"/>
+      <c r="BT34" s="28"/>
+      <c r="BU34" s="28"/>
+      <c r="BV34" s="28"/>
+      <c r="BW34" s="28"/>
+      <c r="BX34" s="28"/>
+      <c r="BY34" s="28"/>
+      <c r="BZ34" s="28"/>
+      <c r="CA34" s="28"/>
+      <c r="CB34" s="28"/>
+      <c r="CC34" s="28"/>
+      <c r="CD34" s="28"/>
+      <c r="CE34" s="28"/>
+      <c r="CF34" s="28"/>
+      <c r="CG34" s="28"/>
+      <c r="CI34" s="27"/>
+      <c r="CJ34" s="27"/>
+      <c r="CK34" s="27"/>
+      <c r="CL34" s="27"/>
+      <c r="CM34" s="27"/>
+      <c r="CN34" s="27"/>
+      <c r="CO34" s="27"/>
+      <c r="CP34" s="27"/>
+      <c r="CQ34" s="27"/>
+      <c r="CR34" s="27"/>
+      <c r="CS34" s="27"/>
+      <c r="CT34" s="27"/>
+      <c r="CU34" s="27"/>
+      <c r="CV34" s="27"/>
+      <c r="CW34" s="27"/>
+      <c r="CX34" s="27"/>
+      <c r="CY34" s="27"/>
+      <c r="CZ34" s="27"/>
+      <c r="DA34" s="27"/>
+      <c r="DB34" s="27"/>
+      <c r="DC34" s="27"/>
+      <c r="DD34" s="27"/>
+      <c r="DE34" s="27"/>
+      <c r="DF34" s="27"/>
+      <c r="DG34" s="27"/>
+      <c r="DH34" s="27"/>
+      <c r="DI34" s="27"/>
+      <c r="DJ34" s="27"/>
+      <c r="DK34" s="27"/>
+      <c r="DL34" s="27"/>
+      <c r="DM34" s="27"/>
+      <c r="DN34" s="27"/>
+      <c r="DO34" s="27"/>
+      <c r="DP34" s="27"/>
+      <c r="DQ34" s="27"/>
+      <c r="DR34" s="27"/>
+      <c r="DS34" s="27"/>
+      <c r="DT34" s="27"/>
+      <c r="DU34" s="27"/>
+      <c r="DV34" s="27"/>
+      <c r="DW34" s="27"/>
+      <c r="DX34" s="27"/>
+      <c r="DY34" s="27"/>
+      <c r="DZ34" s="27"/>
+      <c r="EA34" s="27"/>
+      <c r="EB34" s="27"/>
+      <c r="EC34" s="27"/>
+      <c r="ED34" s="27"/>
+      <c r="EE34" s="27"/>
+      <c r="EF34" s="27"/>
+      <c r="EG34" s="27"/>
+      <c r="EH34" s="27"/>
+      <c r="EI34" s="27"/>
+      <c r="EJ34" s="27"/>
+      <c r="EK34" s="27"/>
+      <c r="EL34" s="27"/>
+      <c r="EM34" s="27"/>
+      <c r="EN34" s="27"/>
+      <c r="EO34" s="27"/>
+      <c r="EP34" s="27"/>
+      <c r="EQ34" s="27"/>
+      <c r="ER34" s="27"/>
+      <c r="ES34" s="27"/>
+      <c r="ET34" s="27"/>
+      <c r="EU34" s="27"/>
+      <c r="EV34" s="27"/>
+      <c r="EW34" s="27"/>
+      <c r="EX34" s="27"/>
+      <c r="EY34" s="27"/>
+      <c r="EZ34" s="27"/>
+      <c r="FA34" s="27"/>
+      <c r="FB34" s="27"/>
+      <c r="FC34" s="27"/>
+      <c r="FD34" s="27"/>
+      <c r="FE34" s="27"/>
     </row>
-    <row r="34" spans="1:161" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="42" t="s">
-        <v>82</v>
-      </c>
-      <c r="B34" s="43"/>
-      <c r="C34" s="43"/>
-      <c r="D34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="43"/>
-      <c r="H34" s="43"/>
-      <c r="I34" s="43"/>
-      <c r="J34" s="43"/>
-      <c r="K34" s="43"/>
-      <c r="L34" s="43"/>
-      <c r="M34" s="43"/>
-      <c r="N34" s="43"/>
-      <c r="O34" s="43"/>
-      <c r="P34" s="43"/>
-      <c r="Q34" s="43"/>
-      <c r="R34" s="43"/>
-      <c r="S34" s="43"/>
-      <c r="T34" s="44"/>
-      <c r="U34" s="45"/>
-      <c r="V34" s="46"/>
-      <c r="W34" s="46"/>
-      <c r="X34" s="46"/>
-      <c r="Y34" s="46"/>
-      <c r="Z34" s="46"/>
-      <c r="AA34" s="46"/>
-      <c r="AB34" s="47"/>
-      <c r="AC34" s="48"/>
-      <c r="AD34" s="49"/>
-      <c r="AE34" s="49"/>
-      <c r="AF34" s="49"/>
-      <c r="AG34" s="49"/>
-      <c r="AH34" s="56"/>
-      <c r="AI34" s="50" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ34" s="51"/>
-      <c r="AK34" s="51"/>
-      <c r="AL34" s="51"/>
-      <c r="AM34" s="51"/>
-      <c r="AN34" s="51"/>
-      <c r="AO34" s="51"/>
-      <c r="AP34" s="51"/>
-      <c r="AQ34" s="51"/>
-      <c r="AR34" s="51"/>
-      <c r="AS34" s="52"/>
-      <c r="AT34" s="38">
-        <v>11</v>
-      </c>
-      <c r="AU34" s="39"/>
-      <c r="AV34" s="39"/>
-      <c r="AW34" s="39"/>
-      <c r="AX34" s="39"/>
-      <c r="AY34" s="39"/>
-      <c r="AZ34" s="39"/>
-      <c r="BA34" s="40"/>
-      <c r="BB34" s="38">
-        <v>202.83</v>
-      </c>
-      <c r="BC34" s="39"/>
-      <c r="BD34" s="39"/>
-      <c r="BE34" s="39"/>
-      <c r="BF34" s="39"/>
-      <c r="BG34" s="39"/>
-      <c r="BH34" s="39"/>
-      <c r="BI34" s="39"/>
-      <c r="BJ34" s="39"/>
-      <c r="BK34" s="39"/>
-      <c r="BL34" s="40"/>
-      <c r="BM34" s="38"/>
-      <c r="BN34" s="39"/>
-      <c r="BO34" s="39"/>
-      <c r="BP34" s="39"/>
-      <c r="BQ34" s="39"/>
-      <c r="BR34" s="39"/>
-      <c r="BS34" s="39"/>
-      <c r="BT34" s="39"/>
-      <c r="BU34" s="39"/>
-      <c r="BV34" s="39"/>
-      <c r="BW34" s="39"/>
-      <c r="BX34" s="39"/>
-      <c r="BY34" s="39"/>
-      <c r="BZ34" s="39"/>
-      <c r="CA34" s="40"/>
-      <c r="CB34" s="38"/>
-      <c r="CC34" s="39"/>
-      <c r="CD34" s="39"/>
-      <c r="CE34" s="39"/>
-      <c r="CF34" s="39"/>
-      <c r="CG34" s="39"/>
-      <c r="CH34" s="39"/>
-      <c r="CI34" s="39"/>
-      <c r="CJ34" s="39"/>
-      <c r="CK34" s="40"/>
-      <c r="CL34" s="38"/>
-      <c r="CM34" s="39"/>
-      <c r="CN34" s="39"/>
-      <c r="CO34" s="39"/>
-      <c r="CP34" s="39"/>
-      <c r="CQ34" s="39"/>
-      <c r="CR34" s="39"/>
-      <c r="CS34" s="39"/>
-      <c r="CT34" s="39"/>
-      <c r="CU34" s="40"/>
-      <c r="CV34" s="38"/>
-      <c r="CW34" s="39"/>
-      <c r="CX34" s="39"/>
-      <c r="CY34" s="39"/>
-      <c r="CZ34" s="39"/>
-      <c r="DA34" s="39"/>
-      <c r="DB34" s="39"/>
-      <c r="DC34" s="39"/>
-      <c r="DD34" s="39"/>
-      <c r="DE34" s="39"/>
-      <c r="DF34" s="39"/>
-      <c r="DG34" s="40"/>
-      <c r="DH34" s="38">
-        <v>2231.13</v>
-      </c>
-      <c r="DI34" s="39"/>
-      <c r="DJ34" s="39"/>
-      <c r="DK34" s="39"/>
-      <c r="DL34" s="39"/>
-      <c r="DM34" s="39"/>
-      <c r="DN34" s="39"/>
-      <c r="DO34" s="39"/>
-      <c r="DP34" s="39"/>
-      <c r="DQ34" s="39"/>
-      <c r="DR34" s="39"/>
-      <c r="DS34" s="39"/>
-      <c r="DT34" s="39"/>
-      <c r="DU34" s="39"/>
-      <c r="DV34" s="40"/>
-      <c r="DW34" s="48"/>
-      <c r="DX34" s="49"/>
-      <c r="DY34" s="49"/>
-      <c r="DZ34" s="49"/>
-      <c r="EA34" s="49"/>
-      <c r="EB34" s="49"/>
-      <c r="EC34" s="49"/>
-      <c r="ED34" s="49"/>
-      <c r="EE34" s="49"/>
-      <c r="EF34" s="56"/>
-      <c r="EG34" s="53"/>
-      <c r="EH34" s="54"/>
-      <c r="EI34" s="54"/>
-      <c r="EJ34" s="54"/>
-      <c r="EK34" s="54"/>
-      <c r="EL34" s="54"/>
-      <c r="EM34" s="54"/>
-      <c r="EN34" s="54"/>
-      <c r="EO34" s="54"/>
-      <c r="EP34" s="54"/>
-      <c r="EQ34" s="54"/>
-      <c r="ER34" s="54"/>
-      <c r="ES34" s="55"/>
-      <c r="ET34" s="48"/>
-      <c r="EU34" s="49"/>
-      <c r="EV34" s="49"/>
-      <c r="EW34" s="49"/>
-      <c r="EX34" s="49"/>
-      <c r="EY34" s="49"/>
-      <c r="EZ34" s="49"/>
-      <c r="FA34" s="49"/>
-      <c r="FB34" s="49"/>
-      <c r="FC34" s="49"/>
-      <c r="FD34" s="49"/>
-      <c r="FE34" s="56"/>
+    <row r="35" spans="1:161" s="7" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AM35" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="AN35" s="29"/>
+      <c r="AO35" s="29"/>
+      <c r="AP35" s="29"/>
+      <c r="AQ35" s="29"/>
+      <c r="AR35" s="29"/>
+      <c r="AS35" s="29"/>
+      <c r="AT35" s="29"/>
+      <c r="AU35" s="29"/>
+      <c r="AV35" s="29"/>
+      <c r="AW35" s="29"/>
+      <c r="AX35" s="29"/>
+      <c r="AY35" s="29"/>
+      <c r="AZ35" s="29"/>
+      <c r="BA35" s="29"/>
+      <c r="BB35" s="29"/>
+      <c r="BC35" s="6"/>
+      <c r="BD35" s="6"/>
+      <c r="BE35" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="BF35" s="29"/>
+      <c r="BG35" s="29"/>
+      <c r="BH35" s="29"/>
+      <c r="BI35" s="29"/>
+      <c r="BJ35" s="29"/>
+      <c r="BK35" s="29"/>
+      <c r="BL35" s="29"/>
+      <c r="BM35" s="29"/>
+      <c r="BN35" s="29"/>
+      <c r="BO35" s="29"/>
+      <c r="BP35" s="29"/>
+      <c r="BQ35" s="29"/>
+      <c r="BR35" s="29"/>
+      <c r="BS35" s="29"/>
+      <c r="BT35" s="29"/>
+      <c r="BU35" s="29"/>
+      <c r="BV35" s="29"/>
+      <c r="BW35" s="29"/>
+      <c r="BX35" s="29"/>
+      <c r="BY35" s="29"/>
+      <c r="BZ35" s="29"/>
+      <c r="CA35" s="29"/>
+      <c r="CB35" s="29"/>
+      <c r="CC35" s="29"/>
+      <c r="CD35" s="29"/>
+      <c r="CE35" s="29"/>
+      <c r="CF35" s="29"/>
+      <c r="CG35" s="29"/>
+      <c r="CI35" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="CJ35" s="34"/>
+      <c r="CK35" s="34"/>
+      <c r="CL35" s="34"/>
+      <c r="CM35" s="34"/>
+      <c r="CN35" s="34"/>
+      <c r="CO35" s="34"/>
+      <c r="CP35" s="34"/>
+      <c r="CQ35" s="34"/>
+      <c r="CR35" s="34"/>
+      <c r="CS35" s="34"/>
+      <c r="CT35" s="34"/>
+      <c r="CU35" s="34"/>
+      <c r="CV35" s="34"/>
+      <c r="CW35" s="34"/>
+      <c r="CX35" s="34"/>
+      <c r="CY35" s="34"/>
+      <c r="CZ35" s="34"/>
+      <c r="DA35" s="34"/>
+      <c r="DB35" s="34"/>
+      <c r="DC35" s="34"/>
+      <c r="DD35" s="34"/>
+      <c r="DE35" s="34"/>
+      <c r="DF35" s="34"/>
+      <c r="DG35" s="34"/>
+      <c r="DH35" s="34"/>
+      <c r="DI35" s="34"/>
+      <c r="DJ35" s="34"/>
+      <c r="DK35" s="34"/>
+      <c r="DL35" s="34"/>
+      <c r="DM35" s="34"/>
+      <c r="DN35" s="34"/>
+      <c r="DO35" s="34"/>
+      <c r="DP35" s="34"/>
+      <c r="DQ35" s="34"/>
+      <c r="DR35" s="34"/>
+      <c r="DS35" s="34"/>
+      <c r="DT35" s="34"/>
+      <c r="DU35" s="34"/>
+      <c r="DV35" s="34"/>
+      <c r="DW35" s="34"/>
+      <c r="DX35" s="34"/>
+      <c r="DY35" s="34"/>
+      <c r="DZ35" s="34"/>
+      <c r="EA35" s="34"/>
+      <c r="EB35" s="34"/>
+      <c r="EC35" s="34"/>
+      <c r="ED35" s="34"/>
+      <c r="EE35" s="34"/>
+      <c r="EF35" s="34"/>
+      <c r="EG35" s="34"/>
+      <c r="EH35" s="34"/>
+      <c r="EI35" s="34"/>
+      <c r="EJ35" s="34"/>
+      <c r="EK35" s="34"/>
+      <c r="EL35" s="34"/>
+      <c r="EM35" s="34"/>
+      <c r="EN35" s="34"/>
+      <c r="EO35" s="34"/>
+      <c r="EP35" s="34"/>
+      <c r="EQ35" s="34"/>
+      <c r="ER35" s="34"/>
+      <c r="ES35" s="34"/>
+      <c r="ET35" s="34"/>
+      <c r="EU35" s="34"/>
+      <c r="EV35" s="34"/>
+      <c r="EW35" s="34"/>
+      <c r="EX35" s="34"/>
+      <c r="EY35" s="34"/>
+      <c r="EZ35" s="34"/>
+      <c r="FA35" s="34"/>
+      <c r="FB35" s="34"/>
+      <c r="FC35" s="34"/>
+      <c r="FD35" s="34"/>
+      <c r="FE35" s="34"/>
     </row>
-    <row r="35" spans="1:161" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A35" s="42"/>
-      <c r="B35" s="43"/>
-      <c r="C35" s="43"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="43"/>
-      <c r="K35" s="43"/>
-      <c r="L35" s="43"/>
-      <c r="M35" s="43"/>
-      <c r="N35" s="43"/>
-      <c r="O35" s="43"/>
-      <c r="P35" s="43"/>
-      <c r="Q35" s="43"/>
-      <c r="R35" s="43"/>
-      <c r="S35" s="43"/>
-      <c r="T35" s="44"/>
-      <c r="U35" s="45"/>
-      <c r="V35" s="46"/>
-      <c r="W35" s="46"/>
-      <c r="X35" s="46"/>
-      <c r="Y35" s="46"/>
-      <c r="Z35" s="46"/>
-      <c r="AA35" s="46"/>
-      <c r="AB35" s="47"/>
-      <c r="AC35" s="48"/>
-      <c r="AD35" s="49"/>
-      <c r="AE35" s="49"/>
-      <c r="AF35" s="49"/>
-      <c r="AG35" s="49"/>
-      <c r="AH35" s="49"/>
-      <c r="AI35" s="50"/>
-      <c r="AJ35" s="51"/>
-      <c r="AK35" s="51"/>
-      <c r="AL35" s="51"/>
-      <c r="AM35" s="51"/>
-      <c r="AN35" s="51"/>
-      <c r="AO35" s="51"/>
-      <c r="AP35" s="51"/>
-      <c r="AQ35" s="51"/>
-      <c r="AR35" s="51"/>
-      <c r="AS35" s="52"/>
-      <c r="AT35" s="38"/>
-      <c r="AU35" s="39"/>
-      <c r="AV35" s="39"/>
-      <c r="AW35" s="39"/>
-      <c r="AX35" s="39"/>
-      <c r="AY35" s="39"/>
-      <c r="AZ35" s="39"/>
-      <c r="BA35" s="40"/>
-      <c r="BB35" s="38"/>
-      <c r="BC35" s="39"/>
-      <c r="BD35" s="39"/>
-      <c r="BE35" s="39"/>
-      <c r="BF35" s="39"/>
-      <c r="BG35" s="39"/>
-      <c r="BH35" s="39"/>
-      <c r="BI35" s="39"/>
-      <c r="BJ35" s="39"/>
-      <c r="BK35" s="39"/>
-      <c r="BL35" s="40"/>
-      <c r="BM35" s="38"/>
-      <c r="BN35" s="39"/>
-      <c r="BO35" s="39"/>
-      <c r="BP35" s="39"/>
-      <c r="BQ35" s="39"/>
-      <c r="BR35" s="39"/>
-      <c r="BS35" s="39"/>
-      <c r="BT35" s="39"/>
-      <c r="BU35" s="39"/>
-      <c r="BV35" s="39"/>
-      <c r="BW35" s="39"/>
-      <c r="BX35" s="39"/>
-      <c r="BY35" s="39"/>
-      <c r="BZ35" s="39"/>
-      <c r="CA35" s="40"/>
-      <c r="CB35" s="38"/>
-      <c r="CC35" s="39"/>
-      <c r="CD35" s="39"/>
-      <c r="CE35" s="39"/>
-      <c r="CF35" s="39"/>
-      <c r="CG35" s="39"/>
-      <c r="CH35" s="39"/>
-      <c r="CI35" s="39"/>
-      <c r="CJ35" s="39"/>
-      <c r="CK35" s="40"/>
-      <c r="CL35" s="38"/>
-      <c r="CM35" s="39"/>
-      <c r="CN35" s="39"/>
-      <c r="CO35" s="39"/>
-      <c r="CP35" s="39"/>
-      <c r="CQ35" s="39"/>
-      <c r="CR35" s="39"/>
-      <c r="CS35" s="39"/>
-      <c r="CT35" s="39"/>
-      <c r="CU35" s="40"/>
-      <c r="CV35" s="38"/>
-      <c r="CW35" s="39"/>
-      <c r="CX35" s="39"/>
-      <c r="CY35" s="39"/>
-      <c r="CZ35" s="39"/>
-      <c r="DA35" s="39"/>
-      <c r="DB35" s="39"/>
-      <c r="DC35" s="39"/>
-      <c r="DD35" s="39"/>
-      <c r="DE35" s="39"/>
-      <c r="DF35" s="39"/>
-      <c r="DG35" s="40"/>
-      <c r="DH35" s="38"/>
-      <c r="DI35" s="39"/>
-      <c r="DJ35" s="39"/>
-      <c r="DK35" s="39"/>
-      <c r="DL35" s="39"/>
-      <c r="DM35" s="39"/>
-      <c r="DN35" s="39"/>
-      <c r="DO35" s="39"/>
-      <c r="DP35" s="39"/>
-      <c r="DQ35" s="39"/>
-      <c r="DR35" s="39"/>
-      <c r="DS35" s="39"/>
-      <c r="DT35" s="39"/>
-      <c r="DU35" s="39"/>
-      <c r="DV35" s="40"/>
-      <c r="DW35" s="48"/>
-      <c r="DX35" s="49"/>
-      <c r="DY35" s="49"/>
-      <c r="DZ35" s="49"/>
-      <c r="EA35" s="49"/>
-      <c r="EB35" s="49"/>
-      <c r="EC35" s="49"/>
-      <c r="ED35" s="49"/>
-      <c r="EE35" s="49"/>
-      <c r="EF35" s="49"/>
-      <c r="EG35" s="53"/>
-      <c r="EH35" s="54"/>
-      <c r="EI35" s="54"/>
-      <c r="EJ35" s="54"/>
-      <c r="EK35" s="54"/>
-      <c r="EL35" s="54"/>
-      <c r="EM35" s="54"/>
-      <c r="EN35" s="54"/>
-      <c r="EO35" s="54"/>
-      <c r="EP35" s="54"/>
-      <c r="EQ35" s="54"/>
-      <c r="ER35" s="54"/>
-      <c r="ES35" s="55"/>
-      <c r="ET35" s="41"/>
-      <c r="EU35" s="41"/>
-      <c r="EV35" s="41"/>
-      <c r="EW35" s="41"/>
-      <c r="EX35" s="41"/>
-      <c r="EY35" s="41"/>
-      <c r="EZ35" s="41"/>
-      <c r="FA35" s="41"/>
-      <c r="FB35" s="41"/>
-      <c r="FC35" s="41"/>
-      <c r="FD35" s="41"/>
-      <c r="FE35" s="41"/>
-    </row>
-    <row r="36" spans="1:161" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A36" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="B36" s="37"/>
-      <c r="C36" s="37"/>
-      <c r="D36" s="37"/>
-      <c r="E36" s="37"/>
-      <c r="F36" s="37"/>
-      <c r="G36" s="37"/>
-      <c r="H36" s="37"/>
-      <c r="I36" s="37"/>
-      <c r="J36" s="37"/>
-      <c r="K36" s="37"/>
-      <c r="L36" s="37"/>
-      <c r="M36" s="37"/>
-      <c r="N36" s="37"/>
-      <c r="O36" s="37"/>
-      <c r="P36" s="37"/>
-      <c r="Q36" s="37"/>
-      <c r="R36" s="37"/>
-      <c r="S36" s="37"/>
-      <c r="T36" s="37"/>
-      <c r="U36" s="37"/>
-      <c r="V36" s="37"/>
-      <c r="W36" s="37"/>
-      <c r="X36" s="37"/>
-      <c r="Y36" s="37"/>
-      <c r="Z36" s="37"/>
-      <c r="AA36" s="37"/>
-      <c r="AB36" s="37"/>
-      <c r="AC36" s="37"/>
-      <c r="AD36" s="37"/>
-      <c r="AE36" s="37"/>
-      <c r="AF36" s="37"/>
-      <c r="AG36" s="37"/>
-      <c r="AH36" s="37"/>
-      <c r="AI36" s="37"/>
-      <c r="AJ36" s="37"/>
-      <c r="AK36" s="37"/>
-      <c r="AL36" s="37"/>
-      <c r="AM36" s="37"/>
-      <c r="AN36" s="37"/>
-      <c r="AO36" s="37"/>
-      <c r="AP36" s="37"/>
-      <c r="AQ36" s="37"/>
-      <c r="AR36" s="37"/>
-      <c r="AS36" s="37"/>
-      <c r="AT36" s="37"/>
-      <c r="AU36" s="37"/>
-      <c r="AV36" s="37"/>
-      <c r="AW36" s="37"/>
-      <c r="AX36" s="37"/>
-      <c r="AY36" s="37"/>
-      <c r="AZ36" s="37"/>
-      <c r="BA36" s="37"/>
-      <c r="BB36" s="37"/>
-      <c r="BC36" s="37"/>
-      <c r="BD36" s="37"/>
-      <c r="BE36" s="37"/>
-      <c r="BF36" s="37"/>
-      <c r="BG36" s="37"/>
-      <c r="BH36" s="37"/>
-      <c r="BI36" s="37"/>
-      <c r="BJ36" s="37"/>
-      <c r="BK36" s="37"/>
-      <c r="BL36" s="37"/>
-      <c r="BM36" s="38"/>
-      <c r="BN36" s="39"/>
-      <c r="BO36" s="39"/>
-      <c r="BP36" s="39"/>
-      <c r="BQ36" s="39"/>
-      <c r="BR36" s="39"/>
-      <c r="BS36" s="39"/>
-      <c r="BT36" s="39"/>
-      <c r="BU36" s="39"/>
-      <c r="BV36" s="39"/>
-      <c r="BW36" s="39"/>
-      <c r="BX36" s="39"/>
-      <c r="BY36" s="39"/>
-      <c r="BZ36" s="39"/>
-      <c r="CA36" s="40"/>
-      <c r="CB36" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="CC36" s="39"/>
-      <c r="CD36" s="39"/>
-      <c r="CE36" s="39"/>
-      <c r="CF36" s="39"/>
-      <c r="CG36" s="39"/>
-      <c r="CH36" s="39"/>
-      <c r="CI36" s="39"/>
-      <c r="CJ36" s="39"/>
-      <c r="CK36" s="39"/>
-      <c r="CL36" s="39"/>
-      <c r="CM36" s="39"/>
-      <c r="CN36" s="39"/>
-      <c r="CO36" s="39"/>
-      <c r="CP36" s="39"/>
-      <c r="CQ36" s="39"/>
-      <c r="CR36" s="39"/>
-      <c r="CS36" s="39"/>
-      <c r="CT36" s="39"/>
-      <c r="CU36" s="40"/>
-      <c r="CV36" s="35"/>
-      <c r="CW36" s="35"/>
-      <c r="CX36" s="35"/>
-      <c r="CY36" s="35"/>
-      <c r="CZ36" s="35"/>
-      <c r="DA36" s="35"/>
-      <c r="DB36" s="35"/>
-      <c r="DC36" s="35"/>
-      <c r="DD36" s="35"/>
-      <c r="DE36" s="35"/>
-      <c r="DF36" s="35"/>
-      <c r="DG36" s="35"/>
-      <c r="DH36" s="35">
-        <v>54542</v>
-      </c>
-      <c r="DI36" s="35"/>
-      <c r="DJ36" s="35"/>
-      <c r="DK36" s="35"/>
-      <c r="DL36" s="35"/>
-      <c r="DM36" s="35"/>
-      <c r="DN36" s="35"/>
-      <c r="DO36" s="35"/>
-      <c r="DP36" s="35"/>
-      <c r="DQ36" s="35"/>
-      <c r="DR36" s="35"/>
-      <c r="DS36" s="35"/>
-      <c r="DT36" s="35"/>
-      <c r="DU36" s="35"/>
-      <c r="DV36" s="35"/>
-    </row>
-    <row r="37" spans="1:161" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:161" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="CD38" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:161" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AH39" s="28"/>
-      <c r="AI39" s="28"/>
-      <c r="AJ39" s="28"/>
-      <c r="AK39" s="28"/>
-      <c r="AL39" s="28"/>
-      <c r="AM39" s="28"/>
-      <c r="AN39" s="28"/>
-      <c r="AO39" s="28"/>
-      <c r="AP39" s="28"/>
-      <c r="AQ39" s="28"/>
-      <c r="AR39" s="28"/>
-      <c r="AS39" s="28"/>
-      <c r="AT39" s="28"/>
-      <c r="AU39" s="28"/>
-      <c r="AV39" s="28"/>
-      <c r="AW39" s="28"/>
-      <c r="AZ39" s="28"/>
-      <c r="BA39" s="28"/>
-      <c r="BB39" s="28"/>
-      <c r="BC39" s="28"/>
-      <c r="BD39" s="28"/>
-      <c r="BE39" s="28"/>
-      <c r="BF39" s="28"/>
-      <c r="BG39" s="28"/>
-      <c r="BH39" s="28"/>
-      <c r="BI39" s="28"/>
-      <c r="BJ39" s="28"/>
-      <c r="BK39" s="28"/>
-      <c r="BL39" s="28"/>
-      <c r="BM39" s="28"/>
-      <c r="BN39" s="28"/>
-      <c r="BO39" s="28"/>
-      <c r="BP39" s="28"/>
-      <c r="BQ39" s="28"/>
-      <c r="BR39" s="28"/>
-      <c r="BS39" s="28"/>
-      <c r="BT39" s="28"/>
-      <c r="BU39" s="28"/>
-      <c r="BV39" s="28"/>
-      <c r="BW39" s="28"/>
-      <c r="BX39" s="28"/>
-      <c r="BY39" s="28"/>
-      <c r="BZ39" s="28"/>
-      <c r="CA39" s="28"/>
-      <c r="CB39" s="28"/>
-      <c r="CD39" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="DK39" s="28"/>
-      <c r="DL39" s="28"/>
-      <c r="DM39" s="28"/>
-      <c r="DN39" s="28"/>
-      <c r="DO39" s="28"/>
-      <c r="DP39" s="28"/>
-      <c r="DQ39" s="28"/>
-      <c r="DR39" s="28"/>
-      <c r="DS39" s="28"/>
-      <c r="DT39" s="28"/>
-      <c r="DU39" s="28"/>
-      <c r="DV39" s="28"/>
-      <c r="DW39" s="28"/>
-      <c r="DX39" s="28"/>
-      <c r="DY39" s="28"/>
-      <c r="DZ39" s="28"/>
-      <c r="EC39" s="28"/>
-      <c r="ED39" s="28"/>
-      <c r="EE39" s="28"/>
-      <c r="EF39" s="28"/>
-      <c r="EG39" s="28"/>
-      <c r="EH39" s="28"/>
-      <c r="EI39" s="28"/>
-      <c r="EJ39" s="28"/>
-      <c r="EK39" s="28"/>
-      <c r="EL39" s="28"/>
-      <c r="EM39" s="28"/>
-      <c r="EN39" s="28"/>
-      <c r="EO39" s="28"/>
-      <c r="EP39" s="28"/>
-      <c r="EQ39" s="28"/>
-      <c r="ER39" s="28"/>
-      <c r="ES39" s="28"/>
-      <c r="ET39" s="28"/>
-      <c r="EU39" s="28"/>
-      <c r="EV39" s="28"/>
-      <c r="EW39" s="28"/>
-      <c r="EX39" s="28"/>
-      <c r="EY39" s="28"/>
-      <c r="EZ39" s="28"/>
-      <c r="FA39" s="28"/>
-      <c r="FB39" s="28"/>
-      <c r="FC39" s="28"/>
-      <c r="FD39" s="28"/>
-      <c r="FE39" s="28"/>
-    </row>
-    <row r="40" spans="1:161" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AH40" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="AI40" s="29"/>
-      <c r="AJ40" s="29"/>
-      <c r="AK40" s="29"/>
-      <c r="AL40" s="29"/>
-      <c r="AM40" s="29"/>
-      <c r="AN40" s="29"/>
-      <c r="AO40" s="29"/>
-      <c r="AP40" s="29"/>
-      <c r="AQ40" s="29"/>
-      <c r="AR40" s="29"/>
-      <c r="AS40" s="29"/>
-      <c r="AT40" s="29"/>
-      <c r="AU40" s="29"/>
-      <c r="AV40" s="29"/>
-      <c r="AW40" s="29"/>
-      <c r="AX40" s="6"/>
-      <c r="AY40" s="6"/>
-      <c r="AZ40" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="BA40" s="29"/>
-      <c r="BB40" s="29"/>
-      <c r="BC40" s="29"/>
-      <c r="BD40" s="29"/>
-      <c r="BE40" s="29"/>
-      <c r="BF40" s="29"/>
-      <c r="BG40" s="29"/>
-      <c r="BH40" s="29"/>
-      <c r="BI40" s="29"/>
-      <c r="BJ40" s="29"/>
-      <c r="BK40" s="29"/>
-      <c r="BL40" s="29"/>
-      <c r="BM40" s="29"/>
-      <c r="BN40" s="29"/>
-      <c r="BO40" s="29"/>
-      <c r="BP40" s="29"/>
-      <c r="BQ40" s="29"/>
-      <c r="BR40" s="29"/>
-      <c r="BS40" s="29"/>
-      <c r="BT40" s="29"/>
-      <c r="BU40" s="29"/>
-      <c r="BV40" s="29"/>
-      <c r="BW40" s="29"/>
-      <c r="BX40" s="29"/>
-      <c r="BY40" s="29"/>
-      <c r="BZ40" s="29"/>
-      <c r="CA40" s="29"/>
-      <c r="CB40" s="29"/>
-      <c r="DK40" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="DL40" s="29"/>
-      <c r="DM40" s="29"/>
-      <c r="DN40" s="29"/>
-      <c r="DO40" s="29"/>
-      <c r="DP40" s="29"/>
-      <c r="DQ40" s="29"/>
-      <c r="DR40" s="29"/>
-      <c r="DS40" s="29"/>
-      <c r="DT40" s="29"/>
-      <c r="DU40" s="29"/>
-      <c r="DV40" s="29"/>
-      <c r="DW40" s="29"/>
-      <c r="DX40" s="29"/>
-      <c r="DY40" s="29"/>
-      <c r="DZ40" s="29"/>
-      <c r="EA40" s="6"/>
-      <c r="EB40" s="6"/>
-      <c r="EC40" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="ED40" s="29"/>
-      <c r="EE40" s="29"/>
-      <c r="EF40" s="29"/>
-      <c r="EG40" s="29"/>
-      <c r="EH40" s="29"/>
-      <c r="EI40" s="29"/>
-      <c r="EJ40" s="29"/>
-      <c r="EK40" s="29"/>
-      <c r="EL40" s="29"/>
-      <c r="EM40" s="29"/>
-      <c r="EN40" s="29"/>
-      <c r="EO40" s="29"/>
-      <c r="EP40" s="29"/>
-      <c r="EQ40" s="29"/>
-      <c r="ER40" s="29"/>
-      <c r="ES40" s="29"/>
-      <c r="ET40" s="29"/>
-      <c r="EU40" s="29"/>
-      <c r="EV40" s="29"/>
-      <c r="EW40" s="29"/>
-      <c r="EX40" s="29"/>
-      <c r="EY40" s="29"/>
-      <c r="EZ40" s="29"/>
-      <c r="FA40" s="29"/>
-      <c r="FB40" s="29"/>
-      <c r="FC40" s="29"/>
-      <c r="FD40" s="29"/>
-      <c r="FE40" s="29"/>
-    </row>
-    <row r="41" spans="1:161" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="42" spans="1:161" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM42" s="28"/>
-      <c r="AN42" s="28"/>
-      <c r="AO42" s="28"/>
-      <c r="AP42" s="28"/>
-      <c r="AQ42" s="28"/>
-      <c r="AR42" s="28"/>
-      <c r="AS42" s="28"/>
-      <c r="AT42" s="28"/>
-      <c r="AU42" s="28"/>
-      <c r="AV42" s="28"/>
-      <c r="AW42" s="28"/>
-      <c r="AX42" s="28"/>
-      <c r="AY42" s="28"/>
-      <c r="AZ42" s="28"/>
-      <c r="BA42" s="28"/>
-      <c r="BB42" s="28"/>
-      <c r="BE42" s="28"/>
-      <c r="BF42" s="28"/>
-      <c r="BG42" s="28"/>
-      <c r="BH42" s="28"/>
-      <c r="BI42" s="28"/>
-      <c r="BJ42" s="28"/>
-      <c r="BK42" s="28"/>
-      <c r="BL42" s="28"/>
-      <c r="BM42" s="28"/>
-      <c r="BN42" s="28"/>
-      <c r="BO42" s="28"/>
-      <c r="BP42" s="28"/>
-      <c r="BQ42" s="28"/>
-      <c r="BR42" s="28"/>
-      <c r="BS42" s="28"/>
-      <c r="BT42" s="28"/>
-      <c r="BU42" s="28"/>
-      <c r="BV42" s="28"/>
-      <c r="BW42" s="28"/>
-      <c r="BX42" s="28"/>
-      <c r="BY42" s="28"/>
-      <c r="BZ42" s="28"/>
-      <c r="CA42" s="28"/>
-      <c r="CB42" s="28"/>
-      <c r="CC42" s="28"/>
-      <c r="CD42" s="28"/>
-      <c r="CE42" s="28"/>
-      <c r="CF42" s="28"/>
-      <c r="CG42" s="28"/>
-      <c r="CI42" s="27"/>
-      <c r="CJ42" s="27"/>
-      <c r="CK42" s="27"/>
-      <c r="CL42" s="27"/>
-      <c r="CM42" s="27"/>
-      <c r="CN42" s="27"/>
-      <c r="CO42" s="27"/>
-      <c r="CP42" s="27"/>
-      <c r="CQ42" s="27"/>
-      <c r="CR42" s="27"/>
-      <c r="CS42" s="27"/>
-      <c r="CT42" s="27"/>
-      <c r="CU42" s="27"/>
-      <c r="CV42" s="27"/>
-      <c r="CW42" s="27"/>
-      <c r="CX42" s="27"/>
-      <c r="CY42" s="27"/>
-      <c r="CZ42" s="27"/>
-      <c r="DA42" s="27"/>
-      <c r="DB42" s="27"/>
-      <c r="DC42" s="27"/>
-      <c r="DD42" s="27"/>
-      <c r="DE42" s="27"/>
-      <c r="DF42" s="27"/>
-      <c r="DG42" s="27"/>
-      <c r="DH42" s="27"/>
-      <c r="DI42" s="27"/>
-      <c r="DJ42" s="27"/>
-      <c r="DK42" s="27"/>
-      <c r="DL42" s="27"/>
-      <c r="DM42" s="27"/>
-      <c r="DN42" s="27"/>
-      <c r="DO42" s="27"/>
-      <c r="DP42" s="27"/>
-      <c r="DQ42" s="27"/>
-      <c r="DR42" s="27"/>
-      <c r="DS42" s="27"/>
-      <c r="DT42" s="27"/>
-      <c r="DU42" s="27"/>
-      <c r="DV42" s="27"/>
-      <c r="DW42" s="27"/>
-      <c r="DX42" s="27"/>
-      <c r="DY42" s="27"/>
-      <c r="DZ42" s="27"/>
-      <c r="EA42" s="27"/>
-      <c r="EB42" s="27"/>
-      <c r="EC42" s="27"/>
-      <c r="ED42" s="27"/>
-      <c r="EE42" s="27"/>
-      <c r="EF42" s="27"/>
-      <c r="EG42" s="27"/>
-      <c r="EH42" s="27"/>
-      <c r="EI42" s="27"/>
-      <c r="EJ42" s="27"/>
-      <c r="EK42" s="27"/>
-      <c r="EL42" s="27"/>
-      <c r="EM42" s="27"/>
-      <c r="EN42" s="27"/>
-      <c r="EO42" s="27"/>
-      <c r="EP42" s="27"/>
-      <c r="EQ42" s="27"/>
-      <c r="ER42" s="27"/>
-      <c r="ES42" s="27"/>
-      <c r="ET42" s="27"/>
-      <c r="EU42" s="27"/>
-      <c r="EV42" s="27"/>
-      <c r="EW42" s="27"/>
-      <c r="EX42" s="27"/>
-      <c r="EY42" s="27"/>
-      <c r="EZ42" s="27"/>
-      <c r="FA42" s="27"/>
-      <c r="FB42" s="27"/>
-      <c r="FC42" s="27"/>
-      <c r="FD42" s="27"/>
-      <c r="FE42" s="27"/>
-    </row>
-    <row r="43" spans="1:161" s="7" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AM43" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="AN43" s="29"/>
-      <c r="AO43" s="29"/>
-      <c r="AP43" s="29"/>
-      <c r="AQ43" s="29"/>
-      <c r="AR43" s="29"/>
-      <c r="AS43" s="29"/>
-      <c r="AT43" s="29"/>
-      <c r="AU43" s="29"/>
-      <c r="AV43" s="29"/>
-      <c r="AW43" s="29"/>
-      <c r="AX43" s="29"/>
-      <c r="AY43" s="29"/>
-      <c r="AZ43" s="29"/>
-      <c r="BA43" s="29"/>
-      <c r="BB43" s="29"/>
-      <c r="BC43" s="6"/>
-      <c r="BD43" s="6"/>
-      <c r="BE43" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="BF43" s="29"/>
-      <c r="BG43" s="29"/>
-      <c r="BH43" s="29"/>
-      <c r="BI43" s="29"/>
-      <c r="BJ43" s="29"/>
-      <c r="BK43" s="29"/>
-      <c r="BL43" s="29"/>
-      <c r="BM43" s="29"/>
-      <c r="BN43" s="29"/>
-      <c r="BO43" s="29"/>
-      <c r="BP43" s="29"/>
-      <c r="BQ43" s="29"/>
-      <c r="BR43" s="29"/>
-      <c r="BS43" s="29"/>
-      <c r="BT43" s="29"/>
-      <c r="BU43" s="29"/>
-      <c r="BV43" s="29"/>
-      <c r="BW43" s="29"/>
-      <c r="BX43" s="29"/>
-      <c r="BY43" s="29"/>
-      <c r="BZ43" s="29"/>
-      <c r="CA43" s="29"/>
-      <c r="CB43" s="29"/>
-      <c r="CC43" s="29"/>
-      <c r="CD43" s="29"/>
-      <c r="CE43" s="29"/>
-      <c r="CF43" s="29"/>
-      <c r="CG43" s="29"/>
-      <c r="CI43" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="CJ43" s="34"/>
-      <c r="CK43" s="34"/>
-      <c r="CL43" s="34"/>
-      <c r="CM43" s="34"/>
-      <c r="CN43" s="34"/>
-      <c r="CO43" s="34"/>
-      <c r="CP43" s="34"/>
-      <c r="CQ43" s="34"/>
-      <c r="CR43" s="34"/>
-      <c r="CS43" s="34"/>
-      <c r="CT43" s="34"/>
-      <c r="CU43" s="34"/>
-      <c r="CV43" s="34"/>
-      <c r="CW43" s="34"/>
-      <c r="CX43" s="34"/>
-      <c r="CY43" s="34"/>
-      <c r="CZ43" s="34"/>
-      <c r="DA43" s="34"/>
-      <c r="DB43" s="34"/>
-      <c r="DC43" s="34"/>
-      <c r="DD43" s="34"/>
-      <c r="DE43" s="34"/>
-      <c r="DF43" s="34"/>
-      <c r="DG43" s="34"/>
-      <c r="DH43" s="34"/>
-      <c r="DI43" s="34"/>
-      <c r="DJ43" s="34"/>
-      <c r="DK43" s="34"/>
-      <c r="DL43" s="34"/>
-      <c r="DM43" s="34"/>
-      <c r="DN43" s="34"/>
-      <c r="DO43" s="34"/>
-      <c r="DP43" s="34"/>
-      <c r="DQ43" s="34"/>
-      <c r="DR43" s="34"/>
-      <c r="DS43" s="34"/>
-      <c r="DT43" s="34"/>
-      <c r="DU43" s="34"/>
-      <c r="DV43" s="34"/>
-      <c r="DW43" s="34"/>
-      <c r="DX43" s="34"/>
-      <c r="DY43" s="34"/>
-      <c r="DZ43" s="34"/>
-      <c r="EA43" s="34"/>
-      <c r="EB43" s="34"/>
-      <c r="EC43" s="34"/>
-      <c r="ED43" s="34"/>
-      <c r="EE43" s="34"/>
-      <c r="EF43" s="34"/>
-      <c r="EG43" s="34"/>
-      <c r="EH43" s="34"/>
-      <c r="EI43" s="34"/>
-      <c r="EJ43" s="34"/>
-      <c r="EK43" s="34"/>
-      <c r="EL43" s="34"/>
-      <c r="EM43" s="34"/>
-      <c r="EN43" s="34"/>
-      <c r="EO43" s="34"/>
-      <c r="EP43" s="34"/>
-      <c r="EQ43" s="34"/>
-      <c r="ER43" s="34"/>
-      <c r="ES43" s="34"/>
-      <c r="ET43" s="34"/>
-      <c r="EU43" s="34"/>
-      <c r="EV43" s="34"/>
-      <c r="EW43" s="34"/>
-      <c r="EX43" s="34"/>
-      <c r="EY43" s="34"/>
-      <c r="EZ43" s="34"/>
-      <c r="FA43" s="34"/>
-      <c r="FB43" s="34"/>
-      <c r="FC43" s="34"/>
-      <c r="FD43" s="34"/>
-      <c r="FE43" s="34"/>
-    </row>
-    <row r="44" spans="1:161" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:161" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="224">
-    <mergeCell ref="DH34:DV34"/>
-    <mergeCell ref="DW34:EF34"/>
-    <mergeCell ref="EG34:ES34"/>
-    <mergeCell ref="ET34:FE34"/>
-    <mergeCell ref="BB34:BL34"/>
-    <mergeCell ref="BM34:CA34"/>
-    <mergeCell ref="CB34:CK34"/>
-    <mergeCell ref="CL34:CU34"/>
-    <mergeCell ref="CV34:DG34"/>
-    <mergeCell ref="A34:T34"/>
-    <mergeCell ref="U34:AB34"/>
-    <mergeCell ref="AC34:AH34"/>
-    <mergeCell ref="AI34:AS34"/>
-    <mergeCell ref="AT34:BA34"/>
-    <mergeCell ref="EG32:ES32"/>
-    <mergeCell ref="ET32:FE32"/>
-    <mergeCell ref="A33:T33"/>
-    <mergeCell ref="U33:AB33"/>
-    <mergeCell ref="AC33:AH33"/>
-    <mergeCell ref="AI33:AS33"/>
-    <mergeCell ref="AT33:BA33"/>
-    <mergeCell ref="BB33:BL33"/>
-    <mergeCell ref="BM33:CA33"/>
-    <mergeCell ref="CB33:CK33"/>
-    <mergeCell ref="CL33:CU33"/>
-    <mergeCell ref="CV33:DG33"/>
-    <mergeCell ref="DH33:DV33"/>
-    <mergeCell ref="DW33:EF33"/>
-    <mergeCell ref="EG33:ES33"/>
-    <mergeCell ref="ET33:FE33"/>
-    <mergeCell ref="DH31:DV31"/>
-    <mergeCell ref="DW31:EF31"/>
-    <mergeCell ref="EG31:ES31"/>
-    <mergeCell ref="ET31:FE31"/>
-    <mergeCell ref="A32:T32"/>
-    <mergeCell ref="U32:AB32"/>
-    <mergeCell ref="AC32:AH32"/>
-    <mergeCell ref="AI32:AS32"/>
-    <mergeCell ref="AT32:BA32"/>
-    <mergeCell ref="BB32:BL32"/>
-    <mergeCell ref="BM32:CA32"/>
-    <mergeCell ref="CB32:CK32"/>
-    <mergeCell ref="CL32:CU32"/>
-    <mergeCell ref="CV32:DG32"/>
-    <mergeCell ref="DH32:DV32"/>
-    <mergeCell ref="DW32:EF32"/>
-    <mergeCell ref="BB31:BL31"/>
-    <mergeCell ref="BM31:CA31"/>
-    <mergeCell ref="CB31:CK31"/>
-    <mergeCell ref="CL31:CU31"/>
-    <mergeCell ref="CV31:DG31"/>
-    <mergeCell ref="A31:T31"/>
-    <mergeCell ref="U31:AB31"/>
-    <mergeCell ref="AC31:AH31"/>
-    <mergeCell ref="AI31:AS31"/>
-    <mergeCell ref="AT31:BA31"/>
-    <mergeCell ref="EG29:ES29"/>
-    <mergeCell ref="ET29:FE29"/>
-    <mergeCell ref="A30:T30"/>
-    <mergeCell ref="U30:AB30"/>
-    <mergeCell ref="AC30:AH30"/>
-    <mergeCell ref="AI30:AS30"/>
-    <mergeCell ref="AT30:BA30"/>
-    <mergeCell ref="BB30:BL30"/>
-    <mergeCell ref="BM30:CA30"/>
-    <mergeCell ref="CB30:CK30"/>
-    <mergeCell ref="CL30:CU30"/>
-    <mergeCell ref="CV30:DG30"/>
-    <mergeCell ref="DH30:DV30"/>
-    <mergeCell ref="DW30:EF30"/>
-    <mergeCell ref="EG30:ES30"/>
-    <mergeCell ref="ET30:FE30"/>
-    <mergeCell ref="DH28:DV28"/>
-    <mergeCell ref="DW28:EF28"/>
-    <mergeCell ref="EG28:ES28"/>
-    <mergeCell ref="ET28:FE28"/>
-    <mergeCell ref="A29:T29"/>
-    <mergeCell ref="U29:AB29"/>
-    <mergeCell ref="AC29:AH29"/>
-    <mergeCell ref="AI29:AS29"/>
-    <mergeCell ref="AT29:BA29"/>
-    <mergeCell ref="BB29:BL29"/>
-    <mergeCell ref="BM29:CA29"/>
-    <mergeCell ref="CB29:CK29"/>
-    <mergeCell ref="CL29:CU29"/>
-    <mergeCell ref="CV29:DG29"/>
-    <mergeCell ref="DH29:DV29"/>
-    <mergeCell ref="DW29:EF29"/>
-    <mergeCell ref="BB28:BL28"/>
-    <mergeCell ref="BM28:CA28"/>
-    <mergeCell ref="CB28:CK28"/>
-    <mergeCell ref="CL28:CU28"/>
-    <mergeCell ref="CV28:DG28"/>
-    <mergeCell ref="A28:T28"/>
-    <mergeCell ref="U28:AB28"/>
-    <mergeCell ref="AC28:AH28"/>
-    <mergeCell ref="AI28:AS28"/>
-    <mergeCell ref="AT28:BA28"/>
+  <mergeCells count="112">
     <mergeCell ref="EG26:ES26"/>
     <mergeCell ref="ET26:FE26"/>
-    <mergeCell ref="A27:T27"/>
-    <mergeCell ref="U27:AB27"/>
-    <mergeCell ref="AC27:AH27"/>
-    <mergeCell ref="AI27:AS27"/>
-    <mergeCell ref="AT27:BA27"/>
-    <mergeCell ref="BB27:BL27"/>
-    <mergeCell ref="BM27:CA27"/>
-    <mergeCell ref="CB27:CK27"/>
-    <mergeCell ref="CL27:CU27"/>
-    <mergeCell ref="CV27:DG27"/>
-    <mergeCell ref="DH27:DV27"/>
-    <mergeCell ref="DW27:EF27"/>
-    <mergeCell ref="EG27:ES27"/>
-    <mergeCell ref="ET27:FE27"/>
     <mergeCell ref="DH25:DV25"/>
     <mergeCell ref="DW25:EF25"/>
     <mergeCell ref="EG25:ES25"/>
@@ -6617,25 +5097,25 @@
     <mergeCell ref="AC25:AH25"/>
     <mergeCell ref="AI25:AS25"/>
     <mergeCell ref="AT25:BA25"/>
-    <mergeCell ref="ET35:FE35"/>
-    <mergeCell ref="A35:T35"/>
-    <mergeCell ref="U35:AB35"/>
-    <mergeCell ref="AC35:AH35"/>
-    <mergeCell ref="AI35:AS35"/>
-    <mergeCell ref="CL35:CU35"/>
-    <mergeCell ref="CV35:DG35"/>
-    <mergeCell ref="DH35:DV35"/>
-    <mergeCell ref="DW35:EF35"/>
-    <mergeCell ref="EG35:ES35"/>
-    <mergeCell ref="AT35:BA35"/>
-    <mergeCell ref="BB35:BL35"/>
-    <mergeCell ref="BM35:CA35"/>
-    <mergeCell ref="CB35:CK35"/>
-    <mergeCell ref="DH36:DV36"/>
-    <mergeCell ref="A36:BL36"/>
-    <mergeCell ref="BM36:CA36"/>
-    <mergeCell ref="CB36:CU36"/>
-    <mergeCell ref="CV36:DG36"/>
+    <mergeCell ref="ET27:FE27"/>
+    <mergeCell ref="A27:T27"/>
+    <mergeCell ref="U27:AB27"/>
+    <mergeCell ref="AC27:AH27"/>
+    <mergeCell ref="AI27:AS27"/>
+    <mergeCell ref="CL27:CU27"/>
+    <mergeCell ref="CV27:DG27"/>
+    <mergeCell ref="DH27:DV27"/>
+    <mergeCell ref="DW27:EF27"/>
+    <mergeCell ref="EG27:ES27"/>
+    <mergeCell ref="AT27:BA27"/>
+    <mergeCell ref="BB27:BL27"/>
+    <mergeCell ref="BM27:CA27"/>
+    <mergeCell ref="CB27:CK27"/>
+    <mergeCell ref="DH28:DV28"/>
+    <mergeCell ref="A28:BL28"/>
+    <mergeCell ref="BM28:CA28"/>
+    <mergeCell ref="CB28:CU28"/>
+    <mergeCell ref="CV28:DG28"/>
     <mergeCell ref="A22:T23"/>
     <mergeCell ref="U22:AB23"/>
     <mergeCell ref="AC22:AS22"/>
@@ -6651,23 +5131,23 @@
     <mergeCell ref="BB24:BL24"/>
     <mergeCell ref="BM24:CA24"/>
     <mergeCell ref="CB24:CK24"/>
-    <mergeCell ref="CI43:FE43"/>
-    <mergeCell ref="AM42:BB42"/>
-    <mergeCell ref="BE42:CG42"/>
-    <mergeCell ref="AM43:BB43"/>
-    <mergeCell ref="BE43:CG43"/>
-    <mergeCell ref="CI42:FE42"/>
-    <mergeCell ref="AZ39:CB39"/>
-    <mergeCell ref="AZ40:CB40"/>
+    <mergeCell ref="CI35:FE35"/>
+    <mergeCell ref="AM34:BB34"/>
+    <mergeCell ref="BE34:CG34"/>
+    <mergeCell ref="AM35:BB35"/>
+    <mergeCell ref="BE35:CG35"/>
+    <mergeCell ref="CI34:FE34"/>
+    <mergeCell ref="AZ31:CB31"/>
+    <mergeCell ref="AZ32:CB32"/>
     <mergeCell ref="ET22:FE23"/>
     <mergeCell ref="A20:CO20"/>
     <mergeCell ref="CP20:EZ20"/>
-    <mergeCell ref="DK39:DZ39"/>
-    <mergeCell ref="EC39:FE39"/>
-    <mergeCell ref="DK40:DZ40"/>
-    <mergeCell ref="EC40:FE40"/>
-    <mergeCell ref="AH39:AW39"/>
-    <mergeCell ref="AH40:AW40"/>
+    <mergeCell ref="DK31:DZ31"/>
+    <mergeCell ref="EC31:FE31"/>
+    <mergeCell ref="DK32:DZ32"/>
+    <mergeCell ref="EC32:FE32"/>
+    <mergeCell ref="AH31:AW31"/>
+    <mergeCell ref="AH32:AW32"/>
     <mergeCell ref="DW23:EF23"/>
     <mergeCell ref="EG23:ES23"/>
     <mergeCell ref="BB22:BL23"/>

</xml_diff>

<commit_message>
Add FileHandler class to control loading, saving and closing excel files
</commit_message>
<xml_diff>
--- a/winApp/bin/Debug/Output.xlsx
+++ b/winApp/bin/Debug/Output.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\WinApp\winApp\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\WinApp\winApp\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5932C49D-CACB-4D29-92EA-B0C086FC30BB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9009C0C9-D690-4C3D-BF94-3737791102BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6705" yWindow="1320" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28695" yWindow="3345" windowWidth="23685" windowHeight="11340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="стр.1" sheetId="1" r:id="rId1"/>
@@ -3991,7 +3991,7 @@
       <c r="AR25" s="27"/>
       <c r="AS25" s="28"/>
       <c r="AT25" s="29">
-        <v>782</v>
+        <v>458</v>
       </c>
       <c r="AU25" s="30"/>
       <c r="AV25" s="30"/>
@@ -4001,7 +4001,7 @@
       <c r="AZ25" s="30"/>
       <c r="BA25" s="31"/>
       <c r="BB25" s="29">
-        <v>786.16</v>
+        <v>757.74</v>
       </c>
       <c r="BC25" s="30"/>
       <c r="BD25" s="30"/>
@@ -4061,7 +4061,7 @@
       <c r="DF25" s="30"/>
       <c r="DG25" s="31"/>
       <c r="DH25" s="29">
-        <v>614777.12</v>
+        <v>347044.92</v>
       </c>
       <c r="DI25" s="30"/>
       <c r="DJ25" s="30"/>
@@ -4164,7 +4164,7 @@
       <c r="AR26" s="27"/>
       <c r="AS26" s="28"/>
       <c r="AT26" s="29">
-        <v>828</v>
+        <v>519</v>
       </c>
       <c r="AU26" s="30"/>
       <c r="AV26" s="30"/>
@@ -4174,7 +4174,7 @@
       <c r="AZ26" s="30"/>
       <c r="BA26" s="31"/>
       <c r="BB26" s="29">
-        <v>648.21</v>
+        <v>654.08000000000004</v>
       </c>
       <c r="BC26" s="30"/>
       <c r="BD26" s="30"/>
@@ -4234,7 +4234,7 @@
       <c r="DF26" s="30"/>
       <c r="DG26" s="31"/>
       <c r="DH26" s="29">
-        <v>536717.88</v>
+        <v>339467.52000000002</v>
       </c>
       <c r="DI26" s="30"/>
       <c r="DJ26" s="30"/>
@@ -4337,7 +4337,7 @@
       <c r="AR27" s="27"/>
       <c r="AS27" s="28"/>
       <c r="AT27" s="29">
-        <v>1340</v>
+        <v>5418</v>
       </c>
       <c r="AU27" s="30"/>
       <c r="AV27" s="30"/>
@@ -4347,7 +4347,7 @@
       <c r="AZ27" s="30"/>
       <c r="BA27" s="31"/>
       <c r="BB27" s="29">
-        <v>2758.95</v>
+        <v>2670.42</v>
       </c>
       <c r="BC27" s="30"/>
       <c r="BD27" s="30"/>
@@ -4407,7 +4407,7 @@
       <c r="DF27" s="30"/>
       <c r="DG27" s="31"/>
       <c r="DH27" s="29">
-        <v>3696992.9999999995</v>
+        <v>14468335.560000001</v>
       </c>
       <c r="DI27" s="30"/>
       <c r="DJ27" s="30"/>
@@ -4739,7 +4739,7 @@
       <c r="DF29" s="51"/>
       <c r="DG29" s="51"/>
       <c r="DH29" s="51">
-        <v>4848488</v>
+        <v>15154848</v>
       </c>
       <c r="DI29" s="51"/>
       <c r="DJ29" s="51"/>

</xml_diff>

<commit_message>
Complete process killer to Excel processes
</commit_message>
<xml_diff>
--- a/winApp/bin/Debug/Output.xlsx
+++ b/winApp/bin/Debug/Output.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\WinApp\winApp\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\WinApp\winApp\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9009C0C9-D690-4C3D-BF94-3737791102BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{00524F92-C46D-41A3-B07F-060BB2B18493}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="3345" windowWidth="23685" windowHeight="11340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="стр.1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">стр.1!$A$1:$FE$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">стр.1!$A$1:$FE$45</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="73">
   <si>
     <t>Единица
 измерения</t>
@@ -213,16 +213,43 @@
     <t xml:space="preserve">, </t>
   </si>
   <si>
-    <t>Песка</t>
-  </si>
-  <si>
-    <t>м3</t>
-  </si>
-  <si>
-    <t>Щебня</t>
-  </si>
-  <si>
-    <t>Бетона</t>
+    <t xml:space="preserve">Труба канализационная наружная d=160х2000 мм </t>
+  </si>
+  <si>
+    <t>шт</t>
+  </si>
+  <si>
+    <t>Труба гофрированная 400мм с раструбом SN8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Труба гофрированная 300 мм с раструбом SN8 </t>
+  </si>
+  <si>
+    <t>Труба ПП Прагма OD 160 гофрированная (6м)</t>
+  </si>
+  <si>
+    <t>Муфта Корсис ID 200</t>
+  </si>
+  <si>
+    <t>Муфта для гофрированной трубы Электрокор</t>
+  </si>
+  <si>
+    <t>Муфта электросварная 50 мм</t>
+  </si>
+  <si>
+    <t>Соединительная муфта ДРК 100 мм Универсальная</t>
+  </si>
+  <si>
+    <t>Фланцевое соединение компрессионное 75x2 1/2“</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Седелка компрессионная </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Изоляция для труб </t>
+  </si>
+  <si>
+    <t>М</t>
   </si>
 </sst>
 </file>
@@ -846,7 +873,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:FE37"/>
+  <dimension ref="A1:FE45"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <selection activeCell="CJ30" sqref="CJ30"/>
@@ -3940,7 +3967,7 @@
       <c r="FD24" s="59"/>
       <c r="FE24" s="59"/>
     </row>
-    <row r="25" spans="1:161" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:161" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="18" t="s">
         <v>60</v>
       </c>
@@ -3991,7 +4018,7 @@
       <c r="AR25" s="27"/>
       <c r="AS25" s="28"/>
       <c r="AT25" s="29">
-        <v>458</v>
+        <v>1</v>
       </c>
       <c r="AU25" s="30"/>
       <c r="AV25" s="30"/>
@@ -4001,7 +4028,7 @@
       <c r="AZ25" s="30"/>
       <c r="BA25" s="31"/>
       <c r="BB25" s="29">
-        <v>757.74</v>
+        <v>1824.4</v>
       </c>
       <c r="BC25" s="30"/>
       <c r="BD25" s="30"/>
@@ -4061,7 +4088,7 @@
       <c r="DF25" s="30"/>
       <c r="DG25" s="31"/>
       <c r="DH25" s="29">
-        <v>347044.92</v>
+        <v>1824.4</v>
       </c>
       <c r="DI25" s="30"/>
       <c r="DJ25" s="30"/>
@@ -4113,7 +4140,7 @@
       <c r="FD25" s="25"/>
       <c r="FE25" s="61"/>
     </row>
-    <row r="26" spans="1:161" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:161" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="18" t="s">
         <v>62</v>
       </c>
@@ -4164,7 +4191,7 @@
       <c r="AR26" s="27"/>
       <c r="AS26" s="28"/>
       <c r="AT26" s="29">
-        <v>519</v>
+        <v>1</v>
       </c>
       <c r="AU26" s="30"/>
       <c r="AV26" s="30"/>
@@ -4174,7 +4201,7 @@
       <c r="AZ26" s="30"/>
       <c r="BA26" s="31"/>
       <c r="BB26" s="29">
-        <v>654.08000000000004</v>
+        <v>1824.4</v>
       </c>
       <c r="BC26" s="30"/>
       <c r="BD26" s="30"/>
@@ -4234,7 +4261,7 @@
       <c r="DF26" s="30"/>
       <c r="DG26" s="31"/>
       <c r="DH26" s="29">
-        <v>339467.52000000002</v>
+        <v>1824.4</v>
       </c>
       <c r="DI26" s="30"/>
       <c r="DJ26" s="30"/>
@@ -4286,7 +4313,7 @@
       <c r="FD26" s="25"/>
       <c r="FE26" s="61"/>
     </row>
-    <row r="27" spans="1:161" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:161" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="18" t="s">
         <v>63</v>
       </c>
@@ -4337,7 +4364,7 @@
       <c r="AR27" s="27"/>
       <c r="AS27" s="28"/>
       <c r="AT27" s="29">
-        <v>5418</v>
+        <v>1</v>
       </c>
       <c r="AU27" s="30"/>
       <c r="AV27" s="30"/>
@@ -4347,7 +4374,7 @@
       <c r="AZ27" s="30"/>
       <c r="BA27" s="31"/>
       <c r="BB27" s="29">
-        <v>2670.42</v>
+        <v>1824.4</v>
       </c>
       <c r="BC27" s="30"/>
       <c r="BD27" s="30"/>
@@ -4407,7 +4434,7 @@
       <c r="DF27" s="30"/>
       <c r="DG27" s="31"/>
       <c r="DH27" s="29">
-        <v>14468335.560000001</v>
+        <v>1824.4</v>
       </c>
       <c r="DI27" s="30"/>
       <c r="DJ27" s="30"/>
@@ -4459,8 +4486,10 @@
       <c r="FD27" s="25"/>
       <c r="FE27" s="61"/>
     </row>
-    <row r="28" spans="1:161" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A28" s="18"/>
+    <row r="28" spans="1:161" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="18" t="s">
+        <v>64</v>
+      </c>
       <c r="B28" s="19"/>
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
@@ -4493,8 +4522,10 @@
       <c r="AE28" s="25"/>
       <c r="AF28" s="25"/>
       <c r="AG28" s="25"/>
-      <c r="AH28" s="25"/>
-      <c r="AI28" s="26"/>
+      <c r="AH28" s="61"/>
+      <c r="AI28" s="26" t="s">
+        <v>61</v>
+      </c>
       <c r="AJ28" s="27"/>
       <c r="AK28" s="27"/>
       <c r="AL28" s="27"/>
@@ -4505,7 +4536,9 @@
       <c r="AQ28" s="27"/>
       <c r="AR28" s="27"/>
       <c r="AS28" s="28"/>
-      <c r="AT28" s="29"/>
+      <c r="AT28" s="29">
+        <v>1</v>
+      </c>
       <c r="AU28" s="30"/>
       <c r="AV28" s="30"/>
       <c r="AW28" s="30"/>
@@ -4513,7 +4546,9 @@
       <c r="AY28" s="30"/>
       <c r="AZ28" s="30"/>
       <c r="BA28" s="31"/>
-      <c r="BB28" s="29"/>
+      <c r="BB28" s="29">
+        <v>1824.4</v>
+      </c>
       <c r="BC28" s="30"/>
       <c r="BD28" s="30"/>
       <c r="BE28" s="30"/>
@@ -4571,7 +4606,9 @@
       <c r="DE28" s="30"/>
       <c r="DF28" s="30"/>
       <c r="DG28" s="31"/>
-      <c r="DH28" s="29"/>
+      <c r="DH28" s="29">
+        <v>1824.4</v>
+      </c>
       <c r="DI28" s="30"/>
       <c r="DJ28" s="30"/>
       <c r="DK28" s="30"/>
@@ -4595,7 +4632,7 @@
       <c r="EC28" s="25"/>
       <c r="ED28" s="25"/>
       <c r="EE28" s="25"/>
-      <c r="EF28" s="25"/>
+      <c r="EF28" s="61"/>
       <c r="EG28" s="32"/>
       <c r="EH28" s="33"/>
       <c r="EI28" s="33"/>
@@ -4609,86 +4646,92 @@
       <c r="EQ28" s="33"/>
       <c r="ER28" s="33"/>
       <c r="ES28" s="34"/>
-      <c r="ET28" s="17"/>
-      <c r="EU28" s="17"/>
-      <c r="EV28" s="17"/>
-      <c r="EW28" s="17"/>
-      <c r="EX28" s="17"/>
-      <c r="EY28" s="17"/>
-      <c r="EZ28" s="17"/>
-      <c r="FA28" s="17"/>
-      <c r="FB28" s="17"/>
-      <c r="FC28" s="17"/>
-      <c r="FD28" s="17"/>
-      <c r="FE28" s="17"/>
+      <c r="ET28" s="24"/>
+      <c r="EU28" s="25"/>
+      <c r="EV28" s="25"/>
+      <c r="EW28" s="25"/>
+      <c r="EX28" s="25"/>
+      <c r="EY28" s="25"/>
+      <c r="EZ28" s="25"/>
+      <c r="FA28" s="25"/>
+      <c r="FB28" s="25"/>
+      <c r="FC28" s="25"/>
+      <c r="FD28" s="25"/>
+      <c r="FE28" s="61"/>
     </row>
-    <row r="29" spans="1:161" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A29" s="52" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" s="53"/>
-      <c r="C29" s="53"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="53"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="53"/>
-      <c r="I29" s="53"/>
-      <c r="J29" s="53"/>
-      <c r="K29" s="53"/>
-      <c r="L29" s="53"/>
-      <c r="M29" s="53"/>
-      <c r="N29" s="53"/>
-      <c r="O29" s="53"/>
-      <c r="P29" s="53"/>
-      <c r="Q29" s="53"/>
-      <c r="R29" s="53"/>
-      <c r="S29" s="53"/>
-      <c r="T29" s="53"/>
-      <c r="U29" s="53"/>
-      <c r="V29" s="53"/>
-      <c r="W29" s="53"/>
-      <c r="X29" s="53"/>
-      <c r="Y29" s="53"/>
-      <c r="Z29" s="53"/>
-      <c r="AA29" s="53"/>
-      <c r="AB29" s="53"/>
-      <c r="AC29" s="53"/>
-      <c r="AD29" s="53"/>
-      <c r="AE29" s="53"/>
-      <c r="AF29" s="53"/>
-      <c r="AG29" s="53"/>
-      <c r="AH29" s="53"/>
-      <c r="AI29" s="53"/>
-      <c r="AJ29" s="53"/>
-      <c r="AK29" s="53"/>
-      <c r="AL29" s="53"/>
-      <c r="AM29" s="53"/>
-      <c r="AN29" s="53"/>
-      <c r="AO29" s="53"/>
-      <c r="AP29" s="53"/>
-      <c r="AQ29" s="53"/>
-      <c r="AR29" s="53"/>
-      <c r="AS29" s="53"/>
-      <c r="AT29" s="53"/>
-      <c r="AU29" s="53"/>
-      <c r="AV29" s="53"/>
-      <c r="AW29" s="53"/>
-      <c r="AX29" s="53"/>
-      <c r="AY29" s="53"/>
-      <c r="AZ29" s="53"/>
-      <c r="BA29" s="53"/>
-      <c r="BB29" s="53"/>
-      <c r="BC29" s="53"/>
-      <c r="BD29" s="53"/>
-      <c r="BE29" s="53"/>
-      <c r="BF29" s="53"/>
-      <c r="BG29" s="53"/>
-      <c r="BH29" s="53"/>
-      <c r="BI29" s="53"/>
-      <c r="BJ29" s="53"/>
-      <c r="BK29" s="53"/>
-      <c r="BL29" s="53"/>
+    <row r="29" spans="1:161" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="19"/>
+      <c r="Q29" s="19"/>
+      <c r="R29" s="19"/>
+      <c r="S29" s="19"/>
+      <c r="T29" s="20"/>
+      <c r="U29" s="21"/>
+      <c r="V29" s="22"/>
+      <c r="W29" s="22"/>
+      <c r="X29" s="22"/>
+      <c r="Y29" s="22"/>
+      <c r="Z29" s="22"/>
+      <c r="AA29" s="22"/>
+      <c r="AB29" s="23"/>
+      <c r="AC29" s="24"/>
+      <c r="AD29" s="25"/>
+      <c r="AE29" s="25"/>
+      <c r="AF29" s="25"/>
+      <c r="AG29" s="25"/>
+      <c r="AH29" s="61"/>
+      <c r="AI29" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ29" s="27"/>
+      <c r="AK29" s="27"/>
+      <c r="AL29" s="27"/>
+      <c r="AM29" s="27"/>
+      <c r="AN29" s="27"/>
+      <c r="AO29" s="27"/>
+      <c r="AP29" s="27"/>
+      <c r="AQ29" s="27"/>
+      <c r="AR29" s="27"/>
+      <c r="AS29" s="28"/>
+      <c r="AT29" s="29">
+        <v>2</v>
+      </c>
+      <c r="AU29" s="30"/>
+      <c r="AV29" s="30"/>
+      <c r="AW29" s="30"/>
+      <c r="AX29" s="30"/>
+      <c r="AY29" s="30"/>
+      <c r="AZ29" s="30"/>
+      <c r="BA29" s="31"/>
+      <c r="BB29" s="29">
+        <v>912.2</v>
+      </c>
+      <c r="BC29" s="30"/>
+      <c r="BD29" s="30"/>
+      <c r="BE29" s="30"/>
+      <c r="BF29" s="30"/>
+      <c r="BG29" s="30"/>
+      <c r="BH29" s="30"/>
+      <c r="BI29" s="30"/>
+      <c r="BJ29" s="30"/>
+      <c r="BK29" s="30"/>
+      <c r="BL29" s="31"/>
       <c r="BM29" s="29"/>
       <c r="BN29" s="30"/>
       <c r="BO29" s="30"/>
@@ -4704,9 +4747,7 @@
       <c r="BY29" s="30"/>
       <c r="BZ29" s="30"/>
       <c r="CA29" s="31"/>
-      <c r="CB29" s="29" t="s">
-        <v>23</v>
-      </c>
+      <c r="CB29" s="29"/>
       <c r="CC29" s="30"/>
       <c r="CD29" s="30"/>
       <c r="CE29" s="30"/>
@@ -4715,8 +4756,8 @@
       <c r="CH29" s="30"/>
       <c r="CI29" s="30"/>
       <c r="CJ29" s="30"/>
-      <c r="CK29" s="30"/>
-      <c r="CL29" s="30"/>
+      <c r="CK29" s="31"/>
+      <c r="CL29" s="29"/>
       <c r="CM29" s="30"/>
       <c r="CN29" s="30"/>
       <c r="CO29" s="30"/>
@@ -4726,514 +4767,1996 @@
       <c r="CS29" s="30"/>
       <c r="CT29" s="30"/>
       <c r="CU29" s="31"/>
-      <c r="CV29" s="51"/>
-      <c r="CW29" s="51"/>
-      <c r="CX29" s="51"/>
-      <c r="CY29" s="51"/>
-      <c r="CZ29" s="51"/>
-      <c r="DA29" s="51"/>
-      <c r="DB29" s="51"/>
-      <c r="DC29" s="51"/>
-      <c r="DD29" s="51"/>
-      <c r="DE29" s="51"/>
-      <c r="DF29" s="51"/>
-      <c r="DG29" s="51"/>
-      <c r="DH29" s="51">
-        <v>15154848</v>
-      </c>
-      <c r="DI29" s="51"/>
-      <c r="DJ29" s="51"/>
-      <c r="DK29" s="51"/>
-      <c r="DL29" s="51"/>
-      <c r="DM29" s="51"/>
-      <c r="DN29" s="51"/>
-      <c r="DO29" s="51"/>
-      <c r="DP29" s="51"/>
-      <c r="DQ29" s="51"/>
-      <c r="DR29" s="51"/>
-      <c r="DS29" s="51"/>
-      <c r="DT29" s="51"/>
-      <c r="DU29" s="51"/>
-      <c r="DV29" s="51"/>
+      <c r="CV29" s="29"/>
+      <c r="CW29" s="30"/>
+      <c r="CX29" s="30"/>
+      <c r="CY29" s="30"/>
+      <c r="CZ29" s="30"/>
+      <c r="DA29" s="30"/>
+      <c r="DB29" s="30"/>
+      <c r="DC29" s="30"/>
+      <c r="DD29" s="30"/>
+      <c r="DE29" s="30"/>
+      <c r="DF29" s="30"/>
+      <c r="DG29" s="31"/>
+      <c r="DH29" s="29">
+        <v>1824.4</v>
+      </c>
+      <c r="DI29" s="30"/>
+      <c r="DJ29" s="30"/>
+      <c r="DK29" s="30"/>
+      <c r="DL29" s="30"/>
+      <c r="DM29" s="30"/>
+      <c r="DN29" s="30"/>
+      <c r="DO29" s="30"/>
+      <c r="DP29" s="30"/>
+      <c r="DQ29" s="30"/>
+      <c r="DR29" s="30"/>
+      <c r="DS29" s="30"/>
+      <c r="DT29" s="30"/>
+      <c r="DU29" s="30"/>
+      <c r="DV29" s="31"/>
+      <c r="DW29" s="24"/>
+      <c r="DX29" s="25"/>
+      <c r="DY29" s="25"/>
+      <c r="DZ29" s="25"/>
+      <c r="EA29" s="25"/>
+      <c r="EB29" s="25"/>
+      <c r="EC29" s="25"/>
+      <c r="ED29" s="25"/>
+      <c r="EE29" s="25"/>
+      <c r="EF29" s="61"/>
+      <c r="EG29" s="32"/>
+      <c r="EH29" s="33"/>
+      <c r="EI29" s="33"/>
+      <c r="EJ29" s="33"/>
+      <c r="EK29" s="33"/>
+      <c r="EL29" s="33"/>
+      <c r="EM29" s="33"/>
+      <c r="EN29" s="33"/>
+      <c r="EO29" s="33"/>
+      <c r="EP29" s="33"/>
+      <c r="EQ29" s="33"/>
+      <c r="ER29" s="33"/>
+      <c r="ES29" s="34"/>
+      <c r="ET29" s="24"/>
+      <c r="EU29" s="25"/>
+      <c r="EV29" s="25"/>
+      <c r="EW29" s="25"/>
+      <c r="EX29" s="25"/>
+      <c r="EY29" s="25"/>
+      <c r="EZ29" s="25"/>
+      <c r="FA29" s="25"/>
+      <c r="FB29" s="25"/>
+      <c r="FC29" s="25"/>
+      <c r="FD29" s="25"/>
+      <c r="FE29" s="61"/>
     </row>
-    <row r="30" spans="1:161" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:161" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+    <row r="30" spans="1:161" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="19"/>
+      <c r="Q30" s="19"/>
+      <c r="R30" s="19"/>
+      <c r="S30" s="19"/>
+      <c r="T30" s="20"/>
+      <c r="U30" s="21"/>
+      <c r="V30" s="22"/>
+      <c r="W30" s="22"/>
+      <c r="X30" s="22"/>
+      <c r="Y30" s="22"/>
+      <c r="Z30" s="22"/>
+      <c r="AA30" s="22"/>
+      <c r="AB30" s="23"/>
+      <c r="AC30" s="24"/>
+      <c r="AD30" s="25"/>
+      <c r="AE30" s="25"/>
+      <c r="AF30" s="25"/>
+      <c r="AG30" s="25"/>
+      <c r="AH30" s="61"/>
+      <c r="AI30" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ30" s="27"/>
+      <c r="AK30" s="27"/>
+      <c r="AL30" s="27"/>
+      <c r="AM30" s="27"/>
+      <c r="AN30" s="27"/>
+      <c r="AO30" s="27"/>
+      <c r="AP30" s="27"/>
+      <c r="AQ30" s="27"/>
+      <c r="AR30" s="27"/>
+      <c r="AS30" s="28"/>
+      <c r="AT30" s="29">
+        <v>2</v>
+      </c>
+      <c r="AU30" s="30"/>
+      <c r="AV30" s="30"/>
+      <c r="AW30" s="30"/>
+      <c r="AX30" s="30"/>
+      <c r="AY30" s="30"/>
+      <c r="AZ30" s="30"/>
+      <c r="BA30" s="31"/>
+      <c r="BB30" s="29">
+        <v>912.2</v>
+      </c>
+      <c r="BC30" s="30"/>
+      <c r="BD30" s="30"/>
+      <c r="BE30" s="30"/>
+      <c r="BF30" s="30"/>
+      <c r="BG30" s="30"/>
+      <c r="BH30" s="30"/>
+      <c r="BI30" s="30"/>
+      <c r="BJ30" s="30"/>
+      <c r="BK30" s="30"/>
+      <c r="BL30" s="31"/>
+      <c r="BM30" s="29"/>
+      <c r="BN30" s="30"/>
+      <c r="BO30" s="30"/>
+      <c r="BP30" s="30"/>
+      <c r="BQ30" s="30"/>
+      <c r="BR30" s="30"/>
+      <c r="BS30" s="30"/>
+      <c r="BT30" s="30"/>
+      <c r="BU30" s="30"/>
+      <c r="BV30" s="30"/>
+      <c r="BW30" s="30"/>
+      <c r="BX30" s="30"/>
+      <c r="BY30" s="30"/>
+      <c r="BZ30" s="30"/>
+      <c r="CA30" s="31"/>
+      <c r="CB30" s="29"/>
+      <c r="CC30" s="30"/>
+      <c r="CD30" s="30"/>
+      <c r="CE30" s="30"/>
+      <c r="CF30" s="30"/>
+      <c r="CG30" s="30"/>
+      <c r="CH30" s="30"/>
+      <c r="CI30" s="30"/>
+      <c r="CJ30" s="30"/>
+      <c r="CK30" s="31"/>
+      <c r="CL30" s="29"/>
+      <c r="CM30" s="30"/>
+      <c r="CN30" s="30"/>
+      <c r="CO30" s="30"/>
+      <c r="CP30" s="30"/>
+      <c r="CQ30" s="30"/>
+      <c r="CR30" s="30"/>
+      <c r="CS30" s="30"/>
+      <c r="CT30" s="30"/>
+      <c r="CU30" s="31"/>
+      <c r="CV30" s="29"/>
+      <c r="CW30" s="30"/>
+      <c r="CX30" s="30"/>
+      <c r="CY30" s="30"/>
+      <c r="CZ30" s="30"/>
+      <c r="DA30" s="30"/>
+      <c r="DB30" s="30"/>
+      <c r="DC30" s="30"/>
+      <c r="DD30" s="30"/>
+      <c r="DE30" s="30"/>
+      <c r="DF30" s="30"/>
+      <c r="DG30" s="31"/>
+      <c r="DH30" s="29">
+        <v>1824.4</v>
+      </c>
+      <c r="DI30" s="30"/>
+      <c r="DJ30" s="30"/>
+      <c r="DK30" s="30"/>
+      <c r="DL30" s="30"/>
+      <c r="DM30" s="30"/>
+      <c r="DN30" s="30"/>
+      <c r="DO30" s="30"/>
+      <c r="DP30" s="30"/>
+      <c r="DQ30" s="30"/>
+      <c r="DR30" s="30"/>
+      <c r="DS30" s="30"/>
+      <c r="DT30" s="30"/>
+      <c r="DU30" s="30"/>
+      <c r="DV30" s="31"/>
+      <c r="DW30" s="24"/>
+      <c r="DX30" s="25"/>
+      <c r="DY30" s="25"/>
+      <c r="DZ30" s="25"/>
+      <c r="EA30" s="25"/>
+      <c r="EB30" s="25"/>
+      <c r="EC30" s="25"/>
+      <c r="ED30" s="25"/>
+      <c r="EE30" s="25"/>
+      <c r="EF30" s="61"/>
+      <c r="EG30" s="32"/>
+      <c r="EH30" s="33"/>
+      <c r="EI30" s="33"/>
+      <c r="EJ30" s="33"/>
+      <c r="EK30" s="33"/>
+      <c r="EL30" s="33"/>
+      <c r="EM30" s="33"/>
+      <c r="EN30" s="33"/>
+      <c r="EO30" s="33"/>
+      <c r="EP30" s="33"/>
+      <c r="EQ30" s="33"/>
+      <c r="ER30" s="33"/>
+      <c r="ES30" s="34"/>
+      <c r="ET30" s="24"/>
+      <c r="EU30" s="25"/>
+      <c r="EV30" s="25"/>
+      <c r="EW30" s="25"/>
+      <c r="EX30" s="25"/>
+      <c r="EY30" s="25"/>
+      <c r="EZ30" s="25"/>
+      <c r="FA30" s="25"/>
+      <c r="FB30" s="25"/>
+      <c r="FC30" s="25"/>
+      <c r="FD30" s="25"/>
+      <c r="FE30" s="61"/>
+    </row>
+    <row r="31" spans="1:161" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="19"/>
+      <c r="Q31" s="19"/>
+      <c r="R31" s="19"/>
+      <c r="S31" s="19"/>
+      <c r="T31" s="20"/>
+      <c r="U31" s="21"/>
+      <c r="V31" s="22"/>
+      <c r="W31" s="22"/>
+      <c r="X31" s="22"/>
+      <c r="Y31" s="22"/>
+      <c r="Z31" s="22"/>
+      <c r="AA31" s="22"/>
+      <c r="AB31" s="23"/>
+      <c r="AC31" s="24"/>
+      <c r="AD31" s="25"/>
+      <c r="AE31" s="25"/>
+      <c r="AF31" s="25"/>
+      <c r="AG31" s="25"/>
+      <c r="AH31" s="61"/>
+      <c r="AI31" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ31" s="27"/>
+      <c r="AK31" s="27"/>
+      <c r="AL31" s="27"/>
+      <c r="AM31" s="27"/>
+      <c r="AN31" s="27"/>
+      <c r="AO31" s="27"/>
+      <c r="AP31" s="27"/>
+      <c r="AQ31" s="27"/>
+      <c r="AR31" s="27"/>
+      <c r="AS31" s="28"/>
+      <c r="AT31" s="29">
+        <v>3</v>
+      </c>
+      <c r="AU31" s="30"/>
+      <c r="AV31" s="30"/>
+      <c r="AW31" s="30"/>
+      <c r="AX31" s="30"/>
+      <c r="AY31" s="30"/>
+      <c r="AZ31" s="30"/>
+      <c r="BA31" s="31"/>
+      <c r="BB31" s="29">
+        <v>592.92999999999995</v>
+      </c>
+      <c r="BC31" s="30"/>
+      <c r="BD31" s="30"/>
+      <c r="BE31" s="30"/>
+      <c r="BF31" s="30"/>
+      <c r="BG31" s="30"/>
+      <c r="BH31" s="30"/>
+      <c r="BI31" s="30"/>
+      <c r="BJ31" s="30"/>
+      <c r="BK31" s="30"/>
+      <c r="BL31" s="31"/>
+      <c r="BM31" s="29"/>
+      <c r="BN31" s="30"/>
+      <c r="BO31" s="30"/>
+      <c r="BP31" s="30"/>
+      <c r="BQ31" s="30"/>
+      <c r="BR31" s="30"/>
+      <c r="BS31" s="30"/>
+      <c r="BT31" s="30"/>
+      <c r="BU31" s="30"/>
+      <c r="BV31" s="30"/>
+      <c r="BW31" s="30"/>
+      <c r="BX31" s="30"/>
+      <c r="BY31" s="30"/>
+      <c r="BZ31" s="30"/>
+      <c r="CA31" s="31"/>
+      <c r="CB31" s="29"/>
+      <c r="CC31" s="30"/>
+      <c r="CD31" s="30"/>
+      <c r="CE31" s="30"/>
+      <c r="CF31" s="30"/>
+      <c r="CG31" s="30"/>
+      <c r="CH31" s="30"/>
+      <c r="CI31" s="30"/>
+      <c r="CJ31" s="30"/>
+      <c r="CK31" s="31"/>
+      <c r="CL31" s="29"/>
+      <c r="CM31" s="30"/>
+      <c r="CN31" s="30"/>
+      <c r="CO31" s="30"/>
+      <c r="CP31" s="30"/>
+      <c r="CQ31" s="30"/>
+      <c r="CR31" s="30"/>
+      <c r="CS31" s="30"/>
+      <c r="CT31" s="30"/>
+      <c r="CU31" s="31"/>
+      <c r="CV31" s="29"/>
+      <c r="CW31" s="30"/>
+      <c r="CX31" s="30"/>
+      <c r="CY31" s="30"/>
+      <c r="CZ31" s="30"/>
+      <c r="DA31" s="30"/>
+      <c r="DB31" s="30"/>
+      <c r="DC31" s="30"/>
+      <c r="DD31" s="30"/>
+      <c r="DE31" s="30"/>
+      <c r="DF31" s="30"/>
+      <c r="DG31" s="31"/>
+      <c r="DH31" s="29">
+        <v>1778.79</v>
+      </c>
+      <c r="DI31" s="30"/>
+      <c r="DJ31" s="30"/>
+      <c r="DK31" s="30"/>
+      <c r="DL31" s="30"/>
+      <c r="DM31" s="30"/>
+      <c r="DN31" s="30"/>
+      <c r="DO31" s="30"/>
+      <c r="DP31" s="30"/>
+      <c r="DQ31" s="30"/>
+      <c r="DR31" s="30"/>
+      <c r="DS31" s="30"/>
+      <c r="DT31" s="30"/>
+      <c r="DU31" s="30"/>
+      <c r="DV31" s="31"/>
+      <c r="DW31" s="24"/>
+      <c r="DX31" s="25"/>
+      <c r="DY31" s="25"/>
+      <c r="DZ31" s="25"/>
+      <c r="EA31" s="25"/>
+      <c r="EB31" s="25"/>
+      <c r="EC31" s="25"/>
+      <c r="ED31" s="25"/>
+      <c r="EE31" s="25"/>
+      <c r="EF31" s="61"/>
+      <c r="EG31" s="32"/>
+      <c r="EH31" s="33"/>
+      <c r="EI31" s="33"/>
+      <c r="EJ31" s="33"/>
+      <c r="EK31" s="33"/>
+      <c r="EL31" s="33"/>
+      <c r="EM31" s="33"/>
+      <c r="EN31" s="33"/>
+      <c r="EO31" s="33"/>
+      <c r="EP31" s="33"/>
+      <c r="EQ31" s="33"/>
+      <c r="ER31" s="33"/>
+      <c r="ES31" s="34"/>
+      <c r="ET31" s="24"/>
+      <c r="EU31" s="25"/>
+      <c r="EV31" s="25"/>
+      <c r="EW31" s="25"/>
+      <c r="EX31" s="25"/>
+      <c r="EY31" s="25"/>
+      <c r="EZ31" s="25"/>
+      <c r="FA31" s="25"/>
+      <c r="FB31" s="25"/>
+      <c r="FC31" s="25"/>
+      <c r="FD31" s="25"/>
+      <c r="FE31" s="61"/>
+    </row>
+    <row r="32" spans="1:161" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="19"/>
+      <c r="P32" s="19"/>
+      <c r="Q32" s="19"/>
+      <c r="R32" s="19"/>
+      <c r="S32" s="19"/>
+      <c r="T32" s="20"/>
+      <c r="U32" s="21"/>
+      <c r="V32" s="22"/>
+      <c r="W32" s="22"/>
+      <c r="X32" s="22"/>
+      <c r="Y32" s="22"/>
+      <c r="Z32" s="22"/>
+      <c r="AA32" s="22"/>
+      <c r="AB32" s="23"/>
+      <c r="AC32" s="24"/>
+      <c r="AD32" s="25"/>
+      <c r="AE32" s="25"/>
+      <c r="AF32" s="25"/>
+      <c r="AG32" s="25"/>
+      <c r="AH32" s="61"/>
+      <c r="AI32" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ32" s="27"/>
+      <c r="AK32" s="27"/>
+      <c r="AL32" s="27"/>
+      <c r="AM32" s="27"/>
+      <c r="AN32" s="27"/>
+      <c r="AO32" s="27"/>
+      <c r="AP32" s="27"/>
+      <c r="AQ32" s="27"/>
+      <c r="AR32" s="27"/>
+      <c r="AS32" s="28"/>
+      <c r="AT32" s="29">
+        <v>3</v>
+      </c>
+      <c r="AU32" s="30"/>
+      <c r="AV32" s="30"/>
+      <c r="AW32" s="30"/>
+      <c r="AX32" s="30"/>
+      <c r="AY32" s="30"/>
+      <c r="AZ32" s="30"/>
+      <c r="BA32" s="31"/>
+      <c r="BB32" s="29">
+        <v>592.92999999999995</v>
+      </c>
+      <c r="BC32" s="30"/>
+      <c r="BD32" s="30"/>
+      <c r="BE32" s="30"/>
+      <c r="BF32" s="30"/>
+      <c r="BG32" s="30"/>
+      <c r="BH32" s="30"/>
+      <c r="BI32" s="30"/>
+      <c r="BJ32" s="30"/>
+      <c r="BK32" s="30"/>
+      <c r="BL32" s="31"/>
+      <c r="BM32" s="29"/>
+      <c r="BN32" s="30"/>
+      <c r="BO32" s="30"/>
+      <c r="BP32" s="30"/>
+      <c r="BQ32" s="30"/>
+      <c r="BR32" s="30"/>
+      <c r="BS32" s="30"/>
+      <c r="BT32" s="30"/>
+      <c r="BU32" s="30"/>
+      <c r="BV32" s="30"/>
+      <c r="BW32" s="30"/>
+      <c r="BX32" s="30"/>
+      <c r="BY32" s="30"/>
+      <c r="BZ32" s="30"/>
+      <c r="CA32" s="31"/>
+      <c r="CB32" s="29"/>
+      <c r="CC32" s="30"/>
+      <c r="CD32" s="30"/>
+      <c r="CE32" s="30"/>
+      <c r="CF32" s="30"/>
+      <c r="CG32" s="30"/>
+      <c r="CH32" s="30"/>
+      <c r="CI32" s="30"/>
+      <c r="CJ32" s="30"/>
+      <c r="CK32" s="31"/>
+      <c r="CL32" s="29"/>
+      <c r="CM32" s="30"/>
+      <c r="CN32" s="30"/>
+      <c r="CO32" s="30"/>
+      <c r="CP32" s="30"/>
+      <c r="CQ32" s="30"/>
+      <c r="CR32" s="30"/>
+      <c r="CS32" s="30"/>
+      <c r="CT32" s="30"/>
+      <c r="CU32" s="31"/>
+      <c r="CV32" s="29"/>
+      <c r="CW32" s="30"/>
+      <c r="CX32" s="30"/>
+      <c r="CY32" s="30"/>
+      <c r="CZ32" s="30"/>
+      <c r="DA32" s="30"/>
+      <c r="DB32" s="30"/>
+      <c r="DC32" s="30"/>
+      <c r="DD32" s="30"/>
+      <c r="DE32" s="30"/>
+      <c r="DF32" s="30"/>
+      <c r="DG32" s="31"/>
+      <c r="DH32" s="29">
+        <v>1778.79</v>
+      </c>
+      <c r="DI32" s="30"/>
+      <c r="DJ32" s="30"/>
+      <c r="DK32" s="30"/>
+      <c r="DL32" s="30"/>
+      <c r="DM32" s="30"/>
+      <c r="DN32" s="30"/>
+      <c r="DO32" s="30"/>
+      <c r="DP32" s="30"/>
+      <c r="DQ32" s="30"/>
+      <c r="DR32" s="30"/>
+      <c r="DS32" s="30"/>
+      <c r="DT32" s="30"/>
+      <c r="DU32" s="30"/>
+      <c r="DV32" s="31"/>
+      <c r="DW32" s="24"/>
+      <c r="DX32" s="25"/>
+      <c r="DY32" s="25"/>
+      <c r="DZ32" s="25"/>
+      <c r="EA32" s="25"/>
+      <c r="EB32" s="25"/>
+      <c r="EC32" s="25"/>
+      <c r="ED32" s="25"/>
+      <c r="EE32" s="25"/>
+      <c r="EF32" s="61"/>
+      <c r="EG32" s="32"/>
+      <c r="EH32" s="33"/>
+      <c r="EI32" s="33"/>
+      <c r="EJ32" s="33"/>
+      <c r="EK32" s="33"/>
+      <c r="EL32" s="33"/>
+      <c r="EM32" s="33"/>
+      <c r="EN32" s="33"/>
+      <c r="EO32" s="33"/>
+      <c r="EP32" s="33"/>
+      <c r="EQ32" s="33"/>
+      <c r="ER32" s="33"/>
+      <c r="ES32" s="34"/>
+      <c r="ET32" s="24"/>
+      <c r="EU32" s="25"/>
+      <c r="EV32" s="25"/>
+      <c r="EW32" s="25"/>
+      <c r="EX32" s="25"/>
+      <c r="EY32" s="25"/>
+      <c r="EZ32" s="25"/>
+      <c r="FA32" s="25"/>
+      <c r="FB32" s="25"/>
+      <c r="FC32" s="25"/>
+      <c r="FD32" s="25"/>
+      <c r="FE32" s="61"/>
+    </row>
+    <row r="33" spans="1:161" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="19"/>
+      <c r="O33" s="19"/>
+      <c r="P33" s="19"/>
+      <c r="Q33" s="19"/>
+      <c r="R33" s="19"/>
+      <c r="S33" s="19"/>
+      <c r="T33" s="20"/>
+      <c r="U33" s="21"/>
+      <c r="V33" s="22"/>
+      <c r="W33" s="22"/>
+      <c r="X33" s="22"/>
+      <c r="Y33" s="22"/>
+      <c r="Z33" s="22"/>
+      <c r="AA33" s="22"/>
+      <c r="AB33" s="23"/>
+      <c r="AC33" s="24"/>
+      <c r="AD33" s="25"/>
+      <c r="AE33" s="25"/>
+      <c r="AF33" s="25"/>
+      <c r="AG33" s="25"/>
+      <c r="AH33" s="61"/>
+      <c r="AI33" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ33" s="27"/>
+      <c r="AK33" s="27"/>
+      <c r="AL33" s="27"/>
+      <c r="AM33" s="27"/>
+      <c r="AN33" s="27"/>
+      <c r="AO33" s="27"/>
+      <c r="AP33" s="27"/>
+      <c r="AQ33" s="27"/>
+      <c r="AR33" s="27"/>
+      <c r="AS33" s="28"/>
+      <c r="AT33" s="29">
+        <v>3</v>
+      </c>
+      <c r="AU33" s="30"/>
+      <c r="AV33" s="30"/>
+      <c r="AW33" s="30"/>
+      <c r="AX33" s="30"/>
+      <c r="AY33" s="30"/>
+      <c r="AZ33" s="30"/>
+      <c r="BA33" s="31"/>
+      <c r="BB33" s="29">
+        <v>592.92999999999995</v>
+      </c>
+      <c r="BC33" s="30"/>
+      <c r="BD33" s="30"/>
+      <c r="BE33" s="30"/>
+      <c r="BF33" s="30"/>
+      <c r="BG33" s="30"/>
+      <c r="BH33" s="30"/>
+      <c r="BI33" s="30"/>
+      <c r="BJ33" s="30"/>
+      <c r="BK33" s="30"/>
+      <c r="BL33" s="31"/>
+      <c r="BM33" s="29"/>
+      <c r="BN33" s="30"/>
+      <c r="BO33" s="30"/>
+      <c r="BP33" s="30"/>
+      <c r="BQ33" s="30"/>
+      <c r="BR33" s="30"/>
+      <c r="BS33" s="30"/>
+      <c r="BT33" s="30"/>
+      <c r="BU33" s="30"/>
+      <c r="BV33" s="30"/>
+      <c r="BW33" s="30"/>
+      <c r="BX33" s="30"/>
+      <c r="BY33" s="30"/>
+      <c r="BZ33" s="30"/>
+      <c r="CA33" s="31"/>
+      <c r="CB33" s="29"/>
+      <c r="CC33" s="30"/>
+      <c r="CD33" s="30"/>
+      <c r="CE33" s="30"/>
+      <c r="CF33" s="30"/>
+      <c r="CG33" s="30"/>
+      <c r="CH33" s="30"/>
+      <c r="CI33" s="30"/>
+      <c r="CJ33" s="30"/>
+      <c r="CK33" s="31"/>
+      <c r="CL33" s="29"/>
+      <c r="CM33" s="30"/>
+      <c r="CN33" s="30"/>
+      <c r="CO33" s="30"/>
+      <c r="CP33" s="30"/>
+      <c r="CQ33" s="30"/>
+      <c r="CR33" s="30"/>
+      <c r="CS33" s="30"/>
+      <c r="CT33" s="30"/>
+      <c r="CU33" s="31"/>
+      <c r="CV33" s="29"/>
+      <c r="CW33" s="30"/>
+      <c r="CX33" s="30"/>
+      <c r="CY33" s="30"/>
+      <c r="CZ33" s="30"/>
+      <c r="DA33" s="30"/>
+      <c r="DB33" s="30"/>
+      <c r="DC33" s="30"/>
+      <c r="DD33" s="30"/>
+      <c r="DE33" s="30"/>
+      <c r="DF33" s="30"/>
+      <c r="DG33" s="31"/>
+      <c r="DH33" s="29">
+        <v>1778.79</v>
+      </c>
+      <c r="DI33" s="30"/>
+      <c r="DJ33" s="30"/>
+      <c r="DK33" s="30"/>
+      <c r="DL33" s="30"/>
+      <c r="DM33" s="30"/>
+      <c r="DN33" s="30"/>
+      <c r="DO33" s="30"/>
+      <c r="DP33" s="30"/>
+      <c r="DQ33" s="30"/>
+      <c r="DR33" s="30"/>
+      <c r="DS33" s="30"/>
+      <c r="DT33" s="30"/>
+      <c r="DU33" s="30"/>
+      <c r="DV33" s="31"/>
+      <c r="DW33" s="24"/>
+      <c r="DX33" s="25"/>
+      <c r="DY33" s="25"/>
+      <c r="DZ33" s="25"/>
+      <c r="EA33" s="25"/>
+      <c r="EB33" s="25"/>
+      <c r="EC33" s="25"/>
+      <c r="ED33" s="25"/>
+      <c r="EE33" s="25"/>
+      <c r="EF33" s="61"/>
+      <c r="EG33" s="32"/>
+      <c r="EH33" s="33"/>
+      <c r="EI33" s="33"/>
+      <c r="EJ33" s="33"/>
+      <c r="EK33" s="33"/>
+      <c r="EL33" s="33"/>
+      <c r="EM33" s="33"/>
+      <c r="EN33" s="33"/>
+      <c r="EO33" s="33"/>
+      <c r="EP33" s="33"/>
+      <c r="EQ33" s="33"/>
+      <c r="ER33" s="33"/>
+      <c r="ES33" s="34"/>
+      <c r="ET33" s="24"/>
+      <c r="EU33" s="25"/>
+      <c r="EV33" s="25"/>
+      <c r="EW33" s="25"/>
+      <c r="EX33" s="25"/>
+      <c r="EY33" s="25"/>
+      <c r="EZ33" s="25"/>
+      <c r="FA33" s="25"/>
+      <c r="FB33" s="25"/>
+      <c r="FC33" s="25"/>
+      <c r="FD33" s="25"/>
+      <c r="FE33" s="61"/>
+    </row>
+    <row r="34" spans="1:161" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+      <c r="O34" s="19"/>
+      <c r="P34" s="19"/>
+      <c r="Q34" s="19"/>
+      <c r="R34" s="19"/>
+      <c r="S34" s="19"/>
+      <c r="T34" s="20"/>
+      <c r="U34" s="21"/>
+      <c r="V34" s="22"/>
+      <c r="W34" s="22"/>
+      <c r="X34" s="22"/>
+      <c r="Y34" s="22"/>
+      <c r="Z34" s="22"/>
+      <c r="AA34" s="22"/>
+      <c r="AB34" s="23"/>
+      <c r="AC34" s="24"/>
+      <c r="AD34" s="25"/>
+      <c r="AE34" s="25"/>
+      <c r="AF34" s="25"/>
+      <c r="AG34" s="25"/>
+      <c r="AH34" s="61"/>
+      <c r="AI34" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ34" s="27"/>
+      <c r="AK34" s="27"/>
+      <c r="AL34" s="27"/>
+      <c r="AM34" s="27"/>
+      <c r="AN34" s="27"/>
+      <c r="AO34" s="27"/>
+      <c r="AP34" s="27"/>
+      <c r="AQ34" s="27"/>
+      <c r="AR34" s="27"/>
+      <c r="AS34" s="28"/>
+      <c r="AT34" s="29">
+        <v>3</v>
+      </c>
+      <c r="AU34" s="30"/>
+      <c r="AV34" s="30"/>
+      <c r="AW34" s="30"/>
+      <c r="AX34" s="30"/>
+      <c r="AY34" s="30"/>
+      <c r="AZ34" s="30"/>
+      <c r="BA34" s="31"/>
+      <c r="BB34" s="29">
+        <v>592.92999999999995</v>
+      </c>
+      <c r="BC34" s="30"/>
+      <c r="BD34" s="30"/>
+      <c r="BE34" s="30"/>
+      <c r="BF34" s="30"/>
+      <c r="BG34" s="30"/>
+      <c r="BH34" s="30"/>
+      <c r="BI34" s="30"/>
+      <c r="BJ34" s="30"/>
+      <c r="BK34" s="30"/>
+      <c r="BL34" s="31"/>
+      <c r="BM34" s="29"/>
+      <c r="BN34" s="30"/>
+      <c r="BO34" s="30"/>
+      <c r="BP34" s="30"/>
+      <c r="BQ34" s="30"/>
+      <c r="BR34" s="30"/>
+      <c r="BS34" s="30"/>
+      <c r="BT34" s="30"/>
+      <c r="BU34" s="30"/>
+      <c r="BV34" s="30"/>
+      <c r="BW34" s="30"/>
+      <c r="BX34" s="30"/>
+      <c r="BY34" s="30"/>
+      <c r="BZ34" s="30"/>
+      <c r="CA34" s="31"/>
+      <c r="CB34" s="29"/>
+      <c r="CC34" s="30"/>
+      <c r="CD34" s="30"/>
+      <c r="CE34" s="30"/>
+      <c r="CF34" s="30"/>
+      <c r="CG34" s="30"/>
+      <c r="CH34" s="30"/>
+      <c r="CI34" s="30"/>
+      <c r="CJ34" s="30"/>
+      <c r="CK34" s="31"/>
+      <c r="CL34" s="29"/>
+      <c r="CM34" s="30"/>
+      <c r="CN34" s="30"/>
+      <c r="CO34" s="30"/>
+      <c r="CP34" s="30"/>
+      <c r="CQ34" s="30"/>
+      <c r="CR34" s="30"/>
+      <c r="CS34" s="30"/>
+      <c r="CT34" s="30"/>
+      <c r="CU34" s="31"/>
+      <c r="CV34" s="29"/>
+      <c r="CW34" s="30"/>
+      <c r="CX34" s="30"/>
+      <c r="CY34" s="30"/>
+      <c r="CZ34" s="30"/>
+      <c r="DA34" s="30"/>
+      <c r="DB34" s="30"/>
+      <c r="DC34" s="30"/>
+      <c r="DD34" s="30"/>
+      <c r="DE34" s="30"/>
+      <c r="DF34" s="30"/>
+      <c r="DG34" s="31"/>
+      <c r="DH34" s="29">
+        <v>1778.79</v>
+      </c>
+      <c r="DI34" s="30"/>
+      <c r="DJ34" s="30"/>
+      <c r="DK34" s="30"/>
+      <c r="DL34" s="30"/>
+      <c r="DM34" s="30"/>
+      <c r="DN34" s="30"/>
+      <c r="DO34" s="30"/>
+      <c r="DP34" s="30"/>
+      <c r="DQ34" s="30"/>
+      <c r="DR34" s="30"/>
+      <c r="DS34" s="30"/>
+      <c r="DT34" s="30"/>
+      <c r="DU34" s="30"/>
+      <c r="DV34" s="31"/>
+      <c r="DW34" s="24"/>
+      <c r="DX34" s="25"/>
+      <c r="DY34" s="25"/>
+      <c r="DZ34" s="25"/>
+      <c r="EA34" s="25"/>
+      <c r="EB34" s="25"/>
+      <c r="EC34" s="25"/>
+      <c r="ED34" s="25"/>
+      <c r="EE34" s="25"/>
+      <c r="EF34" s="61"/>
+      <c r="EG34" s="32"/>
+      <c r="EH34" s="33"/>
+      <c r="EI34" s="33"/>
+      <c r="EJ34" s="33"/>
+      <c r="EK34" s="33"/>
+      <c r="EL34" s="33"/>
+      <c r="EM34" s="33"/>
+      <c r="EN34" s="33"/>
+      <c r="EO34" s="33"/>
+      <c r="EP34" s="33"/>
+      <c r="EQ34" s="33"/>
+      <c r="ER34" s="33"/>
+      <c r="ES34" s="34"/>
+      <c r="ET34" s="24"/>
+      <c r="EU34" s="25"/>
+      <c r="EV34" s="25"/>
+      <c r="EW34" s="25"/>
+      <c r="EX34" s="25"/>
+      <c r="EY34" s="25"/>
+      <c r="EZ34" s="25"/>
+      <c r="FA34" s="25"/>
+      <c r="FB34" s="25"/>
+      <c r="FC34" s="25"/>
+      <c r="FD34" s="25"/>
+      <c r="FE34" s="61"/>
+    </row>
+    <row r="35" spans="1:161" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="19"/>
+      <c r="O35" s="19"/>
+      <c r="P35" s="19"/>
+      <c r="Q35" s="19"/>
+      <c r="R35" s="19"/>
+      <c r="S35" s="19"/>
+      <c r="T35" s="20"/>
+      <c r="U35" s="21"/>
+      <c r="V35" s="22"/>
+      <c r="W35" s="22"/>
+      <c r="X35" s="22"/>
+      <c r="Y35" s="22"/>
+      <c r="Z35" s="22"/>
+      <c r="AA35" s="22"/>
+      <c r="AB35" s="23"/>
+      <c r="AC35" s="24"/>
+      <c r="AD35" s="25"/>
+      <c r="AE35" s="25"/>
+      <c r="AF35" s="25"/>
+      <c r="AG35" s="25"/>
+      <c r="AH35" s="61"/>
+      <c r="AI35" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="AJ35" s="27"/>
+      <c r="AK35" s="27"/>
+      <c r="AL35" s="27"/>
+      <c r="AM35" s="27"/>
+      <c r="AN35" s="27"/>
+      <c r="AO35" s="27"/>
+      <c r="AP35" s="27"/>
+      <c r="AQ35" s="27"/>
+      <c r="AR35" s="27"/>
+      <c r="AS35" s="28"/>
+      <c r="AT35" s="29">
+        <v>3264</v>
+      </c>
+      <c r="AU35" s="30"/>
+      <c r="AV35" s="30"/>
+      <c r="AW35" s="30"/>
+      <c r="AX35" s="30"/>
+      <c r="AY35" s="30"/>
+      <c r="AZ35" s="30"/>
+      <c r="BA35" s="31"/>
+      <c r="BB35" s="29">
+        <v>134.21</v>
+      </c>
+      <c r="BC35" s="30"/>
+      <c r="BD35" s="30"/>
+      <c r="BE35" s="30"/>
+      <c r="BF35" s="30"/>
+      <c r="BG35" s="30"/>
+      <c r="BH35" s="30"/>
+      <c r="BI35" s="30"/>
+      <c r="BJ35" s="30"/>
+      <c r="BK35" s="30"/>
+      <c r="BL35" s="31"/>
+      <c r="BM35" s="29"/>
+      <c r="BN35" s="30"/>
+      <c r="BO35" s="30"/>
+      <c r="BP35" s="30"/>
+      <c r="BQ35" s="30"/>
+      <c r="BR35" s="30"/>
+      <c r="BS35" s="30"/>
+      <c r="BT35" s="30"/>
+      <c r="BU35" s="30"/>
+      <c r="BV35" s="30"/>
+      <c r="BW35" s="30"/>
+      <c r="BX35" s="30"/>
+      <c r="BY35" s="30"/>
+      <c r="BZ35" s="30"/>
+      <c r="CA35" s="31"/>
+      <c r="CB35" s="29"/>
+      <c r="CC35" s="30"/>
+      <c r="CD35" s="30"/>
+      <c r="CE35" s="30"/>
+      <c r="CF35" s="30"/>
+      <c r="CG35" s="30"/>
+      <c r="CH35" s="30"/>
+      <c r="CI35" s="30"/>
+      <c r="CJ35" s="30"/>
+      <c r="CK35" s="31"/>
+      <c r="CL35" s="29"/>
+      <c r="CM35" s="30"/>
+      <c r="CN35" s="30"/>
+      <c r="CO35" s="30"/>
+      <c r="CP35" s="30"/>
+      <c r="CQ35" s="30"/>
+      <c r="CR35" s="30"/>
+      <c r="CS35" s="30"/>
+      <c r="CT35" s="30"/>
+      <c r="CU35" s="31"/>
+      <c r="CV35" s="29"/>
+      <c r="CW35" s="30"/>
+      <c r="CX35" s="30"/>
+      <c r="CY35" s="30"/>
+      <c r="CZ35" s="30"/>
+      <c r="DA35" s="30"/>
+      <c r="DB35" s="30"/>
+      <c r="DC35" s="30"/>
+      <c r="DD35" s="30"/>
+      <c r="DE35" s="30"/>
+      <c r="DF35" s="30"/>
+      <c r="DG35" s="31"/>
+      <c r="DH35" s="29">
+        <v>438061.44</v>
+      </c>
+      <c r="DI35" s="30"/>
+      <c r="DJ35" s="30"/>
+      <c r="DK35" s="30"/>
+      <c r="DL35" s="30"/>
+      <c r="DM35" s="30"/>
+      <c r="DN35" s="30"/>
+      <c r="DO35" s="30"/>
+      <c r="DP35" s="30"/>
+      <c r="DQ35" s="30"/>
+      <c r="DR35" s="30"/>
+      <c r="DS35" s="30"/>
+      <c r="DT35" s="30"/>
+      <c r="DU35" s="30"/>
+      <c r="DV35" s="31"/>
+      <c r="DW35" s="24"/>
+      <c r="DX35" s="25"/>
+      <c r="DY35" s="25"/>
+      <c r="DZ35" s="25"/>
+      <c r="EA35" s="25"/>
+      <c r="EB35" s="25"/>
+      <c r="EC35" s="25"/>
+      <c r="ED35" s="25"/>
+      <c r="EE35" s="25"/>
+      <c r="EF35" s="61"/>
+      <c r="EG35" s="32"/>
+      <c r="EH35" s="33"/>
+      <c r="EI35" s="33"/>
+      <c r="EJ35" s="33"/>
+      <c r="EK35" s="33"/>
+      <c r="EL35" s="33"/>
+      <c r="EM35" s="33"/>
+      <c r="EN35" s="33"/>
+      <c r="EO35" s="33"/>
+      <c r="EP35" s="33"/>
+      <c r="EQ35" s="33"/>
+      <c r="ER35" s="33"/>
+      <c r="ES35" s="34"/>
+      <c r="ET35" s="24"/>
+      <c r="EU35" s="25"/>
+      <c r="EV35" s="25"/>
+      <c r="EW35" s="25"/>
+      <c r="EX35" s="25"/>
+      <c r="EY35" s="25"/>
+      <c r="EZ35" s="25"/>
+      <c r="FA35" s="25"/>
+      <c r="FB35" s="25"/>
+      <c r="FC35" s="25"/>
+      <c r="FD35" s="25"/>
+      <c r="FE35" s="61"/>
+    </row>
+    <row r="36" spans="1:161" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A36" s="18"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="19"/>
+      <c r="N36" s="19"/>
+      <c r="O36" s="19"/>
+      <c r="P36" s="19"/>
+      <c r="Q36" s="19"/>
+      <c r="R36" s="19"/>
+      <c r="S36" s="19"/>
+      <c r="T36" s="20"/>
+      <c r="U36" s="21"/>
+      <c r="V36" s="22"/>
+      <c r="W36" s="22"/>
+      <c r="X36" s="22"/>
+      <c r="Y36" s="22"/>
+      <c r="Z36" s="22"/>
+      <c r="AA36" s="22"/>
+      <c r="AB36" s="23"/>
+      <c r="AC36" s="24"/>
+      <c r="AD36" s="25"/>
+      <c r="AE36" s="25"/>
+      <c r="AF36" s="25"/>
+      <c r="AG36" s="25"/>
+      <c r="AH36" s="25"/>
+      <c r="AI36" s="26"/>
+      <c r="AJ36" s="27"/>
+      <c r="AK36" s="27"/>
+      <c r="AL36" s="27"/>
+      <c r="AM36" s="27"/>
+      <c r="AN36" s="27"/>
+      <c r="AO36" s="27"/>
+      <c r="AP36" s="27"/>
+      <c r="AQ36" s="27"/>
+      <c r="AR36" s="27"/>
+      <c r="AS36" s="28"/>
+      <c r="AT36" s="29"/>
+      <c r="AU36" s="30"/>
+      <c r="AV36" s="30"/>
+      <c r="AW36" s="30"/>
+      <c r="AX36" s="30"/>
+      <c r="AY36" s="30"/>
+      <c r="AZ36" s="30"/>
+      <c r="BA36" s="31"/>
+      <c r="BB36" s="29"/>
+      <c r="BC36" s="30"/>
+      <c r="BD36" s="30"/>
+      <c r="BE36" s="30"/>
+      <c r="BF36" s="30"/>
+      <c r="BG36" s="30"/>
+      <c r="BH36" s="30"/>
+      <c r="BI36" s="30"/>
+      <c r="BJ36" s="30"/>
+      <c r="BK36" s="30"/>
+      <c r="BL36" s="31"/>
+      <c r="BM36" s="29"/>
+      <c r="BN36" s="30"/>
+      <c r="BO36" s="30"/>
+      <c r="BP36" s="30"/>
+      <c r="BQ36" s="30"/>
+      <c r="BR36" s="30"/>
+      <c r="BS36" s="30"/>
+      <c r="BT36" s="30"/>
+      <c r="BU36" s="30"/>
+      <c r="BV36" s="30"/>
+      <c r="BW36" s="30"/>
+      <c r="BX36" s="30"/>
+      <c r="BY36" s="30"/>
+      <c r="BZ36" s="30"/>
+      <c r="CA36" s="31"/>
+      <c r="CB36" s="29"/>
+      <c r="CC36" s="30"/>
+      <c r="CD36" s="30"/>
+      <c r="CE36" s="30"/>
+      <c r="CF36" s="30"/>
+      <c r="CG36" s="30"/>
+      <c r="CH36" s="30"/>
+      <c r="CI36" s="30"/>
+      <c r="CJ36" s="30"/>
+      <c r="CK36" s="31"/>
+      <c r="CL36" s="29"/>
+      <c r="CM36" s="30"/>
+      <c r="CN36" s="30"/>
+      <c r="CO36" s="30"/>
+      <c r="CP36" s="30"/>
+      <c r="CQ36" s="30"/>
+      <c r="CR36" s="30"/>
+      <c r="CS36" s="30"/>
+      <c r="CT36" s="30"/>
+      <c r="CU36" s="31"/>
+      <c r="CV36" s="29"/>
+      <c r="CW36" s="30"/>
+      <c r="CX36" s="30"/>
+      <c r="CY36" s="30"/>
+      <c r="CZ36" s="30"/>
+      <c r="DA36" s="30"/>
+      <c r="DB36" s="30"/>
+      <c r="DC36" s="30"/>
+      <c r="DD36" s="30"/>
+      <c r="DE36" s="30"/>
+      <c r="DF36" s="30"/>
+      <c r="DG36" s="31"/>
+      <c r="DH36" s="29"/>
+      <c r="DI36" s="30"/>
+      <c r="DJ36" s="30"/>
+      <c r="DK36" s="30"/>
+      <c r="DL36" s="30"/>
+      <c r="DM36" s="30"/>
+      <c r="DN36" s="30"/>
+      <c r="DO36" s="30"/>
+      <c r="DP36" s="30"/>
+      <c r="DQ36" s="30"/>
+      <c r="DR36" s="30"/>
+      <c r="DS36" s="30"/>
+      <c r="DT36" s="30"/>
+      <c r="DU36" s="30"/>
+      <c r="DV36" s="31"/>
+      <c r="DW36" s="24"/>
+      <c r="DX36" s="25"/>
+      <c r="DY36" s="25"/>
+      <c r="DZ36" s="25"/>
+      <c r="EA36" s="25"/>
+      <c r="EB36" s="25"/>
+      <c r="EC36" s="25"/>
+      <c r="ED36" s="25"/>
+      <c r="EE36" s="25"/>
+      <c r="EF36" s="25"/>
+      <c r="EG36" s="32"/>
+      <c r="EH36" s="33"/>
+      <c r="EI36" s="33"/>
+      <c r="EJ36" s="33"/>
+      <c r="EK36" s="33"/>
+      <c r="EL36" s="33"/>
+      <c r="EM36" s="33"/>
+      <c r="EN36" s="33"/>
+      <c r="EO36" s="33"/>
+      <c r="EP36" s="33"/>
+      <c r="EQ36" s="33"/>
+      <c r="ER36" s="33"/>
+      <c r="ES36" s="34"/>
+      <c r="ET36" s="17"/>
+      <c r="EU36" s="17"/>
+      <c r="EV36" s="17"/>
+      <c r="EW36" s="17"/>
+      <c r="EX36" s="17"/>
+      <c r="EY36" s="17"/>
+      <c r="EZ36" s="17"/>
+      <c r="FA36" s="17"/>
+      <c r="FB36" s="17"/>
+      <c r="FC36" s="17"/>
+      <c r="FD36" s="17"/>
+      <c r="FE36" s="17"/>
+    </row>
+    <row r="37" spans="1:161" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A37" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="53"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="53"/>
+      <c r="H37" s="53"/>
+      <c r="I37" s="53"/>
+      <c r="J37" s="53"/>
+      <c r="K37" s="53"/>
+      <c r="L37" s="53"/>
+      <c r="M37" s="53"/>
+      <c r="N37" s="53"/>
+      <c r="O37" s="53"/>
+      <c r="P37" s="53"/>
+      <c r="Q37" s="53"/>
+      <c r="R37" s="53"/>
+      <c r="S37" s="53"/>
+      <c r="T37" s="53"/>
+      <c r="U37" s="53"/>
+      <c r="V37" s="53"/>
+      <c r="W37" s="53"/>
+      <c r="X37" s="53"/>
+      <c r="Y37" s="53"/>
+      <c r="Z37" s="53"/>
+      <c r="AA37" s="53"/>
+      <c r="AB37" s="53"/>
+      <c r="AC37" s="53"/>
+      <c r="AD37" s="53"/>
+      <c r="AE37" s="53"/>
+      <c r="AF37" s="53"/>
+      <c r="AG37" s="53"/>
+      <c r="AH37" s="53"/>
+      <c r="AI37" s="53"/>
+      <c r="AJ37" s="53"/>
+      <c r="AK37" s="53"/>
+      <c r="AL37" s="53"/>
+      <c r="AM37" s="53"/>
+      <c r="AN37" s="53"/>
+      <c r="AO37" s="53"/>
+      <c r="AP37" s="53"/>
+      <c r="AQ37" s="53"/>
+      <c r="AR37" s="53"/>
+      <c r="AS37" s="53"/>
+      <c r="AT37" s="53"/>
+      <c r="AU37" s="53"/>
+      <c r="AV37" s="53"/>
+      <c r="AW37" s="53"/>
+      <c r="AX37" s="53"/>
+      <c r="AY37" s="53"/>
+      <c r="AZ37" s="53"/>
+      <c r="BA37" s="53"/>
+      <c r="BB37" s="53"/>
+      <c r="BC37" s="53"/>
+      <c r="BD37" s="53"/>
+      <c r="BE37" s="53"/>
+      <c r="BF37" s="53"/>
+      <c r="BG37" s="53"/>
+      <c r="BH37" s="53"/>
+      <c r="BI37" s="53"/>
+      <c r="BJ37" s="53"/>
+      <c r="BK37" s="53"/>
+      <c r="BL37" s="53"/>
+      <c r="BM37" s="29"/>
+      <c r="BN37" s="30"/>
+      <c r="BO37" s="30"/>
+      <c r="BP37" s="30"/>
+      <c r="BQ37" s="30"/>
+      <c r="BR37" s="30"/>
+      <c r="BS37" s="30"/>
+      <c r="BT37" s="30"/>
+      <c r="BU37" s="30"/>
+      <c r="BV37" s="30"/>
+      <c r="BW37" s="30"/>
+      <c r="BX37" s="30"/>
+      <c r="BY37" s="30"/>
+      <c r="BZ37" s="30"/>
+      <c r="CA37" s="31"/>
+      <c r="CB37" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="CC37" s="30"/>
+      <c r="CD37" s="30"/>
+      <c r="CE37" s="30"/>
+      <c r="CF37" s="30"/>
+      <c r="CG37" s="30"/>
+      <c r="CH37" s="30"/>
+      <c r="CI37" s="30"/>
+      <c r="CJ37" s="30"/>
+      <c r="CK37" s="30"/>
+      <c r="CL37" s="30"/>
+      <c r="CM37" s="30"/>
+      <c r="CN37" s="30"/>
+      <c r="CO37" s="30"/>
+      <c r="CP37" s="30"/>
+      <c r="CQ37" s="30"/>
+      <c r="CR37" s="30"/>
+      <c r="CS37" s="30"/>
+      <c r="CT37" s="30"/>
+      <c r="CU37" s="31"/>
+      <c r="CV37" s="51"/>
+      <c r="CW37" s="51"/>
+      <c r="CX37" s="51"/>
+      <c r="CY37" s="51"/>
+      <c r="CZ37" s="51"/>
+      <c r="DA37" s="51"/>
+      <c r="DB37" s="51"/>
+      <c r="DC37" s="51"/>
+      <c r="DD37" s="51"/>
+      <c r="DE37" s="51"/>
+      <c r="DF37" s="51"/>
+      <c r="DG37" s="51"/>
+      <c r="DH37" s="51">
+        <v>456123</v>
+      </c>
+      <c r="DI37" s="51"/>
+      <c r="DJ37" s="51"/>
+      <c r="DK37" s="51"/>
+      <c r="DL37" s="51"/>
+      <c r="DM37" s="51"/>
+      <c r="DN37" s="51"/>
+      <c r="DO37" s="51"/>
+      <c r="DP37" s="51"/>
+      <c r="DQ37" s="51"/>
+      <c r="DR37" s="51"/>
+      <c r="DS37" s="51"/>
+      <c r="DT37" s="51"/>
+      <c r="DU37" s="51"/>
+      <c r="DV37" s="51"/>
+    </row>
+    <row r="38" spans="1:161" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:161" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="CD31" s="1" t="s">
+      <c r="CD39" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:161" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+    <row r="40" spans="1:161" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AH32" s="36"/>
-      <c r="AI32" s="36"/>
-      <c r="AJ32" s="36"/>
-      <c r="AK32" s="36"/>
-      <c r="AL32" s="36"/>
-      <c r="AM32" s="36"/>
-      <c r="AN32" s="36"/>
-      <c r="AO32" s="36"/>
-      <c r="AP32" s="36"/>
-      <c r="AQ32" s="36"/>
-      <c r="AR32" s="36"/>
-      <c r="AS32" s="36"/>
-      <c r="AT32" s="36"/>
-      <c r="AU32" s="36"/>
-      <c r="AV32" s="36"/>
-      <c r="AW32" s="36"/>
-      <c r="AZ32" s="36"/>
-      <c r="BA32" s="36"/>
-      <c r="BB32" s="36"/>
-      <c r="BC32" s="36"/>
-      <c r="BD32" s="36"/>
-      <c r="BE32" s="36"/>
-      <c r="BF32" s="36"/>
-      <c r="BG32" s="36"/>
-      <c r="BH32" s="36"/>
-      <c r="BI32" s="36"/>
-      <c r="BJ32" s="36"/>
-      <c r="BK32" s="36"/>
-      <c r="BL32" s="36"/>
-      <c r="BM32" s="36"/>
-      <c r="BN32" s="36"/>
-      <c r="BO32" s="36"/>
-      <c r="BP32" s="36"/>
-      <c r="BQ32" s="36"/>
-      <c r="BR32" s="36"/>
-      <c r="BS32" s="36"/>
-      <c r="BT32" s="36"/>
-      <c r="BU32" s="36"/>
-      <c r="BV32" s="36"/>
-      <c r="BW32" s="36"/>
-      <c r="BX32" s="36"/>
-      <c r="BY32" s="36"/>
-      <c r="BZ32" s="36"/>
-      <c r="CA32" s="36"/>
-      <c r="CB32" s="36"/>
-      <c r="CD32" s="1" t="s">
+      <c r="AH40" s="36"/>
+      <c r="AI40" s="36"/>
+      <c r="AJ40" s="36"/>
+      <c r="AK40" s="36"/>
+      <c r="AL40" s="36"/>
+      <c r="AM40" s="36"/>
+      <c r="AN40" s="36"/>
+      <c r="AO40" s="36"/>
+      <c r="AP40" s="36"/>
+      <c r="AQ40" s="36"/>
+      <c r="AR40" s="36"/>
+      <c r="AS40" s="36"/>
+      <c r="AT40" s="36"/>
+      <c r="AU40" s="36"/>
+      <c r="AV40" s="36"/>
+      <c r="AW40" s="36"/>
+      <c r="AZ40" s="36"/>
+      <c r="BA40" s="36"/>
+      <c r="BB40" s="36"/>
+      <c r="BC40" s="36"/>
+      <c r="BD40" s="36"/>
+      <c r="BE40" s="36"/>
+      <c r="BF40" s="36"/>
+      <c r="BG40" s="36"/>
+      <c r="BH40" s="36"/>
+      <c r="BI40" s="36"/>
+      <c r="BJ40" s="36"/>
+      <c r="BK40" s="36"/>
+      <c r="BL40" s="36"/>
+      <c r="BM40" s="36"/>
+      <c r="BN40" s="36"/>
+      <c r="BO40" s="36"/>
+      <c r="BP40" s="36"/>
+      <c r="BQ40" s="36"/>
+      <c r="BR40" s="36"/>
+      <c r="BS40" s="36"/>
+      <c r="BT40" s="36"/>
+      <c r="BU40" s="36"/>
+      <c r="BV40" s="36"/>
+      <c r="BW40" s="36"/>
+      <c r="BX40" s="36"/>
+      <c r="BY40" s="36"/>
+      <c r="BZ40" s="36"/>
+      <c r="CA40" s="36"/>
+      <c r="CB40" s="36"/>
+      <c r="CD40" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="DK32" s="36"/>
-      <c r="DL32" s="36"/>
-      <c r="DM32" s="36"/>
-      <c r="DN32" s="36"/>
-      <c r="DO32" s="36"/>
-      <c r="DP32" s="36"/>
-      <c r="DQ32" s="36"/>
-      <c r="DR32" s="36"/>
-      <c r="DS32" s="36"/>
-      <c r="DT32" s="36"/>
-      <c r="DU32" s="36"/>
-      <c r="DV32" s="36"/>
-      <c r="DW32" s="36"/>
-      <c r="DX32" s="36"/>
-      <c r="DY32" s="36"/>
-      <c r="DZ32" s="36"/>
-      <c r="EC32" s="36"/>
-      <c r="ED32" s="36"/>
-      <c r="EE32" s="36"/>
-      <c r="EF32" s="36"/>
-      <c r="EG32" s="36"/>
-      <c r="EH32" s="36"/>
-      <c r="EI32" s="36"/>
-      <c r="EJ32" s="36"/>
-      <c r="EK32" s="36"/>
-      <c r="EL32" s="36"/>
-      <c r="EM32" s="36"/>
-      <c r="EN32" s="36"/>
-      <c r="EO32" s="36"/>
-      <c r="EP32" s="36"/>
-      <c r="EQ32" s="36"/>
-      <c r="ER32" s="36"/>
-      <c r="ES32" s="36"/>
-      <c r="ET32" s="36"/>
-      <c r="EU32" s="36"/>
-      <c r="EV32" s="36"/>
-      <c r="EW32" s="36"/>
-      <c r="EX32" s="36"/>
-      <c r="EY32" s="36"/>
-      <c r="EZ32" s="36"/>
-      <c r="FA32" s="36"/>
-      <c r="FB32" s="36"/>
-      <c r="FC32" s="36"/>
-      <c r="FD32" s="36"/>
-      <c r="FE32" s="36"/>
+      <c r="DK40" s="36"/>
+      <c r="DL40" s="36"/>
+      <c r="DM40" s="36"/>
+      <c r="DN40" s="36"/>
+      <c r="DO40" s="36"/>
+      <c r="DP40" s="36"/>
+      <c r="DQ40" s="36"/>
+      <c r="DR40" s="36"/>
+      <c r="DS40" s="36"/>
+      <c r="DT40" s="36"/>
+      <c r="DU40" s="36"/>
+      <c r="DV40" s="36"/>
+      <c r="DW40" s="36"/>
+      <c r="DX40" s="36"/>
+      <c r="DY40" s="36"/>
+      <c r="DZ40" s="36"/>
+      <c r="EC40" s="36"/>
+      <c r="ED40" s="36"/>
+      <c r="EE40" s="36"/>
+      <c r="EF40" s="36"/>
+      <c r="EG40" s="36"/>
+      <c r="EH40" s="36"/>
+      <c r="EI40" s="36"/>
+      <c r="EJ40" s="36"/>
+      <c r="EK40" s="36"/>
+      <c r="EL40" s="36"/>
+      <c r="EM40" s="36"/>
+      <c r="EN40" s="36"/>
+      <c r="EO40" s="36"/>
+      <c r="EP40" s="36"/>
+      <c r="EQ40" s="36"/>
+      <c r="ER40" s="36"/>
+      <c r="ES40" s="36"/>
+      <c r="ET40" s="36"/>
+      <c r="EU40" s="36"/>
+      <c r="EV40" s="36"/>
+      <c r="EW40" s="36"/>
+      <c r="EX40" s="36"/>
+      <c r="EY40" s="36"/>
+      <c r="EZ40" s="36"/>
+      <c r="FA40" s="36"/>
+      <c r="FB40" s="36"/>
+      <c r="FC40" s="36"/>
+      <c r="FD40" s="36"/>
+      <c r="FE40" s="36"/>
     </row>
-    <row r="33" spans="1:161" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AH33" s="37" t="s">
+    <row r="41" spans="1:161" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH41" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="AI33" s="37"/>
-      <c r="AJ33" s="37"/>
-      <c r="AK33" s="37"/>
-      <c r="AL33" s="37"/>
-      <c r="AM33" s="37"/>
-      <c r="AN33" s="37"/>
-      <c r="AO33" s="37"/>
-      <c r="AP33" s="37"/>
-      <c r="AQ33" s="37"/>
-      <c r="AR33" s="37"/>
-      <c r="AS33" s="37"/>
-      <c r="AT33" s="37"/>
-      <c r="AU33" s="37"/>
-      <c r="AV33" s="37"/>
-      <c r="AW33" s="37"/>
-      <c r="AX33" s="6"/>
-      <c r="AY33" s="6"/>
-      <c r="AZ33" s="37" t="s">
+      <c r="AI41" s="37"/>
+      <c r="AJ41" s="37"/>
+      <c r="AK41" s="37"/>
+      <c r="AL41" s="37"/>
+      <c r="AM41" s="37"/>
+      <c r="AN41" s="37"/>
+      <c r="AO41" s="37"/>
+      <c r="AP41" s="37"/>
+      <c r="AQ41" s="37"/>
+      <c r="AR41" s="37"/>
+      <c r="AS41" s="37"/>
+      <c r="AT41" s="37"/>
+      <c r="AU41" s="37"/>
+      <c r="AV41" s="37"/>
+      <c r="AW41" s="37"/>
+      <c r="AX41" s="6"/>
+      <c r="AY41" s="6"/>
+      <c r="AZ41" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="BA33" s="37"/>
-      <c r="BB33" s="37"/>
-      <c r="BC33" s="37"/>
-      <c r="BD33" s="37"/>
-      <c r="BE33" s="37"/>
-      <c r="BF33" s="37"/>
-      <c r="BG33" s="37"/>
-      <c r="BH33" s="37"/>
-      <c r="BI33" s="37"/>
-      <c r="BJ33" s="37"/>
-      <c r="BK33" s="37"/>
-      <c r="BL33" s="37"/>
-      <c r="BM33" s="37"/>
-      <c r="BN33" s="37"/>
-      <c r="BO33" s="37"/>
-      <c r="BP33" s="37"/>
-      <c r="BQ33" s="37"/>
-      <c r="BR33" s="37"/>
-      <c r="BS33" s="37"/>
-      <c r="BT33" s="37"/>
-      <c r="BU33" s="37"/>
-      <c r="BV33" s="37"/>
-      <c r="BW33" s="37"/>
-      <c r="BX33" s="37"/>
-      <c r="BY33" s="37"/>
-      <c r="BZ33" s="37"/>
-      <c r="CA33" s="37"/>
-      <c r="CB33" s="37"/>
-      <c r="DK33" s="37" t="s">
+      <c r="BA41" s="37"/>
+      <c r="BB41" s="37"/>
+      <c r="BC41" s="37"/>
+      <c r="BD41" s="37"/>
+      <c r="BE41" s="37"/>
+      <c r="BF41" s="37"/>
+      <c r="BG41" s="37"/>
+      <c r="BH41" s="37"/>
+      <c r="BI41" s="37"/>
+      <c r="BJ41" s="37"/>
+      <c r="BK41" s="37"/>
+      <c r="BL41" s="37"/>
+      <c r="BM41" s="37"/>
+      <c r="BN41" s="37"/>
+      <c r="BO41" s="37"/>
+      <c r="BP41" s="37"/>
+      <c r="BQ41" s="37"/>
+      <c r="BR41" s="37"/>
+      <c r="BS41" s="37"/>
+      <c r="BT41" s="37"/>
+      <c r="BU41" s="37"/>
+      <c r="BV41" s="37"/>
+      <c r="BW41" s="37"/>
+      <c r="BX41" s="37"/>
+      <c r="BY41" s="37"/>
+      <c r="BZ41" s="37"/>
+      <c r="CA41" s="37"/>
+      <c r="CB41" s="37"/>
+      <c r="DK41" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="DL33" s="37"/>
-      <c r="DM33" s="37"/>
-      <c r="DN33" s="37"/>
-      <c r="DO33" s="37"/>
-      <c r="DP33" s="37"/>
-      <c r="DQ33" s="37"/>
-      <c r="DR33" s="37"/>
-      <c r="DS33" s="37"/>
-      <c r="DT33" s="37"/>
-      <c r="DU33" s="37"/>
-      <c r="DV33" s="37"/>
-      <c r="DW33" s="37"/>
-      <c r="DX33" s="37"/>
-      <c r="DY33" s="37"/>
-      <c r="DZ33" s="37"/>
-      <c r="EA33" s="6"/>
-      <c r="EB33" s="6"/>
-      <c r="EC33" s="37" t="s">
+      <c r="DL41" s="37"/>
+      <c r="DM41" s="37"/>
+      <c r="DN41" s="37"/>
+      <c r="DO41" s="37"/>
+      <c r="DP41" s="37"/>
+      <c r="DQ41" s="37"/>
+      <c r="DR41" s="37"/>
+      <c r="DS41" s="37"/>
+      <c r="DT41" s="37"/>
+      <c r="DU41" s="37"/>
+      <c r="DV41" s="37"/>
+      <c r="DW41" s="37"/>
+      <c r="DX41" s="37"/>
+      <c r="DY41" s="37"/>
+      <c r="DZ41" s="37"/>
+      <c r="EA41" s="6"/>
+      <c r="EB41" s="6"/>
+      <c r="EC41" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="ED33" s="37"/>
-      <c r="EE33" s="37"/>
-      <c r="EF33" s="37"/>
-      <c r="EG33" s="37"/>
-      <c r="EH33" s="37"/>
-      <c r="EI33" s="37"/>
-      <c r="EJ33" s="37"/>
-      <c r="EK33" s="37"/>
-      <c r="EL33" s="37"/>
-      <c r="EM33" s="37"/>
-      <c r="EN33" s="37"/>
-      <c r="EO33" s="37"/>
-      <c r="EP33" s="37"/>
-      <c r="EQ33" s="37"/>
-      <c r="ER33" s="37"/>
-      <c r="ES33" s="37"/>
-      <c r="ET33" s="37"/>
-      <c r="EU33" s="37"/>
-      <c r="EV33" s="37"/>
-      <c r="EW33" s="37"/>
-      <c r="EX33" s="37"/>
-      <c r="EY33" s="37"/>
-      <c r="EZ33" s="37"/>
-      <c r="FA33" s="37"/>
-      <c r="FB33" s="37"/>
-      <c r="FC33" s="37"/>
-      <c r="FD33" s="37"/>
-      <c r="FE33" s="37"/>
+      <c r="ED41" s="37"/>
+      <c r="EE41" s="37"/>
+      <c r="EF41" s="37"/>
+      <c r="EG41" s="37"/>
+      <c r="EH41" s="37"/>
+      <c r="EI41" s="37"/>
+      <c r="EJ41" s="37"/>
+      <c r="EK41" s="37"/>
+      <c r="EL41" s="37"/>
+      <c r="EM41" s="37"/>
+      <c r="EN41" s="37"/>
+      <c r="EO41" s="37"/>
+      <c r="EP41" s="37"/>
+      <c r="EQ41" s="37"/>
+      <c r="ER41" s="37"/>
+      <c r="ES41" s="37"/>
+      <c r="ET41" s="37"/>
+      <c r="EU41" s="37"/>
+      <c r="EV41" s="37"/>
+      <c r="EW41" s="37"/>
+      <c r="EX41" s="37"/>
+      <c r="EY41" s="37"/>
+      <c r="EZ41" s="37"/>
+      <c r="FA41" s="37"/>
+      <c r="FB41" s="37"/>
+      <c r="FC41" s="37"/>
+      <c r="FD41" s="37"/>
+      <c r="FE41" s="37"/>
     </row>
-    <row r="34" spans="1:161" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    <row r="42" spans="1:161" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:161" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+    <row r="43" spans="1:161" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AM35" s="36"/>
-      <c r="AN35" s="36"/>
-      <c r="AO35" s="36"/>
-      <c r="AP35" s="36"/>
-      <c r="AQ35" s="36"/>
-      <c r="AR35" s="36"/>
-      <c r="AS35" s="36"/>
-      <c r="AT35" s="36"/>
-      <c r="AU35" s="36"/>
-      <c r="AV35" s="36"/>
-      <c r="AW35" s="36"/>
-      <c r="AX35" s="36"/>
-      <c r="AY35" s="36"/>
-      <c r="AZ35" s="36"/>
-      <c r="BA35" s="36"/>
-      <c r="BB35" s="36"/>
-      <c r="BE35" s="36"/>
-      <c r="BF35" s="36"/>
-      <c r="BG35" s="36"/>
-      <c r="BH35" s="36"/>
-      <c r="BI35" s="36"/>
-      <c r="BJ35" s="36"/>
-      <c r="BK35" s="36"/>
-      <c r="BL35" s="36"/>
-      <c r="BM35" s="36"/>
-      <c r="BN35" s="36"/>
-      <c r="BO35" s="36"/>
-      <c r="BP35" s="36"/>
-      <c r="BQ35" s="36"/>
-      <c r="BR35" s="36"/>
-      <c r="BS35" s="36"/>
-      <c r="BT35" s="36"/>
-      <c r="BU35" s="36"/>
-      <c r="BV35" s="36"/>
-      <c r="BW35" s="36"/>
-      <c r="BX35" s="36"/>
-      <c r="BY35" s="36"/>
-      <c r="BZ35" s="36"/>
-      <c r="CA35" s="36"/>
-      <c r="CB35" s="36"/>
-      <c r="CC35" s="36"/>
-      <c r="CD35" s="36"/>
-      <c r="CE35" s="36"/>
-      <c r="CF35" s="36"/>
-      <c r="CG35" s="36"/>
-      <c r="CI35" s="38"/>
-      <c r="CJ35" s="38"/>
-      <c r="CK35" s="38"/>
-      <c r="CL35" s="38"/>
-      <c r="CM35" s="38"/>
-      <c r="CN35" s="38"/>
-      <c r="CO35" s="38"/>
-      <c r="CP35" s="38"/>
-      <c r="CQ35" s="38"/>
-      <c r="CR35" s="38"/>
-      <c r="CS35" s="38"/>
-      <c r="CT35" s="38"/>
-      <c r="CU35" s="38"/>
-      <c r="CV35" s="38"/>
-      <c r="CW35" s="38"/>
-      <c r="CX35" s="38"/>
-      <c r="CY35" s="38"/>
-      <c r="CZ35" s="38"/>
-      <c r="DA35" s="38"/>
-      <c r="DB35" s="38"/>
-      <c r="DC35" s="38"/>
-      <c r="DD35" s="38"/>
-      <c r="DE35" s="38"/>
-      <c r="DF35" s="38"/>
-      <c r="DG35" s="38"/>
-      <c r="DH35" s="38"/>
-      <c r="DI35" s="38"/>
-      <c r="DJ35" s="38"/>
-      <c r="DK35" s="38"/>
-      <c r="DL35" s="38"/>
-      <c r="DM35" s="38"/>
-      <c r="DN35" s="38"/>
-      <c r="DO35" s="38"/>
-      <c r="DP35" s="38"/>
-      <c r="DQ35" s="38"/>
-      <c r="DR35" s="38"/>
-      <c r="DS35" s="38"/>
-      <c r="DT35" s="38"/>
-      <c r="DU35" s="38"/>
-      <c r="DV35" s="38"/>
-      <c r="DW35" s="38"/>
-      <c r="DX35" s="38"/>
-      <c r="DY35" s="38"/>
-      <c r="DZ35" s="38"/>
-      <c r="EA35" s="38"/>
-      <c r="EB35" s="38"/>
-      <c r="EC35" s="38"/>
-      <c r="ED35" s="38"/>
-      <c r="EE35" s="38"/>
-      <c r="EF35" s="38"/>
-      <c r="EG35" s="38"/>
-      <c r="EH35" s="38"/>
-      <c r="EI35" s="38"/>
-      <c r="EJ35" s="38"/>
-      <c r="EK35" s="38"/>
-      <c r="EL35" s="38"/>
-      <c r="EM35" s="38"/>
-      <c r="EN35" s="38"/>
-      <c r="EO35" s="38"/>
-      <c r="EP35" s="38"/>
-      <c r="EQ35" s="38"/>
-      <c r="ER35" s="38"/>
-      <c r="ES35" s="38"/>
-      <c r="ET35" s="38"/>
-      <c r="EU35" s="38"/>
-      <c r="EV35" s="38"/>
-      <c r="EW35" s="38"/>
-      <c r="EX35" s="38"/>
-      <c r="EY35" s="38"/>
-      <c r="EZ35" s="38"/>
-      <c r="FA35" s="38"/>
-      <c r="FB35" s="38"/>
-      <c r="FC35" s="38"/>
-      <c r="FD35" s="38"/>
-      <c r="FE35" s="38"/>
+      <c r="AM43" s="36"/>
+      <c r="AN43" s="36"/>
+      <c r="AO43" s="36"/>
+      <c r="AP43" s="36"/>
+      <c r="AQ43" s="36"/>
+      <c r="AR43" s="36"/>
+      <c r="AS43" s="36"/>
+      <c r="AT43" s="36"/>
+      <c r="AU43" s="36"/>
+      <c r="AV43" s="36"/>
+      <c r="AW43" s="36"/>
+      <c r="AX43" s="36"/>
+      <c r="AY43" s="36"/>
+      <c r="AZ43" s="36"/>
+      <c r="BA43" s="36"/>
+      <c r="BB43" s="36"/>
+      <c r="BE43" s="36"/>
+      <c r="BF43" s="36"/>
+      <c r="BG43" s="36"/>
+      <c r="BH43" s="36"/>
+      <c r="BI43" s="36"/>
+      <c r="BJ43" s="36"/>
+      <c r="BK43" s="36"/>
+      <c r="BL43" s="36"/>
+      <c r="BM43" s="36"/>
+      <c r="BN43" s="36"/>
+      <c r="BO43" s="36"/>
+      <c r="BP43" s="36"/>
+      <c r="BQ43" s="36"/>
+      <c r="BR43" s="36"/>
+      <c r="BS43" s="36"/>
+      <c r="BT43" s="36"/>
+      <c r="BU43" s="36"/>
+      <c r="BV43" s="36"/>
+      <c r="BW43" s="36"/>
+      <c r="BX43" s="36"/>
+      <c r="BY43" s="36"/>
+      <c r="BZ43" s="36"/>
+      <c r="CA43" s="36"/>
+      <c r="CB43" s="36"/>
+      <c r="CC43" s="36"/>
+      <c r="CD43" s="36"/>
+      <c r="CE43" s="36"/>
+      <c r="CF43" s="36"/>
+      <c r="CG43" s="36"/>
+      <c r="CI43" s="38"/>
+      <c r="CJ43" s="38"/>
+      <c r="CK43" s="38"/>
+      <c r="CL43" s="38"/>
+      <c r="CM43" s="38"/>
+      <c r="CN43" s="38"/>
+      <c r="CO43" s="38"/>
+      <c r="CP43" s="38"/>
+      <c r="CQ43" s="38"/>
+      <c r="CR43" s="38"/>
+      <c r="CS43" s="38"/>
+      <c r="CT43" s="38"/>
+      <c r="CU43" s="38"/>
+      <c r="CV43" s="38"/>
+      <c r="CW43" s="38"/>
+      <c r="CX43" s="38"/>
+      <c r="CY43" s="38"/>
+      <c r="CZ43" s="38"/>
+      <c r="DA43" s="38"/>
+      <c r="DB43" s="38"/>
+      <c r="DC43" s="38"/>
+      <c r="DD43" s="38"/>
+      <c r="DE43" s="38"/>
+      <c r="DF43" s="38"/>
+      <c r="DG43" s="38"/>
+      <c r="DH43" s="38"/>
+      <c r="DI43" s="38"/>
+      <c r="DJ43" s="38"/>
+      <c r="DK43" s="38"/>
+      <c r="DL43" s="38"/>
+      <c r="DM43" s="38"/>
+      <c r="DN43" s="38"/>
+      <c r="DO43" s="38"/>
+      <c r="DP43" s="38"/>
+      <c r="DQ43" s="38"/>
+      <c r="DR43" s="38"/>
+      <c r="DS43" s="38"/>
+      <c r="DT43" s="38"/>
+      <c r="DU43" s="38"/>
+      <c r="DV43" s="38"/>
+      <c r="DW43" s="38"/>
+      <c r="DX43" s="38"/>
+      <c r="DY43" s="38"/>
+      <c r="DZ43" s="38"/>
+      <c r="EA43" s="38"/>
+      <c r="EB43" s="38"/>
+      <c r="EC43" s="38"/>
+      <c r="ED43" s="38"/>
+      <c r="EE43" s="38"/>
+      <c r="EF43" s="38"/>
+      <c r="EG43" s="38"/>
+      <c r="EH43" s="38"/>
+      <c r="EI43" s="38"/>
+      <c r="EJ43" s="38"/>
+      <c r="EK43" s="38"/>
+      <c r="EL43" s="38"/>
+      <c r="EM43" s="38"/>
+      <c r="EN43" s="38"/>
+      <c r="EO43" s="38"/>
+      <c r="EP43" s="38"/>
+      <c r="EQ43" s="38"/>
+      <c r="ER43" s="38"/>
+      <c r="ES43" s="38"/>
+      <c r="ET43" s="38"/>
+      <c r="EU43" s="38"/>
+      <c r="EV43" s="38"/>
+      <c r="EW43" s="38"/>
+      <c r="EX43" s="38"/>
+      <c r="EY43" s="38"/>
+      <c r="EZ43" s="38"/>
+      <c r="FA43" s="38"/>
+      <c r="FB43" s="38"/>
+      <c r="FC43" s="38"/>
+      <c r="FD43" s="38"/>
+      <c r="FE43" s="38"/>
     </row>
-    <row r="36" spans="1:161" s="7" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AM36" s="37" t="s">
+    <row r="44" spans="1:161" s="7" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AM44" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="AN36" s="37"/>
-      <c r="AO36" s="37"/>
-      <c r="AP36" s="37"/>
-      <c r="AQ36" s="37"/>
-      <c r="AR36" s="37"/>
-      <c r="AS36" s="37"/>
-      <c r="AT36" s="37"/>
-      <c r="AU36" s="37"/>
-      <c r="AV36" s="37"/>
-      <c r="AW36" s="37"/>
-      <c r="AX36" s="37"/>
-      <c r="AY36" s="37"/>
-      <c r="AZ36" s="37"/>
-      <c r="BA36" s="37"/>
-      <c r="BB36" s="37"/>
-      <c r="BC36" s="6"/>
-      <c r="BD36" s="6"/>
-      <c r="BE36" s="37" t="s">
+      <c r="AN44" s="37"/>
+      <c r="AO44" s="37"/>
+      <c r="AP44" s="37"/>
+      <c r="AQ44" s="37"/>
+      <c r="AR44" s="37"/>
+      <c r="AS44" s="37"/>
+      <c r="AT44" s="37"/>
+      <c r="AU44" s="37"/>
+      <c r="AV44" s="37"/>
+      <c r="AW44" s="37"/>
+      <c r="AX44" s="37"/>
+      <c r="AY44" s="37"/>
+      <c r="AZ44" s="37"/>
+      <c r="BA44" s="37"/>
+      <c r="BB44" s="37"/>
+      <c r="BC44" s="6"/>
+      <c r="BD44" s="6"/>
+      <c r="BE44" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="BF36" s="37"/>
-      <c r="BG36" s="37"/>
-      <c r="BH36" s="37"/>
-      <c r="BI36" s="37"/>
-      <c r="BJ36" s="37"/>
-      <c r="BK36" s="37"/>
-      <c r="BL36" s="37"/>
-      <c r="BM36" s="37"/>
-      <c r="BN36" s="37"/>
-      <c r="BO36" s="37"/>
-      <c r="BP36" s="37"/>
-      <c r="BQ36" s="37"/>
-      <c r="BR36" s="37"/>
-      <c r="BS36" s="37"/>
-      <c r="BT36" s="37"/>
-      <c r="BU36" s="37"/>
-      <c r="BV36" s="37"/>
-      <c r="BW36" s="37"/>
-      <c r="BX36" s="37"/>
-      <c r="BY36" s="37"/>
-      <c r="BZ36" s="37"/>
-      <c r="CA36" s="37"/>
-      <c r="CB36" s="37"/>
-      <c r="CC36" s="37"/>
-      <c r="CD36" s="37"/>
-      <c r="CE36" s="37"/>
-      <c r="CF36" s="37"/>
-      <c r="CG36" s="37"/>
-      <c r="CI36" s="35" t="s">
+      <c r="BF44" s="37"/>
+      <c r="BG44" s="37"/>
+      <c r="BH44" s="37"/>
+      <c r="BI44" s="37"/>
+      <c r="BJ44" s="37"/>
+      <c r="BK44" s="37"/>
+      <c r="BL44" s="37"/>
+      <c r="BM44" s="37"/>
+      <c r="BN44" s="37"/>
+      <c r="BO44" s="37"/>
+      <c r="BP44" s="37"/>
+      <c r="BQ44" s="37"/>
+      <c r="BR44" s="37"/>
+      <c r="BS44" s="37"/>
+      <c r="BT44" s="37"/>
+      <c r="BU44" s="37"/>
+      <c r="BV44" s="37"/>
+      <c r="BW44" s="37"/>
+      <c r="BX44" s="37"/>
+      <c r="BY44" s="37"/>
+      <c r="BZ44" s="37"/>
+      <c r="CA44" s="37"/>
+      <c r="CB44" s="37"/>
+      <c r="CC44" s="37"/>
+      <c r="CD44" s="37"/>
+      <c r="CE44" s="37"/>
+      <c r="CF44" s="37"/>
+      <c r="CG44" s="37"/>
+      <c r="CI44" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="CJ36" s="35"/>
-      <c r="CK36" s="35"/>
-      <c r="CL36" s="35"/>
-      <c r="CM36" s="35"/>
-      <c r="CN36" s="35"/>
-      <c r="CO36" s="35"/>
-      <c r="CP36" s="35"/>
-      <c r="CQ36" s="35"/>
-      <c r="CR36" s="35"/>
-      <c r="CS36" s="35"/>
-      <c r="CT36" s="35"/>
-      <c r="CU36" s="35"/>
-      <c r="CV36" s="35"/>
-      <c r="CW36" s="35"/>
-      <c r="CX36" s="35"/>
-      <c r="CY36" s="35"/>
-      <c r="CZ36" s="35"/>
-      <c r="DA36" s="35"/>
-      <c r="DB36" s="35"/>
-      <c r="DC36" s="35"/>
-      <c r="DD36" s="35"/>
-      <c r="DE36" s="35"/>
-      <c r="DF36" s="35"/>
-      <c r="DG36" s="35"/>
-      <c r="DH36" s="35"/>
-      <c r="DI36" s="35"/>
-      <c r="DJ36" s="35"/>
-      <c r="DK36" s="35"/>
-      <c r="DL36" s="35"/>
-      <c r="DM36" s="35"/>
-      <c r="DN36" s="35"/>
-      <c r="DO36" s="35"/>
-      <c r="DP36" s="35"/>
-      <c r="DQ36" s="35"/>
-      <c r="DR36" s="35"/>
-      <c r="DS36" s="35"/>
-      <c r="DT36" s="35"/>
-      <c r="DU36" s="35"/>
-      <c r="DV36" s="35"/>
-      <c r="DW36" s="35"/>
-      <c r="DX36" s="35"/>
-      <c r="DY36" s="35"/>
-      <c r="DZ36" s="35"/>
-      <c r="EA36" s="35"/>
-      <c r="EB36" s="35"/>
-      <c r="EC36" s="35"/>
-      <c r="ED36" s="35"/>
-      <c r="EE36" s="35"/>
-      <c r="EF36" s="35"/>
-      <c r="EG36" s="35"/>
-      <c r="EH36" s="35"/>
-      <c r="EI36" s="35"/>
-      <c r="EJ36" s="35"/>
-      <c r="EK36" s="35"/>
-      <c r="EL36" s="35"/>
-      <c r="EM36" s="35"/>
-      <c r="EN36" s="35"/>
-      <c r="EO36" s="35"/>
-      <c r="EP36" s="35"/>
-      <c r="EQ36" s="35"/>
-      <c r="ER36" s="35"/>
-      <c r="ES36" s="35"/>
-      <c r="ET36" s="35"/>
-      <c r="EU36" s="35"/>
-      <c r="EV36" s="35"/>
-      <c r="EW36" s="35"/>
-      <c r="EX36" s="35"/>
-      <c r="EY36" s="35"/>
-      <c r="EZ36" s="35"/>
-      <c r="FA36" s="35"/>
-      <c r="FB36" s="35"/>
-      <c r="FC36" s="35"/>
-      <c r="FD36" s="35"/>
-      <c r="FE36" s="35"/>
+      <c r="CJ44" s="35"/>
+      <c r="CK44" s="35"/>
+      <c r="CL44" s="35"/>
+      <c r="CM44" s="35"/>
+      <c r="CN44" s="35"/>
+      <c r="CO44" s="35"/>
+      <c r="CP44" s="35"/>
+      <c r="CQ44" s="35"/>
+      <c r="CR44" s="35"/>
+      <c r="CS44" s="35"/>
+      <c r="CT44" s="35"/>
+      <c r="CU44" s="35"/>
+      <c r="CV44" s="35"/>
+      <c r="CW44" s="35"/>
+      <c r="CX44" s="35"/>
+      <c r="CY44" s="35"/>
+      <c r="CZ44" s="35"/>
+      <c r="DA44" s="35"/>
+      <c r="DB44" s="35"/>
+      <c r="DC44" s="35"/>
+      <c r="DD44" s="35"/>
+      <c r="DE44" s="35"/>
+      <c r="DF44" s="35"/>
+      <c r="DG44" s="35"/>
+      <c r="DH44" s="35"/>
+      <c r="DI44" s="35"/>
+      <c r="DJ44" s="35"/>
+      <c r="DK44" s="35"/>
+      <c r="DL44" s="35"/>
+      <c r="DM44" s="35"/>
+      <c r="DN44" s="35"/>
+      <c r="DO44" s="35"/>
+      <c r="DP44" s="35"/>
+      <c r="DQ44" s="35"/>
+      <c r="DR44" s="35"/>
+      <c r="DS44" s="35"/>
+      <c r="DT44" s="35"/>
+      <c r="DU44" s="35"/>
+      <c r="DV44" s="35"/>
+      <c r="DW44" s="35"/>
+      <c r="DX44" s="35"/>
+      <c r="DY44" s="35"/>
+      <c r="DZ44" s="35"/>
+      <c r="EA44" s="35"/>
+      <c r="EB44" s="35"/>
+      <c r="EC44" s="35"/>
+      <c r="ED44" s="35"/>
+      <c r="EE44" s="35"/>
+      <c r="EF44" s="35"/>
+      <c r="EG44" s="35"/>
+      <c r="EH44" s="35"/>
+      <c r="EI44" s="35"/>
+      <c r="EJ44" s="35"/>
+      <c r="EK44" s="35"/>
+      <c r="EL44" s="35"/>
+      <c r="EM44" s="35"/>
+      <c r="EN44" s="35"/>
+      <c r="EO44" s="35"/>
+      <c r="EP44" s="35"/>
+      <c r="EQ44" s="35"/>
+      <c r="ER44" s="35"/>
+      <c r="ES44" s="35"/>
+      <c r="ET44" s="35"/>
+      <c r="EU44" s="35"/>
+      <c r="EV44" s="35"/>
+      <c r="EW44" s="35"/>
+      <c r="EX44" s="35"/>
+      <c r="EY44" s="35"/>
+      <c r="EZ44" s="35"/>
+      <c r="FA44" s="35"/>
+      <c r="FB44" s="35"/>
+      <c r="FC44" s="35"/>
+      <c r="FD44" s="35"/>
+      <c r="FE44" s="35"/>
     </row>
-    <row r="37" spans="1:161" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:161" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="124">
+  <mergeCells count="236">
+    <mergeCell ref="EG34:ES34"/>
+    <mergeCell ref="ET34:FE34"/>
+    <mergeCell ref="A35:T35"/>
+    <mergeCell ref="U35:AB35"/>
+    <mergeCell ref="AC35:AH35"/>
+    <mergeCell ref="AI35:AS35"/>
+    <mergeCell ref="AT35:BA35"/>
+    <mergeCell ref="BB35:BL35"/>
+    <mergeCell ref="BM35:CA35"/>
+    <mergeCell ref="CB35:CK35"/>
+    <mergeCell ref="CL35:CU35"/>
+    <mergeCell ref="CV35:DG35"/>
+    <mergeCell ref="DH35:DV35"/>
+    <mergeCell ref="DW35:EF35"/>
+    <mergeCell ref="EG35:ES35"/>
+    <mergeCell ref="ET35:FE35"/>
+    <mergeCell ref="DH33:DV33"/>
+    <mergeCell ref="DW33:EF33"/>
+    <mergeCell ref="EG33:ES33"/>
+    <mergeCell ref="ET33:FE33"/>
+    <mergeCell ref="A34:T34"/>
+    <mergeCell ref="U34:AB34"/>
+    <mergeCell ref="AC34:AH34"/>
+    <mergeCell ref="AI34:AS34"/>
+    <mergeCell ref="AT34:BA34"/>
+    <mergeCell ref="BB34:BL34"/>
+    <mergeCell ref="BM34:CA34"/>
+    <mergeCell ref="CB34:CK34"/>
+    <mergeCell ref="CL34:CU34"/>
+    <mergeCell ref="CV34:DG34"/>
+    <mergeCell ref="DH34:DV34"/>
+    <mergeCell ref="DW34:EF34"/>
+    <mergeCell ref="BB33:BL33"/>
+    <mergeCell ref="BM33:CA33"/>
+    <mergeCell ref="CB33:CK33"/>
+    <mergeCell ref="CL33:CU33"/>
+    <mergeCell ref="CV33:DG33"/>
+    <mergeCell ref="A33:T33"/>
+    <mergeCell ref="U33:AB33"/>
+    <mergeCell ref="AC33:AH33"/>
+    <mergeCell ref="AI33:AS33"/>
+    <mergeCell ref="AT33:BA33"/>
+    <mergeCell ref="EG31:ES31"/>
+    <mergeCell ref="ET31:FE31"/>
+    <mergeCell ref="A32:T32"/>
+    <mergeCell ref="U32:AB32"/>
+    <mergeCell ref="AC32:AH32"/>
+    <mergeCell ref="AI32:AS32"/>
+    <mergeCell ref="AT32:BA32"/>
+    <mergeCell ref="BB32:BL32"/>
+    <mergeCell ref="BM32:CA32"/>
+    <mergeCell ref="CB32:CK32"/>
+    <mergeCell ref="CL32:CU32"/>
+    <mergeCell ref="CV32:DG32"/>
+    <mergeCell ref="DH32:DV32"/>
+    <mergeCell ref="DW32:EF32"/>
+    <mergeCell ref="EG32:ES32"/>
+    <mergeCell ref="ET32:FE32"/>
+    <mergeCell ref="DH30:DV30"/>
+    <mergeCell ref="DW30:EF30"/>
+    <mergeCell ref="EG30:ES30"/>
+    <mergeCell ref="ET30:FE30"/>
+    <mergeCell ref="A31:T31"/>
+    <mergeCell ref="U31:AB31"/>
+    <mergeCell ref="AC31:AH31"/>
+    <mergeCell ref="AI31:AS31"/>
+    <mergeCell ref="AT31:BA31"/>
+    <mergeCell ref="BB31:BL31"/>
+    <mergeCell ref="BM31:CA31"/>
+    <mergeCell ref="CB31:CK31"/>
+    <mergeCell ref="CL31:CU31"/>
+    <mergeCell ref="CV31:DG31"/>
+    <mergeCell ref="DH31:DV31"/>
+    <mergeCell ref="DW31:EF31"/>
+    <mergeCell ref="BB30:BL30"/>
+    <mergeCell ref="BM30:CA30"/>
+    <mergeCell ref="CB30:CK30"/>
+    <mergeCell ref="CL30:CU30"/>
+    <mergeCell ref="CV30:DG30"/>
+    <mergeCell ref="A30:T30"/>
+    <mergeCell ref="U30:AB30"/>
+    <mergeCell ref="AC30:AH30"/>
+    <mergeCell ref="AI30:AS30"/>
+    <mergeCell ref="AT30:BA30"/>
+    <mergeCell ref="EG28:ES28"/>
+    <mergeCell ref="ET28:FE28"/>
+    <mergeCell ref="A29:T29"/>
+    <mergeCell ref="U29:AB29"/>
+    <mergeCell ref="AC29:AH29"/>
+    <mergeCell ref="AI29:AS29"/>
+    <mergeCell ref="AT29:BA29"/>
+    <mergeCell ref="BB29:BL29"/>
+    <mergeCell ref="BM29:CA29"/>
+    <mergeCell ref="CB29:CK29"/>
+    <mergeCell ref="CL29:CU29"/>
+    <mergeCell ref="CV29:DG29"/>
+    <mergeCell ref="DH29:DV29"/>
+    <mergeCell ref="DW29:EF29"/>
+    <mergeCell ref="EG29:ES29"/>
+    <mergeCell ref="ET29:FE29"/>
     <mergeCell ref="DH27:DV27"/>
     <mergeCell ref="DW27:EF27"/>
     <mergeCell ref="EG27:ES27"/>
     <mergeCell ref="ET27:FE27"/>
+    <mergeCell ref="A28:T28"/>
+    <mergeCell ref="U28:AB28"/>
+    <mergeCell ref="AC28:AH28"/>
+    <mergeCell ref="AI28:AS28"/>
+    <mergeCell ref="AT28:BA28"/>
+    <mergeCell ref="BB28:BL28"/>
+    <mergeCell ref="BM28:CA28"/>
+    <mergeCell ref="CB28:CK28"/>
+    <mergeCell ref="CL28:CU28"/>
+    <mergeCell ref="CV28:DG28"/>
+    <mergeCell ref="DH28:DV28"/>
+    <mergeCell ref="DW28:EF28"/>
     <mergeCell ref="BB27:BL27"/>
     <mergeCell ref="BM27:CA27"/>
     <mergeCell ref="CB27:CK27"/>
@@ -5289,16 +6812,16 @@
     <mergeCell ref="CV24:DG24"/>
     <mergeCell ref="AI24:AS24"/>
     <mergeCell ref="AT24:BA24"/>
-    <mergeCell ref="AZ32:CB32"/>
-    <mergeCell ref="AZ33:CB33"/>
+    <mergeCell ref="AZ40:CB40"/>
+    <mergeCell ref="AZ41:CB41"/>
     <mergeCell ref="A20:CO20"/>
     <mergeCell ref="CP20:EZ20"/>
-    <mergeCell ref="DK32:DZ32"/>
-    <mergeCell ref="EC32:FE32"/>
-    <mergeCell ref="DK33:DZ33"/>
-    <mergeCell ref="EC33:FE33"/>
-    <mergeCell ref="AH32:AW32"/>
-    <mergeCell ref="AH33:AW33"/>
+    <mergeCell ref="DK40:DZ40"/>
+    <mergeCell ref="EC40:FE40"/>
+    <mergeCell ref="DK41:DZ41"/>
+    <mergeCell ref="EC41:FE41"/>
+    <mergeCell ref="AH40:AW40"/>
+    <mergeCell ref="AH41:AW41"/>
     <mergeCell ref="DW23:EF23"/>
     <mergeCell ref="EG23:ES23"/>
     <mergeCell ref="BB22:BL23"/>
@@ -5316,11 +6839,11 @@
     <mergeCell ref="BM24:CA24"/>
     <mergeCell ref="CB24:CK24"/>
     <mergeCell ref="A24:T24"/>
-    <mergeCell ref="DH29:DV29"/>
-    <mergeCell ref="A29:BL29"/>
-    <mergeCell ref="BM29:CA29"/>
-    <mergeCell ref="CB29:CU29"/>
-    <mergeCell ref="CV29:DG29"/>
+    <mergeCell ref="DH37:DV37"/>
+    <mergeCell ref="A37:BL37"/>
+    <mergeCell ref="BM37:CA37"/>
+    <mergeCell ref="CB37:CU37"/>
+    <mergeCell ref="CV37:DG37"/>
     <mergeCell ref="A25:T25"/>
     <mergeCell ref="U25:AB25"/>
     <mergeCell ref="AC25:AH25"/>
@@ -5334,26 +6857,26 @@
     <mergeCell ref="AT22:BA23"/>
     <mergeCell ref="AC23:AH23"/>
     <mergeCell ref="AI23:AS23"/>
-    <mergeCell ref="CI36:FE36"/>
-    <mergeCell ref="AM35:BB35"/>
-    <mergeCell ref="BE35:CG35"/>
-    <mergeCell ref="AM36:BB36"/>
-    <mergeCell ref="BE36:CG36"/>
-    <mergeCell ref="CI35:FE35"/>
-    <mergeCell ref="ET28:FE28"/>
-    <mergeCell ref="A28:T28"/>
-    <mergeCell ref="U28:AB28"/>
-    <mergeCell ref="AC28:AH28"/>
-    <mergeCell ref="AI28:AS28"/>
-    <mergeCell ref="CL28:CU28"/>
-    <mergeCell ref="CV28:DG28"/>
-    <mergeCell ref="DH28:DV28"/>
-    <mergeCell ref="DW28:EF28"/>
-    <mergeCell ref="EG28:ES28"/>
-    <mergeCell ref="AT28:BA28"/>
-    <mergeCell ref="BB28:BL28"/>
-    <mergeCell ref="BM28:CA28"/>
-    <mergeCell ref="CB28:CK28"/>
+    <mergeCell ref="CI44:FE44"/>
+    <mergeCell ref="AM43:BB43"/>
+    <mergeCell ref="BE43:CG43"/>
+    <mergeCell ref="AM44:BB44"/>
+    <mergeCell ref="BE44:CG44"/>
+    <mergeCell ref="CI43:FE43"/>
+    <mergeCell ref="ET36:FE36"/>
+    <mergeCell ref="A36:T36"/>
+    <mergeCell ref="U36:AB36"/>
+    <mergeCell ref="AC36:AH36"/>
+    <mergeCell ref="AI36:AS36"/>
+    <mergeCell ref="CL36:CU36"/>
+    <mergeCell ref="CV36:DG36"/>
+    <mergeCell ref="DH36:DV36"/>
+    <mergeCell ref="DW36:EF36"/>
+    <mergeCell ref="EG36:ES36"/>
+    <mergeCell ref="AT36:BA36"/>
+    <mergeCell ref="BB36:BL36"/>
+    <mergeCell ref="BM36:CA36"/>
+    <mergeCell ref="CB36:CK36"/>
   </mergeCells>
   <pageMargins left="0.59055118110236227" right="0.51181102362204722" top="0.78740157480314965" bottom="0.39370078740157483" header="0.19685039370078741" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>